<commit_message>
Excel Reading Writing using Apache POI Jar files
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6B3734-9CDD-4FF5-9BE7-44F09AE829DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C002587-8140-4C30-9354-9F3DC7FF106D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="11" xr2:uid="{849A150D-1512-4727-8FA3-EE95DEABD06B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="11" xr2:uid="{849A150D-1512-4727-8FA3-EE95DEABD06B}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,14 @@
     <sheet name="HRM_Nationality" sheetId="8" r:id="rId8"/>
     <sheet name="Demo_Registration" sheetId="9" r:id="rId9"/>
     <sheet name="Demo_CreateAddress" sheetId="10" r:id="rId10"/>
-    <sheet name="Demo_MultipleProducts" sheetId="11" r:id="rId11"/>
-    <sheet name="Demo_TotalOrders" sheetId="12" r:id="rId12"/>
+    <sheet name="Demo_TotalOrders" sheetId="12" r:id="rId11"/>
+    <sheet name="Demo_MultipleProducts" sheetId="11" r:id="rId12"/>
     <sheet name="Demo_ApplyDiscount" sheetId="13" r:id="rId13"/>
     <sheet name="Demo_PlaceOrder" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -218,12 +218,46 @@
   </si>
   <si>
     <t>Display Fields</t>
+  </si>
+  <si>
+    <t>TestCase ID</t>
+  </si>
+  <si>
+    <t>TestCase Name</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Produ2</t>
+  </si>
+  <si>
+    <t>Product3</t>
+  </si>
+  <si>
+    <t>Product4</t>
+  </si>
+  <si>
+    <t>Product5</t>
+  </si>
+  <si>
+    <t>OrderNumber</t>
+  </si>
+  <si>
+    <t>15623987</t>
+  </si>
+  <si>
+    <t>423131</t>
+  </si>
+  <si>
+    <t>99823987</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -282,10 +316,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,12 +656,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.88671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -658,10 +693,10 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -672,10 +707,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -686,10 +721,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -700,10 +735,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -714,10 +749,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -743,7 +778,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E484FB7C-19A2-4EAD-BDB9-78BE9703E960}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858138AE-A3A4-4921-813E-A4272E6FD6E5}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -755,13 +790,68 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858138AE-A3A4-4921-813E-A4272E6FD6E5}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E484FB7C-19A2-4EAD-BDB9-78BE9703E960}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.33203125"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.21875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J2" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="J4" t="s" s="0">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -790,10 +880,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -806,15 +896,15 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -832,13 +922,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -846,13 +936,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -860,13 +950,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -874,13 +964,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -888,13 +978,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -918,20 +1008,20 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.21875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -967,99 +1057,99 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>33</v>
       </c>
     </row>
@@ -1086,15 +1176,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.21875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1130,13 +1220,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1144,13 +1234,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1158,13 +1248,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1172,13 +1262,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1186,13 +1276,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1240,7 +1330,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9AA29E-979A-4B8C-BE5C-88675B3D66F6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
Integrated Excel Changes for Login and Add User testcases
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE189F-43CF-45C6-ADCB-03C1829B071C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23EF0D1-F2B2-4488-AC66-9BB2F468DB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="3" activeTab="13" xr2:uid="{849A150D-1512-4727-8FA3-EE95DEABD06B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="2" xr2:uid="{849A150D-1512-4727-8FA3-EE95DEABD06B}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="421">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -100,9 +100,6 @@
     <t>EmployeeName</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
     <t>Supervisor Role</t>
   </si>
   <si>
@@ -1295,6 +1292,15 @@
   </si>
   <si>
     <t>TC13_DemoWebshop_PlaceOrder</t>
+  </si>
+  <si>
+    <t>CreateUserName</t>
+  </si>
+  <si>
+    <t>NewUserPassword</t>
+  </si>
+  <si>
+    <t>NewUser Confirm Password</t>
   </si>
 </sst>
 </file>
@@ -1735,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465F3D26-F1A8-4B13-B38D-C40AE737F5AF}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I77" sqref="I77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1749,32 +1755,32 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1782,82 +1788,82 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1865,82 +1871,82 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>365</v>
+      </c>
+      <c r="D13" t="s">
         <v>243</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>366</v>
-      </c>
-      <c r="D13" t="s">
-        <v>244</v>
-      </c>
       <c r="E13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1948,79 +1954,82 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D17" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="E17" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>366</v>
+      </c>
+      <c r="D19" t="s">
         <v>253</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>367</v>
-      </c>
-      <c r="D19" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2028,79 +2037,85 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D21" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="E21" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D22" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="E22" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C24" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B25" t="s">
+        <v>264</v>
+      </c>
+      <c r="C25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D25" t="s">
         <v>265</v>
-      </c>
-      <c r="C25" t="s">
-        <v>368</v>
-      </c>
-      <c r="D25" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2108,79 +2123,85 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C29" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D29" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="E29" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D30" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="E30" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B31" t="s">
+        <v>212</v>
+      </c>
+      <c r="C31" t="s">
+        <v>368</v>
+      </c>
+      <c r="D31" t="s">
         <v>272</v>
-      </c>
-      <c r="B31" t="s">
-        <v>213</v>
-      </c>
-      <c r="C31" t="s">
-        <v>369</v>
-      </c>
-      <c r="D31" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2188,79 +2209,79 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C34" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C35" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B36" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C36" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B37" t="s">
+        <v>283</v>
+      </c>
+      <c r="C37" t="s">
+        <v>369</v>
+      </c>
+      <c r="D37" t="s">
         <v>284</v>
-      </c>
-      <c r="C37" t="s">
-        <v>370</v>
-      </c>
-      <c r="D37" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2268,79 +2289,79 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C39" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D39" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B41" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C41" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B42" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C42" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B43" t="s">
+        <v>295</v>
+      </c>
+      <c r="C43" t="s">
+        <v>370</v>
+      </c>
+      <c r="D43" t="s">
         <v>296</v>
-      </c>
-      <c r="C43" t="s">
-        <v>371</v>
-      </c>
-      <c r="D43" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2348,79 +2369,79 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B45" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B46" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C46" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D46" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B47" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C47" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D47" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C48" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B49" t="s">
+        <v>306</v>
+      </c>
+      <c r="C49" t="s">
+        <v>376</v>
+      </c>
+      <c r="D49" t="s">
         <v>307</v>
-      </c>
-      <c r="C49" t="s">
-        <v>377</v>
-      </c>
-      <c r="D49" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2428,79 +2449,79 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B51" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D51" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D52" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D53" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" t="s">
         <v>319</v>
-      </c>
-      <c r="C55" t="s">
-        <v>41</v>
-      </c>
-      <c r="D55" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2508,79 +2529,79 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D57" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D58" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C60" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D60" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B61" t="s">
+        <v>39</v>
+      </c>
+      <c r="C61" t="s">
+        <v>320</v>
+      </c>
+      <c r="D61" t="s">
         <v>326</v>
-      </c>
-      <c r="B61" t="s">
-        <v>40</v>
-      </c>
-      <c r="C61" t="s">
-        <v>321</v>
-      </c>
-      <c r="D61" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2588,79 +2609,79 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B63" t="s">
         <v>329</v>
       </c>
-      <c r="B63" t="s">
-        <v>330</v>
-      </c>
       <c r="C63" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D63" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B64" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C64" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D64" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B65" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C65" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D65" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B66" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C66" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D66" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B67" t="s">
+        <v>333</v>
+      </c>
+      <c r="C67" t="s">
+        <v>327</v>
+      </c>
+      <c r="D67" t="s">
         <v>334</v>
-      </c>
-      <c r="C67" t="s">
-        <v>328</v>
-      </c>
-      <c r="D67" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2668,79 +2689,79 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B69" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C69" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D69" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B70" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C70" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B71" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C71" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B72" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C72" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D72" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B73" t="s">
+        <v>343</v>
+      </c>
+      <c r="C73" t="s">
+        <v>345</v>
+      </c>
+      <c r="D73" t="s">
         <v>351</v>
-      </c>
-      <c r="B73" t="s">
-        <v>344</v>
-      </c>
-      <c r="C73" t="s">
-        <v>346</v>
-      </c>
-      <c r="D73" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -2748,72 +2769,72 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B75" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C75" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D75" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B76" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C76" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D76" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B77" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C77" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D77" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B78" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C78" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D78" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B79" t="s">
+        <v>362</v>
+      </c>
+      <c r="C79" t="s">
+        <v>417</v>
+      </c>
+      <c r="D79" t="s">
         <v>363</v>
-      </c>
-      <c r="C79" t="s">
-        <v>418</v>
-      </c>
-      <c r="D79" t="s">
-        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -2864,290 +2885,290 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
         <v>77</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>80</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>81</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>82</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" t="s">
         <v>84</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>85</v>
       </c>
-      <c r="N2" t="s">
-        <v>86</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" t="s">
         <v>89</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>90</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>91</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>92</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>93</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>94</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>95</v>
       </c>
-      <c r="N3" t="s">
-        <v>96</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
         <v>97</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" t="s">
         <v>99</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>100</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>101</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>102</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>103</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>104</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>105</v>
       </c>
-      <c r="N4" t="s">
-        <v>106</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" t="s">
         <v>107</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" t="s">
         <v>109</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>110</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" t="s">
         <v>111</v>
       </c>
-      <c r="J5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>112</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>113</v>
       </c>
-      <c r="M5" t="s">
-        <v>114</v>
-      </c>
       <c r="N5" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" t="s">
         <v>115</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" t="s">
         <v>117</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>118</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" t="s">
         <v>119</v>
       </c>
-      <c r="J6" t="s">
-        <v>102</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>120</v>
       </c>
-      <c r="L6" t="s">
-        <v>121</v>
-      </c>
       <c r="M6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3212,173 +3233,173 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H2" t="s">
         <v>161</v>
       </c>
-      <c r="F2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>206</v>
-      </c>
-      <c r="H2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H6" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" t="s">
         <v>206</v>
-      </c>
-      <c r="H6" t="s">
-        <v>162</v>
-      </c>
-      <c r="I6" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3436,221 +3457,221 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
         <v>176</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>177</v>
       </c>
-      <c r="G2" t="s">
-        <v>178</v>
-      </c>
       <c r="H2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2" t="s">
         <v>182</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" t="s">
         <v>177</v>
       </c>
-      <c r="G3" t="s">
-        <v>178</v>
-      </c>
       <c r="H3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" t="s">
         <v>182</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4" t="s">
         <v>177</v>
       </c>
-      <c r="G4" t="s">
-        <v>178</v>
-      </c>
       <c r="H4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I4" t="s">
         <v>182</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" t="s">
         <v>181</v>
       </c>
-      <c r="F5" t="s">
-        <v>177</v>
-      </c>
-      <c r="G5" t="s">
-        <v>178</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>182</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>345</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" t="s">
         <v>177</v>
       </c>
-      <c r="G6" t="s">
-        <v>178</v>
-      </c>
       <c r="H6" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6" t="s">
         <v>182</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="K6" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3675,7 +3696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECF2A06-7E58-4738-8909-81B6983160B5}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3708,203 +3729,203 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" t="s">
         <v>406</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I2" t="s">
         <v>407</v>
       </c>
-      <c r="H2" t="s">
-        <v>407</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>408</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>409</v>
-      </c>
-      <c r="K2" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
+        <v>406</v>
+      </c>
+      <c r="H3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I3" t="s">
         <v>407</v>
       </c>
-      <c r="H3" t="s">
-        <v>407</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>408</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>409</v>
-      </c>
-      <c r="K3" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>411</v>
+      </c>
+      <c r="F4" t="s">
         <v>412</v>
       </c>
-      <c r="F4" t="s">
-        <v>413</v>
-      </c>
       <c r="G4" t="s">
+        <v>406</v>
+      </c>
+      <c r="H4" t="s">
+        <v>406</v>
+      </c>
+      <c r="I4" t="s">
         <v>407</v>
       </c>
-      <c r="H4" t="s">
-        <v>407</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>408</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>409</v>
-      </c>
-      <c r="K4" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>413</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>415</v>
-      </c>
       <c r="G5" t="s">
+        <v>406</v>
+      </c>
+      <c r="H5" t="s">
+        <v>406</v>
+      </c>
+      <c r="I5" t="s">
         <v>407</v>
       </c>
-      <c r="H5" t="s">
-        <v>407</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>408</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>409</v>
-      </c>
-      <c r="K5" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>415</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="G6" t="s">
+        <v>406</v>
+      </c>
+      <c r="H6" t="s">
+        <v>406</v>
+      </c>
+      <c r="I6" t="s">
         <v>407</v>
       </c>
-      <c r="H6" t="s">
-        <v>407</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>408</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>409</v>
-      </c>
-      <c r="K6" t="s">
-        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -3931,7 +3952,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3961,7 +3982,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -3975,7 +3996,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -3989,7 +4010,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -4003,7 +4024,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -4017,7 +4038,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4042,8 +4063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3C6014-9415-4F9B-A997-33FE24BD9D78}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4053,11 +4074,11 @@
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -4077,27 +4098,27 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
+        <v>419</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>23</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4106,30 +4127,30 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4138,30 +4159,30 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4170,30 +4191,30 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" t="s">
-        <v>193</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4202,30 +4223,30 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
         <v>63</v>
       </c>
-      <c r="F5" t="s">
-        <v>194</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>64</v>
       </c>
-      <c r="I5" t="s">
-        <v>65</v>
-      </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4234,22 +4255,22 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
         <v>66</v>
       </c>
-      <c r="F6" t="s">
-        <v>195</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -4278,7 +4299,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4309,30 +4330,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4341,30 +4362,30 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
         <v>136</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>137</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>138</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>139</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>140</v>
-      </c>
-      <c r="J2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4373,30 +4394,30 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
         <v>142</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>143</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>144</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>145</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>146</v>
-      </c>
-      <c r="J3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4405,30 +4426,30 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" t="s">
         <v>148</v>
       </c>
-      <c r="F4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>149</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>150</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>151</v>
-      </c>
-      <c r="J4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4437,30 +4458,30 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" t="s">
         <v>153</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>154</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>155</v>
-      </c>
-      <c r="J5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4469,22 +4490,22 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" t="s">
         <v>157</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>158</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>159</v>
-      </c>
-      <c r="J6" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4530,30 +4551,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4562,30 +4583,30 @@
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="G2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>386</v>
-      </c>
       <c r="J2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4594,30 +4615,30 @@
         <v>10</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="G3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>387</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>389</v>
-      </c>
       <c r="J3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4626,30 +4647,30 @@
         <v>10</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="G4" t="s">
-        <v>138</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>392</v>
-      </c>
       <c r="J4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4658,30 +4679,30 @@
         <v>10</v>
       </c>
       <c r="E5" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="G5" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>395</v>
-      </c>
       <c r="J5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4690,22 +4711,22 @@
         <v>10</v>
       </c>
       <c r="E6" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G6" t="s">
-        <v>138</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>398</v>
-      </c>
       <c r="J6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -4747,30 +4768,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4779,24 +4800,24 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" s="11">
         <v>45027</v>
       </c>
       <c r="G2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4805,24 +4826,24 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F3" s="11">
         <v>45241</v>
       </c>
       <c r="G3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H3" t="s">
         <v>220</v>
-      </c>
-      <c r="H3" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4831,24 +4852,24 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" t="s">
         <v>222</v>
       </c>
-      <c r="F4" t="s">
-        <v>223</v>
-      </c>
       <c r="G4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4857,24 +4878,24 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" t="s">
         <v>224</v>
       </c>
-      <c r="F5" t="s">
-        <v>225</v>
-      </c>
       <c r="G5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4883,16 +4904,16 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>225</v>
+      </c>
+      <c r="F6" t="s">
         <v>226</v>
       </c>
-      <c r="F6" t="s">
-        <v>227</v>
-      </c>
       <c r="G6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4946,21 +4967,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4969,15 +4990,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4986,15 +5007,15 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5003,15 +5024,15 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5020,15 +5041,15 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5037,7 +5058,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -5080,39 +5101,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -5120,13 +5141,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -5134,13 +5155,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -5148,13 +5169,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -5162,13 +5183,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
TC10 Demoworkshop total orders is completed
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arunkumar/IdeaProjects/AutomationCatalogue_TestingFramework/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23EF0D1-F2B2-4488-AC66-9BB2F468DB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27107217-328A-BA4E-9800-0903CBE1DDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="2" xr2:uid="{849A150D-1512-4727-8FA3-EE95DEABD06B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" tabRatio="877" firstSheet="3" activeTab="10" xr2:uid="{849A150D-1512-4727-8FA3-EE95DEABD06B}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="422">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1301,6 +1301,9 @@
   </si>
   <si>
     <t>NewUser Confirm Password</t>
+  </si>
+  <si>
+    <t>TC08_DemoWebshop_TotalOrders</t>
   </si>
 </sst>
 </file>
@@ -1745,15 +1748,15 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>227</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1786,7 +1789,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>231</v>
       </c>
@@ -1800,7 +1803,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>232</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>233</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>234</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>235</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -1869,7 +1872,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>238</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>239</v>
       </c>
@@ -1897,7 +1900,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>240</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>241</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>242</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -1952,7 +1955,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>248</v>
       </c>
@@ -1966,7 +1969,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>249</v>
       </c>
@@ -1980,7 +1983,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>250</v>
       </c>
@@ -1997,7 +2000,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>251</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>252</v>
       </c>
@@ -2025,7 +2028,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2035,7 +2038,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>255</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>256</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>257</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>258</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>259</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2121,7 +2124,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>267</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>268</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>269</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>270</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>271</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -2207,7 +2210,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>274</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>275</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>276</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>277</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>278</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -2287,7 +2290,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>286</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>287</v>
       </c>
@@ -2315,7 +2318,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>288</v>
       </c>
@@ -2329,7 +2332,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>289</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>290</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -2367,7 +2370,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>297</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>298</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>299</v>
       </c>
@@ -2409,7 +2412,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>300</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>301</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2447,7 +2450,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>309</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>310</v>
       </c>
@@ -2475,7 +2478,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>311</v>
       </c>
@@ -2489,7 +2492,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>312</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>313</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -2527,7 +2530,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>321</v>
       </c>
@@ -2541,7 +2544,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>322</v>
       </c>
@@ -2555,7 +2558,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>323</v>
       </c>
@@ -2569,7 +2572,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>324</v>
       </c>
@@ -2583,7 +2586,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>325</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -2607,7 +2610,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>328</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>335</v>
       </c>
@@ -2635,7 +2638,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>336</v>
       </c>
@@ -2649,7 +2652,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>337</v>
       </c>
@@ -2663,7 +2666,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>338</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -2687,7 +2690,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>346</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>347</v>
       </c>
@@ -2715,7 +2718,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>348</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>349</v>
       </c>
@@ -2743,7 +2746,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>350</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -2767,7 +2770,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>353</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>354</v>
       </c>
@@ -2795,7 +2798,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>355</v>
       </c>
@@ -2809,7 +2812,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>356</v>
       </c>
@@ -2823,7 +2826,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>357</v>
       </c>
@@ -2848,30 +2851,30 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2921,7 +2924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>314</v>
       </c>
@@ -2971,7 +2974,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>315</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>316</v>
       </c>
@@ -3071,7 +3074,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>317</v>
       </c>
@@ -3121,7 +3124,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>318</v>
       </c>
@@ -3193,12 +3196,118 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858138AE-A3A4-4921-813E-A4272E6FD6E5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>421</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{CC4CFBCA-994E-A94C-9DE5-C92372322E83}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{0F466D25-F9F9-1241-ACF4-2292CA8EA1EA}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{B2F53106-2EED-8D44-8EA0-ABB7A10A7C30}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{D547E16A-E2FA-4346-9D5E-E2229A078C3C}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{2A435EDA-30B5-914C-BD41-8B6259F4C7FA}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{630C16BD-0DFC-0C4D-8B89-EFF983AA1B97}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{98345781-1744-994F-B464-09AB8F35BAE4}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{C8062AEF-6A9E-6841-B82F-6AEA9DF9F3C7}"/>
+    <hyperlink ref="D5" r:id="rId9" xr:uid="{4557AFFE-29DB-4B4F-A61A-BDA54A71DC8D}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{7F5A2EAB-8ADA-1045-9476-60F1B2460E96}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3211,21 +3320,21 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3257,7 +3366,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>329</v>
       </c>
@@ -3286,7 +3395,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -3315,7 +3424,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>331</v>
       </c>
@@ -3344,7 +3453,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>332</v>
       </c>
@@ -3373,7 +3482,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>333</v>
       </c>
@@ -3426,24 +3535,24 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3484,7 +3593,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>339</v>
       </c>
@@ -3522,7 +3631,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>340</v>
       </c>
@@ -3560,7 +3669,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>341</v>
       </c>
@@ -3598,7 +3707,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>342</v>
       </c>
@@ -3636,7 +3745,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>343</v>
       </c>
@@ -3700,22 +3809,22 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3753,7 +3862,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>358</v>
       </c>
@@ -3788,7 +3897,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>359</v>
       </c>
@@ -3823,7 +3932,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>360</v>
       </c>
@@ -3858,7 +3967,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>361</v>
       </c>
@@ -3893,7 +4002,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>362</v>
       </c>
@@ -3955,15 +4064,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3977,7 +4086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3991,7 +4100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4005,7 +4114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4019,7 +4128,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4033,7 +4142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4063,25 +4172,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3C6014-9415-4F9B-A997-33FE24BD9D78}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4113,7 +4222,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -4145,7 +4254,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4177,7 +4286,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -4209,7 +4318,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -4241,7 +4350,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -4302,21 +4411,21 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4348,7 +4457,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -4380,7 +4489,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -4412,7 +4521,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4444,7 +4553,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -4476,7 +4585,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -4529,15 +4638,15 @@
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4569,7 +4678,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>260</v>
       </c>
@@ -4601,7 +4710,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>261</v>
       </c>
@@ -4633,7 +4742,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>262</v>
       </c>
@@ -4665,7 +4774,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -4697,7 +4806,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>264</v>
       </c>
@@ -4749,18 +4858,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4786,7 +4895,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>202</v>
       </c>
@@ -4812,7 +4921,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>207</v>
       </c>
@@ -4838,7 +4947,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>209</v>
       </c>
@@ -4864,7 +4973,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -4890,7 +4999,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>212</v>
       </c>
@@ -4936,7 +5045,7 @@
       <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4950,16 +5059,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4976,7 +5085,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>291</v>
       </c>
@@ -4993,7 +5102,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>292</v>
       </c>
@@ -5010,7 +5119,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>293</v>
       </c>
@@ -5027,7 +5136,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -5044,7 +5153,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>295</v>
       </c>
@@ -5079,21 +5188,22 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5125,7 +5235,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>302</v>
       </c>
@@ -5139,7 +5249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>303</v>
       </c>
@@ -5153,7 +5263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>304</v>
       </c>
@@ -5167,7 +5277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>305</v>
       </c>
@@ -5181,7 +5291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>306</v>
       </c>
@@ -5210,5 +5320,6 @@
     <hyperlink ref="D6" r:id="rId10" xr:uid="{BE9C2D93-F6A4-4587-A57C-EB59C57C4CA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TC04 & TC13 excel data changes
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arunkumar/IdeaProjects/AutomationCatalogue_TestingFramework/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970CF2B5-4D43-E64C-9544-B72FA536715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9081DB-44CE-4370-B5C5-C77137BF6196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" tabRatio="877" activeTab="6" xr2:uid="{849A150D-1512-4727-8FA3-EE95DEABD06B}"/>
+    <workbookView xWindow="900" yWindow="1980" windowWidth="18100" windowHeight="6970" tabRatio="877" activeTab="4" xr2:uid="{849A150D-1512-4727-8FA3-EE95DEABD06B}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="442">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1352,6 +1352,18 @@
   </si>
   <si>
     <t>Due Date</t>
+  </si>
+  <si>
+    <t>Test Case_ID</t>
+  </si>
+  <si>
+    <t>Test Case_Name</t>
+  </si>
+  <si>
+    <t>User_Name</t>
+  </si>
+  <si>
+    <t>Password_DWS</t>
   </si>
 </sst>
 </file>
@@ -1796,15 +1808,15 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>227</v>
       </c>
@@ -1827,7 +1839,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1837,7 +1849,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>231</v>
       </c>
@@ -1851,7 +1863,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>232</v>
       </c>
@@ -1865,7 +1877,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>233</v>
       </c>
@@ -1882,7 +1894,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>234</v>
       </c>
@@ -1896,7 +1908,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>235</v>
       </c>
@@ -1910,7 +1922,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -1920,7 +1932,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>238</v>
       </c>
@@ -1934,7 +1946,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>239</v>
       </c>
@@ -1948,7 +1960,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>240</v>
       </c>
@@ -1962,7 +1974,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>241</v>
       </c>
@@ -1976,7 +1988,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>242</v>
       </c>
@@ -1993,7 +2005,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -2003,7 +2015,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>248</v>
       </c>
@@ -2017,7 +2029,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>249</v>
       </c>
@@ -2031,7 +2043,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>250</v>
       </c>
@@ -2048,7 +2060,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>251</v>
       </c>
@@ -2062,7 +2074,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>252</v>
       </c>
@@ -2076,7 +2088,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2086,7 +2098,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>255</v>
       </c>
@@ -2103,7 +2115,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>256</v>
       </c>
@@ -2120,7 +2132,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>257</v>
       </c>
@@ -2134,7 +2146,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>258</v>
       </c>
@@ -2148,7 +2160,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>259</v>
       </c>
@@ -2162,7 +2174,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2172,7 +2184,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>267</v>
       </c>
@@ -2186,7 +2198,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>268</v>
       </c>
@@ -2200,7 +2212,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>269</v>
       </c>
@@ -2217,7 +2229,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>270</v>
       </c>
@@ -2234,7 +2246,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>271</v>
       </c>
@@ -2248,7 +2260,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -2258,7 +2270,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>274</v>
       </c>
@@ -2272,7 +2284,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>275</v>
       </c>
@@ -2286,7 +2298,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>276</v>
       </c>
@@ -2300,7 +2312,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>277</v>
       </c>
@@ -2314,7 +2326,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>278</v>
       </c>
@@ -2328,7 +2340,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -2338,7 +2350,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>286</v>
       </c>
@@ -2352,7 +2364,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>287</v>
       </c>
@@ -2366,7 +2378,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>288</v>
       </c>
@@ -2380,7 +2392,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>289</v>
       </c>
@@ -2394,7 +2406,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>290</v>
       </c>
@@ -2408,7 +2420,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -2418,7 +2430,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>297</v>
       </c>
@@ -2432,7 +2444,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>298</v>
       </c>
@@ -2446,7 +2458,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>299</v>
       </c>
@@ -2460,7 +2472,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>300</v>
       </c>
@@ -2474,7 +2486,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>301</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2498,7 +2510,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>309</v>
       </c>
@@ -2512,7 +2524,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>310</v>
       </c>
@@ -2526,7 +2538,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>311</v>
       </c>
@@ -2540,7 +2552,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>312</v>
       </c>
@@ -2554,7 +2566,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>313</v>
       </c>
@@ -2568,7 +2580,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -2578,7 +2590,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>321</v>
       </c>
@@ -2592,7 +2604,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>322</v>
       </c>
@@ -2606,7 +2618,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>323</v>
       </c>
@@ -2620,7 +2632,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>324</v>
       </c>
@@ -2634,7 +2646,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>325</v>
       </c>
@@ -2648,7 +2660,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -2658,7 +2670,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>328</v>
       </c>
@@ -2672,7 +2684,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>335</v>
       </c>
@@ -2686,7 +2698,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>336</v>
       </c>
@@ -2700,7 +2712,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>337</v>
       </c>
@@ -2714,7 +2726,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>338</v>
       </c>
@@ -2728,7 +2740,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -2738,7 +2750,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>346</v>
       </c>
@@ -2752,7 +2764,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>347</v>
       </c>
@@ -2766,7 +2778,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>348</v>
       </c>
@@ -2780,7 +2792,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>349</v>
       </c>
@@ -2794,7 +2806,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>350</v>
       </c>
@@ -2808,7 +2820,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -2818,7 +2830,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>353</v>
       </c>
@@ -2832,7 +2844,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>354</v>
       </c>
@@ -2846,7 +2858,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>355</v>
       </c>
@@ -2860,7 +2872,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>356</v>
       </c>
@@ -2874,7 +2886,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>357</v>
       </c>
@@ -2902,27 +2914,27 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2972,7 +2984,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>314</v>
       </c>
@@ -3022,7 +3034,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>315</v>
       </c>
@@ -3072,7 +3084,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>316</v>
       </c>
@@ -3122,7 +3134,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>317</v>
       </c>
@@ -3172,7 +3184,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>318</v>
       </c>
@@ -3250,15 +3262,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3272,7 +3284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -3286,7 +3298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -3300,7 +3312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -3314,7 +3326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -3328,7 +3340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -3368,21 +3380,21 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3414,7 +3426,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>329</v>
       </c>
@@ -3443,7 +3455,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -3472,7 +3484,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>331</v>
       </c>
@@ -3501,7 +3513,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>332</v>
       </c>
@@ -3530,7 +3542,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>333</v>
       </c>
@@ -3583,24 +3595,24 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3641,7 +3653,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>339</v>
       </c>
@@ -3679,7 +3691,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>340</v>
       </c>
@@ -3717,7 +3729,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>341</v>
       </c>
@@ -3755,7 +3767,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>342</v>
       </c>
@@ -3793,7 +3805,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>343</v>
       </c>
@@ -3854,36 +3866,36 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="59.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>438</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>439</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>440</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>441</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>398</v>
@@ -3910,7 +3922,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>358</v>
       </c>
@@ -3945,7 +3957,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>359</v>
       </c>
@@ -3980,7 +3992,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>360</v>
       </c>
@@ -4015,7 +4027,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>361</v>
       </c>
@@ -4050,7 +4062,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>362</v>
       </c>
@@ -4112,15 +4124,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4148,7 +4160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4162,7 +4174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4176,7 +4188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4190,7 +4202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4224,21 +4236,21 @@
       <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4270,7 +4282,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -4302,7 +4314,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4334,7 +4346,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -4366,7 +4378,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -4398,7 +4410,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -4459,21 +4471,21 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4505,7 +4517,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -4537,7 +4549,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -4569,7 +4581,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4601,7 +4613,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -4633,7 +4645,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -4682,19 +4694,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07E44F-B58F-4D40-935C-D77AA3242FC4}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4726,7 +4739,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>260</v>
       </c>
@@ -4743,7 +4756,7 @@
         <v>383</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G2" t="s">
         <v>137</v>
@@ -4752,13 +4765,13 @@
         <v>383</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>261</v>
       </c>
@@ -4775,7 +4788,7 @@
         <v>386</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G3" t="s">
         <v>137</v>
@@ -4784,13 +4797,13 @@
         <v>386</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>262</v>
       </c>
@@ -4807,7 +4820,7 @@
         <v>389</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G4" t="s">
         <v>137</v>
@@ -4816,13 +4829,13 @@
         <v>389</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -4839,7 +4852,7 @@
         <v>392</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G5" t="s">
         <v>137</v>
@@ -4848,13 +4861,13 @@
         <v>392</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>264</v>
       </c>
@@ -4871,7 +4884,7 @@
         <v>395</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="G6" t="s">
         <v>137</v>
@@ -4880,7 +4893,7 @@
         <v>395</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J6" t="s">
         <v>148</v>
@@ -4906,18 +4919,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4943,7 +4956,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>202</v>
       </c>
@@ -4969,7 +4982,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>207</v>
       </c>
@@ -4995,7 +5008,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>209</v>
       </c>
@@ -5021,7 +5034,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -5047,7 +5060,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>212</v>
       </c>
@@ -5089,26 +5102,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9AA29E-979A-4B8C-BE5C-88675B3D66F6}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5143,7 +5156,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -5178,7 +5191,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>280</v>
       </c>
@@ -5213,7 +5226,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>281</v>
       </c>
@@ -5248,7 +5261,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>282</v>
       </c>
@@ -5283,7 +5296,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>283</v>
       </c>
@@ -5339,16 +5352,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5365,7 +5378,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>291</v>
       </c>
@@ -5382,7 +5395,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>292</v>
       </c>
@@ -5399,7 +5412,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>293</v>
       </c>
@@ -5416,7 +5429,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -5433,7 +5446,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>295</v>
       </c>
@@ -5471,19 +5484,19 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5515,7 +5528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>302</v>
       </c>
@@ -5529,7 +5542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>303</v>
       </c>
@@ -5543,7 +5556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>304</v>
       </c>
@@ -5557,7 +5570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>305</v>
       </c>
@@ -5571,7 +5584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>306</v>
       </c>

</xml_diff>

<commit_message>
Latest Code changes of Arun and Shalini testcases
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B626EF-D52D-4D9C-B492-067083F935A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67379EC-4604-49C3-B0B5-B240ABC10DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="483">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Admin Role</t>
   </si>
   <si>
-    <t>Confirm Password</t>
-  </si>
-  <si>
     <t>TC02-01</t>
   </si>
   <si>
@@ -628,21 +625,6 @@
     <t>User name</t>
   </si>
   <si>
-    <t>Product 1</t>
-  </si>
-  <si>
-    <t>Product 2</t>
-  </si>
-  <si>
-    <t>Product 3</t>
-  </si>
-  <si>
-    <t>Product 4</t>
-  </si>
-  <si>
-    <t>Product 5</t>
-  </si>
-  <si>
     <t>Order ID</t>
   </si>
   <si>
@@ -655,9 +637,6 @@
     <t>14.1-inch Laptop</t>
   </si>
   <si>
-    <t>50's Rockabilly Polka Dot Top JR Plus Size</t>
-  </si>
-  <si>
     <t>Black &amp; White Diamond Heart</t>
   </si>
   <si>
@@ -679,9 +658,6 @@
     <t>TC05-05</t>
   </si>
   <si>
-    <t>TCP Self-Paced Training</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -1373,6 +1349,144 @@
   </si>
   <si>
     <t>6-September-2023</t>
+  </si>
+  <si>
+    <t>Testcase</t>
+  </si>
+  <si>
+    <t>Testcasename</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Confirm password</t>
+  </si>
+  <si>
+    <t>TS08_01</t>
+  </si>
+  <si>
+    <t>TS08_DemoWebshop_Registration</t>
+  </si>
+  <si>
+    <t>aarosagarch@gamil.com</t>
+  </si>
+  <si>
+    <t>sagar</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>TS08_02</t>
+  </si>
+  <si>
+    <t>anupreddy.desai@gmail.com</t>
+  </si>
+  <si>
+    <t>anup</t>
+  </si>
+  <si>
+    <t>reddy</t>
+  </si>
+  <si>
+    <t>TS08_03</t>
+  </si>
+  <si>
+    <t>anupreddy2906@gmail.com</t>
+  </si>
+  <si>
+    <t>Desai</t>
+  </si>
+  <si>
+    <t>Anup</t>
+  </si>
+  <si>
+    <t>TS08_04</t>
+  </si>
+  <si>
+    <t>v.desai1295@gmail.com</t>
+  </si>
+  <si>
+    <t>Venkata</t>
+  </si>
+  <si>
+    <t>TS08_05</t>
+  </si>
+  <si>
+    <t>venkata.desai@gmail.com</t>
+  </si>
+  <si>
+    <t>Product1 Category</t>
+  </si>
+  <si>
+    <t>Product2 Category</t>
+  </si>
+  <si>
+    <t>Product3 Category</t>
+  </si>
+  <si>
+    <t>Product4 Category</t>
+  </si>
+  <si>
+    <t>Apparel &amp; Shoes</t>
+  </si>
+  <si>
+    <t>Computers-Desktop</t>
+  </si>
+  <si>
+    <t>Product 1 Name</t>
+  </si>
+  <si>
+    <t>Product 2 Name</t>
+  </si>
+  <si>
+    <t>Electronics-Cell phones</t>
+  </si>
+  <si>
+    <t>Product 3 Name</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>Product 4 Name</t>
+  </si>
+  <si>
+    <t>Computers-Notebooks</t>
+  </si>
+  <si>
+    <t>Phone Cover</t>
+  </si>
+  <si>
+    <t>Casual Golf Belt</t>
+  </si>
+  <si>
+    <t>$25 Virtual Gift Card</t>
+  </si>
+  <si>
+    <t>Computers-Accessories</t>
+  </si>
+  <si>
+    <t>TCP Coaching day</t>
+  </si>
+  <si>
+    <t>Genuine Leather Handbag with Cell Phone Holder &amp; Many Pockets</t>
+  </si>
+  <si>
+    <t>$50 Physical Gift Card</t>
+  </si>
+  <si>
+    <t>Digital downloads</t>
+  </si>
+  <si>
+    <t>End Year Review 2018 - HQ-CA USA</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1495,6 +1609,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1826,32 +1941,32 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1859,82 +1974,82 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D4" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E5" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D6" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D7" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1942,82 +2057,82 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D9" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D10" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D11" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D12" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D13" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E13" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2025,82 +2140,82 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D15" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D16" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D17" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E17" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D18" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D19" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2108,85 +2223,85 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B21" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C21" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D21" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E21" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B22" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C22" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D22" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E22" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" t="s">
+        <v>353</v>
+      </c>
+      <c r="D23" t="s">
         <v>251</v>
-      </c>
-      <c r="B23" t="s">
-        <v>256</v>
-      </c>
-      <c r="C23" t="s">
-        <v>361</v>
-      </c>
-      <c r="D23" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B24" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C24" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D24" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B25" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C25" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D25" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2194,85 +2309,85 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C27" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D27" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C28" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D28" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B29" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C29" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D29" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="E29" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C30" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D30" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="E30" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B31" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C31" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D31" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2280,79 +2395,79 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B33" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C33" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D33" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B34" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C34" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D34" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B35" t="s">
+        <v>267</v>
+      </c>
+      <c r="C35" t="s">
+        <v>355</v>
+      </c>
+      <c r="D35" t="s">
         <v>270</v>
-      </c>
-      <c r="B35" t="s">
-        <v>275</v>
-      </c>
-      <c r="C35" t="s">
-        <v>363</v>
-      </c>
-      <c r="D35" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B36" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C36" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D36" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B37" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C37" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D37" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2360,79 +2475,79 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B39" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C39" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D39" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B40" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C40" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D40" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B41" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41" t="s">
+        <v>356</v>
+      </c>
+      <c r="D41" t="s">
         <v>282</v>
-      </c>
-      <c r="B41" t="s">
-        <v>287</v>
-      </c>
-      <c r="C41" t="s">
-        <v>364</v>
-      </c>
-      <c r="D41" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B42" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C42" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D42" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B43" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C43" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D43" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2440,79 +2555,79 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B45" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C45" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D45" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B46" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C46" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D46" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B47" t="s">
+        <v>290</v>
+      </c>
+      <c r="C47" t="s">
+        <v>362</v>
+      </c>
+      <c r="D47" t="s">
         <v>293</v>
-      </c>
-      <c r="B47" t="s">
-        <v>298</v>
-      </c>
-      <c r="C47" t="s">
-        <v>370</v>
-      </c>
-      <c r="D47" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B48" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C48" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D48" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B49" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C49" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D49" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2520,79 +2635,79 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B51" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B52" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B53" t="s">
+        <v>302</v>
+      </c>
+      <c r="C53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" t="s">
         <v>305</v>
-      </c>
-      <c r="B53" t="s">
-        <v>310</v>
-      </c>
-      <c r="C53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B54" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B55" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2600,79 +2715,79 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D57" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D58" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D59" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D60" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C61" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D61" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2680,79 +2795,79 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B63" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C63" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D63" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="B64" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="C64" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D64" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B65" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C65" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D65" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B66" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="C66" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D66" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B67" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C67" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D67" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2760,79 +2875,79 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B69" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C69" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D69" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="B70" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C70" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D70" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="B71" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="C71" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D71" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B72" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C72" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D72" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B73" t="s">
+        <v>329</v>
+      </c>
+      <c r="C73" t="s">
+        <v>331</v>
+      </c>
+      <c r="D73" t="s">
         <v>337</v>
-      </c>
-      <c r="C73" t="s">
-        <v>339</v>
-      </c>
-      <c r="D73" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -2840,72 +2955,72 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B75" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C75" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="D75" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B76" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C76" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="D76" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B77" t="s">
+        <v>346</v>
+      </c>
+      <c r="C77" t="s">
+        <v>403</v>
+      </c>
+      <c r="D77" t="s">
         <v>349</v>
-      </c>
-      <c r="B77" t="s">
-        <v>354</v>
-      </c>
-      <c r="C77" t="s">
-        <v>411</v>
-      </c>
-      <c r="D77" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="B78" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C78" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="D78" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="B79" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C79" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="D79" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -2956,290 +3071,290 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
         <v>76</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" t="s">
         <v>78</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>79</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>80</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>81</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" t="s">
         <v>83</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>84</v>
       </c>
-      <c r="N2" t="s">
-        <v>85</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" t="s">
         <v>88</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>89</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>90</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>91</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>92</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>93</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>94</v>
       </c>
-      <c r="N3" t="s">
-        <v>95</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" t="s">
         <v>96</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" t="s">
         <v>98</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>99</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>100</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>101</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>102</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>103</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>104</v>
       </c>
-      <c r="N4" t="s">
-        <v>105</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
         <v>106</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" t="s">
         <v>108</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>109</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" t="s">
         <v>110</v>
       </c>
-      <c r="J5" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>111</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>112</v>
       </c>
-      <c r="M5" t="s">
-        <v>113</v>
-      </c>
       <c r="N5" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" t="s">
         <v>114</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" t="s">
         <v>116</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>117</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" t="s">
         <v>118</v>
       </c>
-      <c r="J6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>119</v>
       </c>
-      <c r="L6" t="s">
-        <v>120</v>
-      </c>
       <c r="M6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3286,7 +3401,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -3294,13 +3409,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -3308,13 +3423,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -3322,13 +3437,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -3336,13 +3451,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -3350,13 +3465,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -3382,10 +3497,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3394,15 +3509,18 @@
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3410,173 +3528,227 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>196</v>
+        <v>461</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B2" t="s">
         <v>197</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>396</v>
+      </c>
+      <c r="F2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" t="s">
+        <v>466</v>
+      </c>
+      <c r="H2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I2" t="s">
+        <v>469</v>
+      </c>
+      <c r="J2" t="s">
+        <v>471</v>
+      </c>
+      <c r="K2" t="s">
+        <v>465</v>
+      </c>
+      <c r="L2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>481</v>
+      </c>
+      <c r="F3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" t="s">
+        <v>399</v>
+      </c>
+      <c r="H3" t="s">
+        <v>400</v>
+      </c>
+      <c r="I3" t="s">
+        <v>401</v>
+      </c>
+      <c r="J3" t="s">
+        <v>402</v>
+      </c>
+      <c r="K3" t="s">
+        <v>396</v>
+      </c>
+      <c r="L3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>473</v>
+      </c>
+      <c r="F4" t="s">
         <v>198</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G4" t="s">
+        <v>469</v>
+      </c>
+      <c r="H4" t="s">
+        <v>474</v>
+      </c>
+      <c r="I4" t="s">
+        <v>465</v>
+      </c>
+      <c r="J4" t="s">
+        <v>475</v>
+      </c>
+      <c r="K4" t="s">
+        <v>481</v>
+      </c>
+      <c r="L4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>399</v>
+      </c>
+      <c r="F5" t="s">
         <v>199</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>323</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="G5" t="s">
+        <v>401</v>
+      </c>
+      <c r="H5" t="s">
+        <v>476</v>
+      </c>
+      <c r="I5" t="s">
+        <v>396</v>
+      </c>
+      <c r="J5" t="s">
+        <v>164</v>
+      </c>
+      <c r="K5" t="s">
+        <v>477</v>
+      </c>
+      <c r="L5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>465</v>
+      </c>
+      <c r="F6" t="s">
+        <v>479</v>
+      </c>
+      <c r="G6" t="s">
+        <v>401</v>
+      </c>
+      <c r="H6" t="s">
+        <v>480</v>
+      </c>
+      <c r="I6" t="s">
+        <v>477</v>
+      </c>
+      <c r="J6" t="s">
         <v>203</v>
       </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="K6" t="s">
+        <v>465</v>
+      </c>
+      <c r="L6" t="s">
         <v>162</v>
-      </c>
-      <c r="F3" t="s">
-        <v>204</v>
-      </c>
-      <c r="G3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H3" t="s">
-        <v>164</v>
-      </c>
-      <c r="I3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>325</v>
-      </c>
-      <c r="B4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F4" t="s">
-        <v>210</v>
-      </c>
-      <c r="G4" t="s">
-        <v>163</v>
-      </c>
-      <c r="H4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>326</v>
-      </c>
-      <c r="B5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F5" t="s">
-        <v>210</v>
-      </c>
-      <c r="G5" t="s">
-        <v>208</v>
-      </c>
-      <c r="H5" t="s">
-        <v>164</v>
-      </c>
-      <c r="I5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>327</v>
-      </c>
-      <c r="B6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>162</v>
-      </c>
-      <c r="F6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G6" t="s">
-        <v>205</v>
-      </c>
-      <c r="H6" t="s">
-        <v>161</v>
-      </c>
-      <c r="I6" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3634,221 +3806,221 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" t="s">
         <v>175</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>176</v>
       </c>
-      <c r="G2" t="s">
-        <v>177</v>
-      </c>
       <c r="H2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" t="s">
         <v>181</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
         <v>176</v>
       </c>
-      <c r="G3" t="s">
-        <v>177</v>
-      </c>
       <c r="H3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3" t="s">
         <v>181</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
         <v>176</v>
       </c>
-      <c r="G4" t="s">
-        <v>177</v>
-      </c>
       <c r="H4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" t="s">
         <v>181</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" t="s">
         <v>180</v>
       </c>
-      <c r="F5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" t="s">
-        <v>177</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>181</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
         <v>176</v>
       </c>
-      <c r="G6" t="s">
-        <v>177</v>
-      </c>
       <c r="H6" t="s">
+        <v>180</v>
+      </c>
+      <c r="I6" t="s">
         <v>181</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="K6" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3894,215 +4066,215 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="B2" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G2" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="H2" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="I2" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="J2" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="K2" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B3" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G3" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="H3" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="I3" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="J3" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="K3" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="B4" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="F4" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="G4" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="H4" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="I4" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="J4" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="K4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B5" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="G5" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="H5" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="I5" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="J5" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="K5" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B6" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="G6" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="H6" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="I6" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="J6" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="K6" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -4159,7 +4331,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4173,7 +4345,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -4187,7 +4359,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -4201,7 +4373,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -4215,7 +4387,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4275,7 +4447,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -4284,18 +4456,18 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4304,30 +4476,30 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4336,30 +4508,30 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4368,30 +4540,30 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4400,30 +4572,30 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
         <v>62</v>
       </c>
-      <c r="F5" t="s">
-        <v>193</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>63</v>
       </c>
-      <c r="I5" t="s">
-        <v>64</v>
-      </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4432,22 +4604,22 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" t="s">
-        <v>194</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4507,30 +4679,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4539,30 +4711,30 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" t="s">
         <v>135</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>136</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>137</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>138</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>139</v>
-      </c>
-      <c r="J2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4571,30 +4743,30 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" t="s">
         <v>141</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>142</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>143</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>144</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>145</v>
-      </c>
-      <c r="J3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4603,30 +4775,30 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" t="s">
         <v>147</v>
       </c>
-      <c r="F4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>148</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>149</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>150</v>
-      </c>
-      <c r="J4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4635,30 +4807,30 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G5" t="s">
+        <v>151</v>
+      </c>
+      <c r="H5" t="s">
         <v>152</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>153</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>154</v>
-      </c>
-      <c r="J5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4667,22 +4839,22 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" t="s">
         <v>156</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>157</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>158</v>
-      </c>
-      <c r="J6" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -4729,30 +4901,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4761,30 +4933,30 @@
         <v>10</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="J2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4793,30 +4965,30 @@
         <v>10</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="G3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="J3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4825,30 +4997,30 @@
         <v>10</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="G4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="J4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B5" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4857,30 +5029,30 @@
         <v>10</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="G5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="J5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4889,22 +5061,22 @@
         <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="G6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="J6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -4946,30 +5118,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4978,24 +5150,24 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="G2" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5004,24 +5176,24 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="G3" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5030,24 +5202,24 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="G4" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5056,24 +5228,24 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="G5" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5082,16 +5254,16 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="G6" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="H6" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -5111,7 +5283,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5145,30 +5317,30 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5177,33 +5349,33 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="G2" t="s">
-        <v>420</v>
+        <v>482</v>
       </c>
       <c r="H2" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5212,33 +5384,33 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="G3" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="H3" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5247,33 +5419,33 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="F4" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="G4" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="H4" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5282,33 +5454,33 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="F5" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="G5" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="H5" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5317,25 +5489,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="F6" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="G6" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="H6" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -5376,21 +5548,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5399,15 +5571,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B3" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5416,15 +5588,15 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B4" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5433,15 +5605,15 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5450,15 +5622,15 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5467,7 +5639,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -5485,139 +5657,226 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I1" s="13" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>443</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>444</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>445</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F2" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>297</v>
+        <v>448</v>
       </c>
       <c r="B3" t="s">
-        <v>370</v>
+        <v>444</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>449</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F3" t="s">
+        <v>451</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>298</v>
+        <v>452</v>
       </c>
       <c r="B4" t="s">
-        <v>370</v>
+        <v>444</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>453</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>454</v>
+      </c>
+      <c r="F4" t="s">
+        <v>455</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>299</v>
+        <v>456</v>
       </c>
       <c r="B5" t="s">
-        <v>370</v>
+        <v>444</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>457</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>458</v>
+      </c>
+      <c r="F5" t="s">
+        <v>454</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>459</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>444</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>460</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>455</v>
+      </c>
+      <c r="F6" t="s">
+        <v>458</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="D3" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="D4" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
-    <hyperlink ref="D5" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{8505C122-2102-4146-B9D7-5E7E4E0527C2}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{F8A6FF10-0F6E-4529-B3EB-9DA5D19BBE35}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{D688E348-9F41-4365-8635-E3E497D8044D}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{A6E973EA-A807-4CDA-9F4D-CA5679A28AE2}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{773D28DD-AEFD-4B00-A8CC-371A958C9482}"/>
+    <hyperlink ref="D2" r:id="rId6" xr:uid="{913C1F99-88B3-40E2-88A9-0E73642C298A}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{85555F14-1A00-489D-839F-4962623D89F4}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{EC2AE3C3-D60E-40A7-9EA9-C860104A0FFC}"/>
+    <hyperlink ref="D5" r:id="rId9" xr:uid="{BA0F4533-F1FE-48E4-979E-0E8B44A92DA2}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{6D3FCDCB-044E-49E6-87F5-319651F27EE0}"/>
+    <hyperlink ref="G2" r:id="rId11" xr:uid="{2A0F8DDB-929D-4DB5-B961-AB1107EF2462}"/>
+    <hyperlink ref="G3" r:id="rId12" xr:uid="{AB13969F-4570-4481-A4F9-799148F68C6F}"/>
+    <hyperlink ref="G4" r:id="rId13" xr:uid="{045939CD-A3D8-433B-AE4A-17DE3C120125}"/>
+    <hyperlink ref="G5" r:id="rId14" xr:uid="{9EC052A2-EE02-49EA-B598-D49BB2777863}"/>
+    <hyperlink ref="G6" r:id="rId15" xr:uid="{3882F933-D459-432F-82B8-857CA1B4CBCA}"/>
+    <hyperlink ref="H2" r:id="rId16" xr:uid="{A02253FE-E3B4-415C-A6D2-E7E4896454DF}"/>
+    <hyperlink ref="H3" r:id="rId17" xr:uid="{499E51C2-76E4-4589-9D09-2EFA90EAC863}"/>
+    <hyperlink ref="H4" r:id="rId18" xr:uid="{9014AEF5-BFDD-4BCA-866A-BF730D30FA20}"/>
+    <hyperlink ref="H5" r:id="rId19" xr:uid="{FFC4B713-AD34-45A1-9833-7C5705B6263D}"/>
+    <hyperlink ref="H6" r:id="rId20" xr:uid="{030AE3A3-14E1-486F-BD5E-106C4A85DE27}"/>
+    <hyperlink ref="I2" r:id="rId21" xr:uid="{18F148A7-E58C-42B5-9FF9-E47C5E943794}"/>
+    <hyperlink ref="I3" r:id="rId22" xr:uid="{7C2E4059-26E3-4700-AEF4-6CC447E57C3C}"/>
+    <hyperlink ref="I4" r:id="rId23" xr:uid="{591360A2-F11D-4865-9ABC-BD80B8FFA414}"/>
+    <hyperlink ref="I5" r:id="rId24" xr:uid="{57834260-FD0C-4DC5-BBAE-34A140B13157}"/>
+    <hyperlink ref="I6" r:id="rId25" xr:uid="{31445ED0-F4B7-454D-92D0-F5E877CB8B1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Latest Code changes of Shalini testcases
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE5C4AB-80B9-4878-B123-5A0739A9579E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90949CE-0365-42FC-A9C8-B5BEE1D07F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="490">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1471,9 +1471,6 @@
     <t>Computers-Accessories</t>
   </si>
   <si>
-    <t>TCP Coaching day</t>
-  </si>
-  <si>
     <t>Genuine Leather Handbag with Cell Phone Holder &amp; Many Pockets</t>
   </si>
   <si>
@@ -1496,12 +1493,28 @@
   </si>
   <si>
     <t>daniel.upton</t>
+  </si>
+  <si>
+    <t>Order number: 1550156</t>
+  </si>
+  <si>
+    <t>Order number: 1550173</t>
+  </si>
+  <si>
+    <t>Order number: 1550182</t>
+  </si>
+  <si>
+    <t>Order number: 1550185</t>
+  </si>
+  <si>
+    <t>Order number: 1550202</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1949,10 +1962,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="63.21875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1992,13 +2005,13 @@
       <c r="A3" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>222</v>
       </c>
     </row>
@@ -2006,13 +2019,13 @@
       <c r="A4" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>222</v>
       </c>
     </row>
@@ -2020,16 +2033,16 @@
       <c r="A5" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>232</v>
       </c>
     </row>
@@ -2037,13 +2050,13 @@
       <c r="A6" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>222</v>
       </c>
     </row>
@@ -2051,13 +2064,13 @@
       <c r="A7" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>222</v>
       </c>
     </row>
@@ -2075,13 +2088,13 @@
       <c r="A9" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2089,13 +2102,13 @@
       <c r="A10" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2103,13 +2116,13 @@
       <c r="A11" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2117,13 +2130,13 @@
       <c r="A12" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2131,16 +2144,16 @@
       <c r="A13" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>229</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>232</v>
       </c>
     </row>
@@ -2158,13 +2171,13 @@
       <c r="A15" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>239</v>
       </c>
     </row>
@@ -2172,13 +2185,13 @@
       <c r="A16" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>239</v>
       </c>
     </row>
@@ -2186,16 +2199,16 @@
       <c r="A17" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>232</v>
       </c>
     </row>
@@ -2203,13 +2216,13 @@
       <c r="A18" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>239</v>
       </c>
     </row>
@@ -2217,13 +2230,13 @@
       <c r="A19" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>239</v>
       </c>
     </row>
@@ -2241,16 +2254,16 @@
       <c r="A21" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>246</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>251</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>232</v>
       </c>
     </row>
@@ -2258,16 +2271,16 @@
       <c r="A22" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>247</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>251</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>232</v>
       </c>
     </row>
@@ -2275,13 +2288,13 @@
       <c r="A23" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>248</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>251</v>
       </c>
     </row>
@@ -2289,13 +2302,13 @@
       <c r="A24" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>249</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="s" s="0">
         <v>251</v>
       </c>
     </row>
@@ -2303,13 +2316,13 @@
       <c r="A25" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>251</v>
       </c>
     </row>
@@ -2327,13 +2340,13 @@
       <c r="A27" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" t="s" s="0">
         <v>258</v>
       </c>
     </row>
@@ -2341,13 +2354,13 @@
       <c r="A28" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" t="s" s="0">
         <v>258</v>
       </c>
     </row>
@@ -2355,16 +2368,16 @@
       <c r="A29" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="s" s="0">
         <v>258</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" t="s" s="0">
         <v>232</v>
       </c>
     </row>
@@ -2372,16 +2385,16 @@
       <c r="A30" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>258</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" t="s" s="0">
         <v>232</v>
       </c>
     </row>
@@ -2389,13 +2402,13 @@
       <c r="A31" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" t="s" s="0">
         <v>258</v>
       </c>
     </row>
@@ -2413,13 +2426,13 @@
       <c r="A33" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>265</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" t="s" s="0">
         <v>270</v>
       </c>
     </row>
@@ -2427,13 +2440,13 @@
       <c r="A34" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="0">
         <v>266</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="s" s="0">
         <v>270</v>
       </c>
     </row>
@@ -2441,13 +2454,13 @@
       <c r="A35" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="0">
         <v>267</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" t="s" s="0">
         <v>270</v>
       </c>
     </row>
@@ -2455,13 +2468,13 @@
       <c r="A36" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>268</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" t="s" s="0">
         <v>270</v>
       </c>
     </row>
@@ -2469,13 +2482,13 @@
       <c r="A37" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>269</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" t="s" s="0">
         <v>270</v>
       </c>
     </row>
@@ -2493,13 +2506,13 @@
       <c r="A39" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>277</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" t="s" s="0">
         <v>282</v>
       </c>
     </row>
@@ -2507,13 +2520,13 @@
       <c r="A40" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>278</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" t="s" s="0">
         <v>282</v>
       </c>
     </row>
@@ -2521,13 +2534,13 @@
       <c r="A41" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="s" s="0">
         <v>279</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" t="s" s="0">
         <v>282</v>
       </c>
     </row>
@@ -2535,13 +2548,13 @@
       <c r="A42" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="s" s="0">
         <v>280</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>282</v>
       </c>
     </row>
@@ -2549,13 +2562,13 @@
       <c r="A43" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" t="s" s="0">
         <v>281</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" t="s" s="0">
         <v>282</v>
       </c>
     </row>
@@ -2573,13 +2586,13 @@
       <c r="A45" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" t="s" s="0">
         <v>288</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" t="s" s="0">
         <v>293</v>
       </c>
     </row>
@@ -2587,13 +2600,13 @@
       <c r="A46" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" t="s" s="0">
         <v>289</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" t="s" s="0">
         <v>293</v>
       </c>
     </row>
@@ -2601,13 +2614,13 @@
       <c r="A47" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" t="s" s="0">
         <v>290</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" t="s" s="0">
         <v>293</v>
       </c>
     </row>
@@ -2615,13 +2628,13 @@
       <c r="A48" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" t="s" s="0">
         <v>291</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" t="s" s="0">
         <v>293</v>
       </c>
     </row>
@@ -2629,13 +2642,13 @@
       <c r="A49" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" t="s" s="0">
         <v>293</v>
       </c>
     </row>
@@ -2653,13 +2666,13 @@
       <c r="A51" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" t="s" s="0">
         <v>305</v>
       </c>
     </row>
@@ -2667,13 +2680,13 @@
       <c r="A52" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" t="s" s="0">
         <v>301</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" t="s" s="0">
         <v>305</v>
       </c>
     </row>
@@ -2681,13 +2694,13 @@
       <c r="A53" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" t="s" s="0">
         <v>302</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" t="s" s="0">
         <v>305</v>
       </c>
     </row>
@@ -2695,13 +2708,13 @@
       <c r="A54" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>305</v>
       </c>
     </row>
@@ -2709,13 +2722,13 @@
       <c r="A55" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" t="s" s="0">
         <v>304</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" t="s" s="0">
         <v>305</v>
       </c>
     </row>
@@ -2733,13 +2746,13 @@
       <c r="A57" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" t="s" s="0">
         <v>306</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" t="s" s="0">
         <v>312</v>
       </c>
     </row>
@@ -2747,13 +2760,13 @@
       <c r="A58" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" t="s" s="0">
         <v>306</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>312</v>
       </c>
     </row>
@@ -2761,13 +2774,13 @@
       <c r="A59" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" t="s" s="0">
         <v>306</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" t="s" s="0">
         <v>312</v>
       </c>
     </row>
@@ -2775,13 +2788,13 @@
       <c r="A60" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" t="s" s="0">
         <v>306</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" t="s" s="0">
         <v>312</v>
       </c>
     </row>
@@ -2789,13 +2802,13 @@
       <c r="A61" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" t="s" s="0">
         <v>306</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" t="s" s="0">
         <v>312</v>
       </c>
     </row>
@@ -2813,13 +2826,13 @@
       <c r="A63" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" t="s" s="0">
         <v>313</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" t="s" s="0">
         <v>320</v>
       </c>
     </row>
@@ -2827,13 +2840,13 @@
       <c r="A64" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" t="s" s="0">
         <v>316</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" t="s" s="0">
         <v>313</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" t="s" s="0">
         <v>320</v>
       </c>
     </row>
@@ -2841,13 +2854,13 @@
       <c r="A65" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" t="s" s="0">
         <v>317</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" t="s" s="0">
         <v>313</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" t="s" s="0">
         <v>320</v>
       </c>
     </row>
@@ -2855,13 +2868,13 @@
       <c r="A66" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" t="s" s="0">
         <v>318</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" t="s" s="0">
         <v>313</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" t="s" s="0">
         <v>320</v>
       </c>
     </row>
@@ -2869,13 +2882,13 @@
       <c r="A67" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" t="s" s="0">
         <v>319</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" t="s" s="0">
         <v>313</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" t="s" s="0">
         <v>320</v>
       </c>
     </row>
@@ -2893,13 +2906,13 @@
       <c r="A69" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" t="s" s="0">
         <v>337</v>
       </c>
     </row>
@@ -2907,13 +2920,13 @@
       <c r="A70" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" t="s" s="0">
         <v>326</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" t="s" s="0">
         <v>337</v>
       </c>
     </row>
@@ -2921,13 +2934,13 @@
       <c r="A71" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" t="s" s="0">
         <v>327</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" t="s" s="0">
         <v>337</v>
       </c>
     </row>
@@ -2935,13 +2948,13 @@
       <c r="A72" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" t="s" s="0">
         <v>328</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" t="s" s="0">
         <v>337</v>
       </c>
     </row>
@@ -2949,13 +2962,13 @@
       <c r="A73" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" t="s" s="0">
         <v>337</v>
       </c>
     </row>
@@ -2973,13 +2986,13 @@
       <c r="A75" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" t="s" s="0">
         <v>344</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" t="s" s="0">
         <v>403</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" t="s" s="0">
         <v>349</v>
       </c>
     </row>
@@ -2987,13 +3000,13 @@
       <c r="A76" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" t="s" s="0">
         <v>345</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" t="s" s="0">
         <v>403</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" t="s" s="0">
         <v>349</v>
       </c>
     </row>
@@ -3001,13 +3014,13 @@
       <c r="A77" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" t="s" s="0">
         <v>346</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" t="s" s="0">
         <v>403</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" t="s" s="0">
         <v>349</v>
       </c>
     </row>
@@ -3015,13 +3028,13 @@
       <c r="A78" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" t="s" s="0">
         <v>347</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" t="s" s="0">
         <v>403</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" t="s" s="0">
         <v>349</v>
       </c>
     </row>
@@ -3029,13 +3042,13 @@
       <c r="A79" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" t="s" s="0">
         <v>348</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" t="s" s="0">
         <v>403</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" t="s" s="0">
         <v>349</v>
       </c>
     </row>
@@ -3055,22 +3068,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.44140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.21875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.44140625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.21875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.33203125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="40.21875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="17.21875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.44140625"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.77734375"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -3124,10 +3137,10 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -3136,34 +3149,34 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>76</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>81</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>84</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -3174,10 +3187,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>301</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3186,34 +3199,34 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>86</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>94</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -3224,10 +3237,10 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>302</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -3236,34 +3249,34 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>104</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -3274,10 +3287,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -3286,31 +3299,31 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>106</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>112</v>
       </c>
       <c r="N5" s="3" t="s">
@@ -3324,10 +3337,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>304</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -3336,31 +3349,31 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>114</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>127</v>
       </c>
       <c r="N6" s="3" t="s">
@@ -3403,10 +3416,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -3424,10 +3437,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>407</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -3438,10 +3451,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>407</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3452,10 +3465,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>407</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -3466,10 +3479,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>407</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -3480,10 +3493,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>407</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -3515,25 +3528,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.21875" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.77734375"/>
+    <col min="7" max="7" customWidth="true" width="21.77734375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="28.88671875"/>
+    <col min="9" max="9" customWidth="true" width="24.21875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5546875"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="28.88671875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="21.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -3578,193 +3591,208 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>396</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>465</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>468</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>470</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>464</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>201</v>
       </c>
+      <c r="M2" t="s" s="0">
+        <v>485</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>316</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>480</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>399</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>400</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>401</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>402</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>396</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>161</v>
       </c>
+      <c r="M3" t="s" s="0">
+        <v>486</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>317</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>472</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>468</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>473</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>464</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>474</v>
       </c>
-      <c r="K4" t="s">
-        <v>480</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="K4" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="L4" t="s" s="0">
         <v>163</v>
       </c>
+      <c r="M4" t="s" s="0">
+        <v>487</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>318</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>399</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>199</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>401</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>475</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>396</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
+        <v>465</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>464</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>477</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>401</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>478</v>
+      </c>
+      <c r="I6" t="s" s="0">
         <v>476</v>
       </c>
-      <c r="L5" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>319</v>
-      </c>
-      <c r="B6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="J6" t="s" s="0">
+        <v>203</v>
+      </c>
+      <c r="K6" t="s" s="0">
         <v>464</v>
       </c>
-      <c r="F6" t="s">
-        <v>478</v>
-      </c>
-      <c r="G6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H6" t="s">
-        <v>479</v>
-      </c>
-      <c r="I6" t="s">
-        <v>476</v>
-      </c>
-      <c r="J6" t="s">
-        <v>203</v>
-      </c>
-      <c r="K6" t="s">
-        <v>464</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>162</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -3793,19 +3821,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.6640625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.21875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.77734375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.21875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.33203125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.6640625"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -3865,16 +3893,16 @@
       <c r="E2" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>181</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -3903,16 +3931,16 @@
       <c r="E3" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>181</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -3941,16 +3969,16 @@
       <c r="E4" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>181</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -3979,16 +4007,16 @@
       <c r="E5" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>181</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -4017,16 +4045,16 @@
       <c r="E6" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>181</v>
       </c>
       <c r="J6" s="3" t="s">
@@ -4067,17 +4095,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.6640625"/>
+    <col min="4" max="4" customWidth="true" width="13.88671875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="59.6640625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.21875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.44140625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.0"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -4119,10 +4147,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>344</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>403</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -4131,33 +4159,33 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>391</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>393</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>394</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>345</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>403</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -4166,33 +4194,33 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>396</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>393</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>394</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>346</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>403</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -4201,33 +4229,33 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>397</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>398</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>393</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>394</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>347</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>403</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -4236,33 +4264,33 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>399</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>393</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>394</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>348</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>403</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -4271,25 +4299,25 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>401</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>393</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>394</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>395</v>
       </c>
     </row>
@@ -4322,10 +4350,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4343,13 +4371,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4357,13 +4385,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4371,13 +4399,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -4385,13 +4413,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -4399,13 +4427,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -4434,16 +4462,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.21875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.44140625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="25.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -4479,28 +4507,28 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>189</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -4511,28 +4539,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>190</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>32</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -4543,28 +4571,28 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>59</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -4575,60 +4603,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>65</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -4669,16 +4697,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.21875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="30.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.21875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="19.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -4714,162 +4742,162 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>156</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>157</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>158</v>
       </c>
     </row>
@@ -4896,11 +4924,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -4936,13 +4964,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>246</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4954,7 +4982,7 @@
       <c r="F2" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>136</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -4963,18 +4991,18 @@
       <c r="I2" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>247</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4986,7 +5014,7 @@
       <c r="F3" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>136</v>
       </c>
       <c r="H3" s="12" t="s">
@@ -4995,18 +5023,18 @@
       <c r="I3" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>248</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -5018,7 +5046,7 @@
       <c r="F4" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>136</v>
       </c>
       <c r="H4" s="12" t="s">
@@ -5027,18 +5055,18 @@
       <c r="I4" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>249</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -5050,7 +5078,7 @@
       <c r="F5" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>136</v>
       </c>
       <c r="H5" s="12" t="s">
@@ -5059,18 +5087,18 @@
       <c r="I5" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -5082,7 +5110,7 @@
       <c r="F6" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>136</v>
       </c>
       <c r="H6" s="12" t="s">
@@ -5091,7 +5119,7 @@
       <c r="I6" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>147</v>
       </c>
     </row>
@@ -5117,13 +5145,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.6640625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.88671875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -5153,132 +5181,132 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>136</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>208</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>210</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>211</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>212</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>209</v>
       </c>
     </row>
@@ -5304,19 +5332,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.21875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="32.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="26.21875"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" width="14.33203125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.109375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.44140625"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.33203125"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5354,38 +5382,38 @@
         <v>419</v>
       </c>
       <c r="L1" s="14" t="s">
+        <v>481</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>484</v>
-      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>265</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>408</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>410</v>
       </c>
-      <c r="G2" t="s">
-        <v>481</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>414</v>
       </c>
       <c r="I2" s="11" t="s">
@@ -5405,28 +5433,28 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>266</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>410</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>412</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>414</v>
       </c>
       <c r="I3" s="11" t="s">
@@ -5446,28 +5474,28 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>267</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>417</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>410</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>412</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>414</v>
       </c>
       <c r="I4" s="11" t="s">
@@ -5487,28 +5515,28 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>268</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>418</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>410</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>412</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>414</v>
       </c>
       <c r="I5" s="11" t="s">
@@ -5528,28 +5556,28 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>269</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>410</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>412</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>414</v>
       </c>
       <c r="I6" s="11" t="s">
@@ -5561,8 +5589,8 @@
       <c r="K6" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="L6" t="s">
-        <v>485</v>
+      <c r="L6" t="s" s="0">
+        <v>484</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>10</v>
@@ -5595,11 +5623,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -5620,87 +5648,87 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>277</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>278</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>279</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>280</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>281</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>361</v>
       </c>
     </row>
@@ -5727,14 +5755,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.21875"/>
+    <col min="6" max="6" customWidth="true" width="9.21875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.5546875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -5767,10 +5795,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>442</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>443</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5779,10 +5807,10 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>445</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>446</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -5796,10 +5824,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>447</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>443</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5808,10 +5836,10 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>449</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>450</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -5825,10 +5853,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>451</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>443</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5837,10 +5865,10 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>453</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>454</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -5854,10 +5882,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>455</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>443</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5866,10 +5894,10 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>457</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>453</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -5883,10 +5911,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>458</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>443</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5895,10 +5923,10 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>454</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>457</v>
       </c>
       <c r="G6" s="2" t="s">

</xml_diff>

<commit_message>
Latest Code changes of Apply Discount
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0030F632-9466-4857-A077-C52E41831BDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46846041-F771-4525-8A00-DDD6A5F48126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="20925" windowHeight="12435" tabRatio="877" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="467">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -496,9 +496,6 @@
     <t>Health Book</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
     <t>Apply Discount Code</t>
   </si>
   <si>
@@ -524,15 +521,6 @@
   </si>
   <si>
     <t>Credit Card</t>
-  </si>
-  <si>
-    <t>Build your own computer</t>
-  </si>
-  <si>
-    <t>Build your own expensive computer</t>
-  </si>
-  <si>
-    <t>Simple Computer</t>
   </si>
   <si>
     <t>Barbara Gordon</t>
@@ -1514,7 +1502,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1548,12 +1536,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1563,12 +1564,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1581,6 +1576,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1902,17 +1902,17 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>
@@ -1921,680 +1921,680 @@
         <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E13" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D17" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E17" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D19" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" t="s">
+        <v>323</v>
+      </c>
+      <c r="D21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" t="s">
+        <v>323</v>
+      </c>
+      <c r="D22" t="s">
+        <v>221</v>
+      </c>
+      <c r="E22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B23" t="s">
+        <v>218</v>
+      </c>
+      <c r="C23" t="s">
+        <v>323</v>
+      </c>
+      <c r="D23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>220</v>
       </c>
-      <c r="C21" t="s">
-        <v>327</v>
-      </c>
-      <c r="D21" t="s">
-        <v>225</v>
-      </c>
-      <c r="E21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C25" t="s">
+        <v>323</v>
+      </c>
+      <c r="D25" t="s">
         <v>221</v>
       </c>
-      <c r="C22" t="s">
-        <v>327</v>
-      </c>
-      <c r="D22" t="s">
-        <v>225</v>
-      </c>
-      <c r="E22" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B23" t="s">
-        <v>222</v>
-      </c>
-      <c r="C23" t="s">
-        <v>327</v>
-      </c>
-      <c r="D23" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B24" t="s">
-        <v>223</v>
-      </c>
-      <c r="C24" t="s">
-        <v>327</v>
-      </c>
-      <c r="D24" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B25" t="s">
-        <v>224</v>
-      </c>
-      <c r="C25" t="s">
-        <v>327</v>
-      </c>
-      <c r="D25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" t="s">
+        <v>324</v>
+      </c>
+      <c r="D27" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" t="s">
+        <v>324</v>
+      </c>
+      <c r="D28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B29" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" t="s">
+        <v>324</v>
+      </c>
+      <c r="D29" t="s">
+        <v>228</v>
+      </c>
+      <c r="E29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" t="s">
+        <v>324</v>
+      </c>
+      <c r="D30" t="s">
+        <v>228</v>
+      </c>
+      <c r="E30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B27" t="s">
-        <v>170</v>
-      </c>
-      <c r="C27" t="s">
-        <v>328</v>
-      </c>
-      <c r="D27" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="B31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" t="s">
+        <v>324</v>
+      </c>
+      <c r="D31" t="s">
         <v>228</v>
       </c>
-      <c r="B28" t="s">
-        <v>174</v>
-      </c>
-      <c r="C28" t="s">
-        <v>328</v>
-      </c>
-      <c r="D28" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B29" t="s">
-        <v>176</v>
-      </c>
-      <c r="C29" t="s">
-        <v>328</v>
-      </c>
-      <c r="D29" t="s">
-        <v>232</v>
-      </c>
-      <c r="E29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B30" t="s">
-        <v>178</v>
-      </c>
-      <c r="C30" t="s">
-        <v>328</v>
-      </c>
-      <c r="D30" t="s">
-        <v>232</v>
-      </c>
-      <c r="E30" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B31" t="s">
-        <v>179</v>
-      </c>
-      <c r="C31" t="s">
-        <v>328</v>
-      </c>
-      <c r="D31" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33" t="s">
+        <v>235</v>
+      </c>
+      <c r="C33" t="s">
+        <v>325</v>
+      </c>
+      <c r="D33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34" t="s">
+        <v>236</v>
+      </c>
+      <c r="C34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D34" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" t="s">
+        <v>237</v>
+      </c>
+      <c r="C35" t="s">
+        <v>325</v>
+      </c>
+      <c r="D35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B36" t="s">
+        <v>238</v>
+      </c>
+      <c r="C36" t="s">
+        <v>325</v>
+      </c>
+      <c r="D36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>239</v>
       </c>
-      <c r="C33" t="s">
-        <v>329</v>
-      </c>
-      <c r="D33" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C37" t="s">
+        <v>325</v>
+      </c>
+      <c r="D37" t="s">
         <v>240</v>
       </c>
-      <c r="C34" t="s">
-        <v>329</v>
-      </c>
-      <c r="D34" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B35" t="s">
-        <v>241</v>
-      </c>
-      <c r="C35" t="s">
-        <v>329</v>
-      </c>
-      <c r="D35" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B36" t="s">
-        <v>242</v>
-      </c>
-      <c r="C36" t="s">
-        <v>329</v>
-      </c>
-      <c r="D36" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B37" t="s">
-        <v>243</v>
-      </c>
-      <c r="C37" t="s">
-        <v>329</v>
-      </c>
-      <c r="D37" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B39" t="s">
+        <v>247</v>
+      </c>
+      <c r="C39" t="s">
+        <v>326</v>
+      </c>
+      <c r="D39" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B40" t="s">
+        <v>248</v>
+      </c>
+      <c r="C40" t="s">
+        <v>326</v>
+      </c>
+      <c r="D40" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B41" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" t="s">
+        <v>326</v>
+      </c>
+      <c r="D41" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B42" t="s">
+        <v>250</v>
+      </c>
+      <c r="C42" t="s">
+        <v>326</v>
+      </c>
+      <c r="D42" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B43" t="s">
         <v>251</v>
       </c>
-      <c r="C39" t="s">
-        <v>330</v>
-      </c>
-      <c r="D39" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C43" t="s">
+        <v>326</v>
+      </c>
+      <c r="D43" t="s">
         <v>252</v>
       </c>
-      <c r="C40" t="s">
-        <v>330</v>
-      </c>
-      <c r="D40" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B41" t="s">
-        <v>253</v>
-      </c>
-      <c r="C41" t="s">
-        <v>330</v>
-      </c>
-      <c r="D41" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="B42" t="s">
-        <v>254</v>
-      </c>
-      <c r="C42" t="s">
-        <v>330</v>
-      </c>
-      <c r="D42" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B43" t="s">
-        <v>255</v>
-      </c>
-      <c r="C43" t="s">
-        <v>330</v>
-      </c>
-      <c r="D43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B45" t="s">
+        <v>258</v>
+      </c>
+      <c r="C45" t="s">
+        <v>332</v>
+      </c>
+      <c r="D45" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B46" t="s">
+        <v>259</v>
+      </c>
+      <c r="C46" t="s">
+        <v>332</v>
+      </c>
+      <c r="D46" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B47" t="s">
+        <v>260</v>
+      </c>
+      <c r="C47" t="s">
+        <v>332</v>
+      </c>
+      <c r="D47" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B48" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" t="s">
+        <v>332</v>
+      </c>
+      <c r="D48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B49" t="s">
         <v>262</v>
       </c>
-      <c r="C45" t="s">
-        <v>336</v>
-      </c>
-      <c r="D45" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C49" t="s">
+        <v>332</v>
+      </c>
+      <c r="D49" t="s">
         <v>263</v>
       </c>
-      <c r="C46" t="s">
-        <v>336</v>
-      </c>
-      <c r="D46" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B47" t="s">
-        <v>264</v>
-      </c>
-      <c r="C47" t="s">
-        <v>336</v>
-      </c>
-      <c r="D47" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B48" t="s">
-        <v>265</v>
-      </c>
-      <c r="C48" t="s">
-        <v>336</v>
-      </c>
-      <c r="D48" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B49" t="s">
-        <v>266</v>
-      </c>
-      <c r="C49" t="s">
-        <v>336</v>
-      </c>
-      <c r="D49" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2604,394 +2604,394 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B51" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B52" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C52" t="s">
         <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B53" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C53" t="s">
         <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B54" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B55" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B57" t="s">
         <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D57" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B58" t="s">
         <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D58" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B59" t="s">
         <v>36</v>
       </c>
       <c r="C59" t="s">
+        <v>276</v>
+      </c>
+      <c r="D59" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="D59" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="B60" t="s">
         <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D60" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B61" t="s">
         <v>38</v>
       </c>
       <c r="C61" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D61" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B63" t="s">
+        <v>285</v>
+      </c>
+      <c r="C63" t="s">
+        <v>283</v>
+      </c>
+      <c r="D63" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B64" t="s">
+        <v>286</v>
+      </c>
+      <c r="C64" t="s">
+        <v>283</v>
+      </c>
+      <c r="D64" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B65" t="s">
+        <v>287</v>
+      </c>
+      <c r="C65" t="s">
+        <v>283</v>
+      </c>
+      <c r="D65" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B66" t="s">
         <v>288</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C66" t="s">
+        <v>283</v>
+      </c>
+      <c r="D66" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B67" t="s">
         <v>289</v>
       </c>
-      <c r="C63" t="s">
-        <v>287</v>
-      </c>
-      <c r="D63" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C67" t="s">
+        <v>283</v>
+      </c>
+      <c r="D67" t="s">
         <v>290</v>
       </c>
-      <c r="C64" t="s">
-        <v>287</v>
-      </c>
-      <c r="D64" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="B65" t="s">
-        <v>291</v>
-      </c>
-      <c r="C65" t="s">
-        <v>287</v>
-      </c>
-      <c r="D65" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="B66" t="s">
-        <v>292</v>
-      </c>
-      <c r="C66" t="s">
-        <v>287</v>
-      </c>
-      <c r="D66" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="B67" t="s">
-        <v>293</v>
-      </c>
-      <c r="C67" t="s">
-        <v>287</v>
-      </c>
-      <c r="D67" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B69" t="s">
+        <v>295</v>
+      </c>
+      <c r="C69" t="s">
+        <v>301</v>
+      </c>
+      <c r="D69" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B70" t="s">
+        <v>296</v>
+      </c>
+      <c r="C70" t="s">
+        <v>301</v>
+      </c>
+      <c r="D70" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B71" t="s">
+        <v>297</v>
+      </c>
+      <c r="C71" t="s">
+        <v>301</v>
+      </c>
+      <c r="D71" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B72" t="s">
+        <v>298</v>
+      </c>
+      <c r="C72" t="s">
+        <v>301</v>
+      </c>
+      <c r="D72" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B73" t="s">
         <v>299</v>
       </c>
-      <c r="C69" t="s">
-        <v>305</v>
-      </c>
-      <c r="D69" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="C73" t="s">
+        <v>301</v>
+      </c>
+      <c r="D73" t="s">
         <v>307</v>
       </c>
-      <c r="B70" t="s">
-        <v>300</v>
-      </c>
-      <c r="C70" t="s">
-        <v>305</v>
-      </c>
-      <c r="D70" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="B71" t="s">
-        <v>301</v>
-      </c>
-      <c r="C71" t="s">
-        <v>305</v>
-      </c>
-      <c r="D71" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B72" t="s">
-        <v>302</v>
-      </c>
-      <c r="C72" t="s">
-        <v>305</v>
-      </c>
-      <c r="D72" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="B73" t="s">
-        <v>303</v>
-      </c>
-      <c r="C73" t="s">
-        <v>305</v>
-      </c>
-      <c r="D73" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B75" t="s">
+        <v>314</v>
+      </c>
+      <c r="C75" t="s">
+        <v>373</v>
+      </c>
+      <c r="D75" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B76" t="s">
+        <v>315</v>
+      </c>
+      <c r="C76" t="s">
+        <v>373</v>
+      </c>
+      <c r="D76" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B77" t="s">
+        <v>316</v>
+      </c>
+      <c r="C77" t="s">
+        <v>373</v>
+      </c>
+      <c r="D77" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C78" t="s">
+        <v>373</v>
+      </c>
+      <c r="D78" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B79" t="s">
         <v>318</v>
       </c>
-      <c r="C75" t="s">
-        <v>377</v>
-      </c>
-      <c r="D75" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="C79" t="s">
+        <v>373</v>
+      </c>
+      <c r="D79" t="s">
         <v>319</v>
-      </c>
-      <c r="C76" t="s">
-        <v>377</v>
-      </c>
-      <c r="D76" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="B77" t="s">
-        <v>320</v>
-      </c>
-      <c r="C77" t="s">
-        <v>377</v>
-      </c>
-      <c r="D77" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="B78" t="s">
-        <v>321</v>
-      </c>
-      <c r="C78" t="s">
-        <v>377</v>
-      </c>
-      <c r="D78" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="B79" t="s">
-        <v>322</v>
-      </c>
-      <c r="C79" t="s">
-        <v>377</v>
-      </c>
-      <c r="D79" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3008,27 +3008,27 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3078,9 +3078,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -3128,9 +3128,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -3178,9 +3178,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
@@ -3228,9 +3228,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -3278,9 +3278,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -3356,15 +3356,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3372,18 +3372,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -3392,12 +3392,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -3406,12 +3406,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -3420,12 +3420,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -3434,12 +3434,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -3470,28 +3470,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3499,45 +3499,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -3546,39 +3546,39 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F2" t="s">
         <v>146</v>
       </c>
       <c r="G2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="J2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="L2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -3587,39 +3587,39 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F3" t="s">
         <v>147</v>
       </c>
       <c r="G3" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I3" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="J3" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="K3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="L3" t="s">
         <v>148</v>
       </c>
       <c r="M3" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -3628,39 +3628,39 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G4" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="H4" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="I4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="J4" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="K4" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="L4" t="s">
         <v>150</v>
       </c>
       <c r="M4" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -3669,39 +3669,39 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G5" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="I5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J5" t="s">
         <v>151</v>
       </c>
       <c r="K5" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="L5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -3710,31 +3710,31 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="F6" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H6" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="I6" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="J6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K6" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="L6" t="s">
         <v>149</v>
       </c>
       <c r="M6" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -3755,68 +3755,72 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="A1:XFD1048576"/>
+      <selection activeCell="E6" sqref="E6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>33</v>
@@ -3824,31 +3828,35 @@
       <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="H2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>300</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>304</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>33</v>
@@ -3856,31 +3864,35 @@
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" t="s">
+        <v>435</v>
+      </c>
+      <c r="F3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="F3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -3888,31 +3900,35 @@
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="K4" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="F4" t="s">
-        <v>160</v>
-      </c>
-      <c r="G4" t="s">
-        <v>161</v>
-      </c>
-      <c r="H4" t="s">
-        <v>165</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>33</v>
@@ -3920,31 +3936,35 @@
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="H5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>33</v>
@@ -3952,24 +3972,28 @@
       <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" t="s">
+        <v>438</v>
+      </c>
+      <c r="F6" t="s">
+        <v>440</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="H6" t="s">
-        <v>165</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>167</v>
-      </c>
+      <c r="J6" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="L6" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3997,65 +4021,65 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -4064,33 +4088,33 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I2" t="s">
+        <v>363</v>
+      </c>
+      <c r="J2" t="s">
+        <v>364</v>
+      </c>
+      <c r="K2" t="s">
         <v>365</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G2" t="s">
-        <v>366</v>
-      </c>
-      <c r="H2" t="s">
-        <v>366</v>
-      </c>
-      <c r="I2" t="s">
-        <v>367</v>
-      </c>
-      <c r="J2" t="s">
-        <v>368</v>
-      </c>
-      <c r="K2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B3" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -4099,33 +4123,33 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>146</v>
       </c>
       <c r="G3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="I3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="J3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="K3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -4134,33 +4158,33 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F4" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G4" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H4" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="I4" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="J4" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="K4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B5" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -4169,33 +4193,33 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="G5" t="s">
+        <v>362</v>
+      </c>
+      <c r="H5" t="s">
+        <v>362</v>
+      </c>
+      <c r="I5" t="s">
+        <v>363</v>
+      </c>
+      <c r="J5" t="s">
+        <v>364</v>
+      </c>
+      <c r="K5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B6" t="s">
         <v>373</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="G5" t="s">
-        <v>366</v>
-      </c>
-      <c r="H5" t="s">
-        <v>366</v>
-      </c>
-      <c r="I5" t="s">
-        <v>367</v>
-      </c>
-      <c r="J5" t="s">
-        <v>368</v>
-      </c>
-      <c r="K5" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B6" t="s">
-        <v>377</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -4204,25 +4228,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="G6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="I6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="J6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="K6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -4252,15 +4276,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4274,12 +4298,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4288,12 +4312,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -4302,12 +4326,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -4316,12 +4340,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -4330,12 +4354,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4364,21 +4388,21 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4395,7 +4419,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -4404,18 +4428,18 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4427,7 +4451,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4442,12 +4466,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4459,7 +4483,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -4474,12 +4498,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4491,7 +4515,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4506,12 +4530,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4523,7 +4547,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -4538,12 +4562,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4555,7 +4579,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4599,19 +4623,19 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4637,12 +4661,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4654,7 +4678,7 @@
         <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="G2" t="s">
         <v>134</v>
@@ -4663,12 +4687,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4683,18 +4707,18 @@
         <v>133</v>
       </c>
       <c r="G3" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4715,12 +4739,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4741,12 +4765,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4788,16 +4812,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4811,30 +4835,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4842,31 +4866,31 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>343</v>
+      <c r="E2" s="9" t="s">
+        <v>339</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G2" t="s">
         <v>134</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>343</v>
+      <c r="H2" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4874,31 +4898,31 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>346</v>
+      <c r="E3" s="9" t="s">
+        <v>342</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G3" t="s">
         <v>134</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>346</v>
+      <c r="H3" s="10" t="s">
+        <v>342</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="J3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4906,31 +4930,31 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>349</v>
+      <c r="E4" s="9" t="s">
+        <v>345</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G4" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>349</v>
+      <c r="H4" s="10" t="s">
+        <v>345</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="J4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4938,31 +4962,31 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>352</v>
+      <c r="E5" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>352</v>
+      <c r="H5" s="10" t="s">
+        <v>348</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="J5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4970,20 +4994,20 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>355</v>
+      <c r="E6" s="9" t="s">
+        <v>351</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G6" t="s">
         <v>134</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>355</v>
+      <c r="H6" s="10" t="s">
+        <v>351</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="J6" t="s">
         <v>140</v>
@@ -5009,18 +5033,18 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5028,30 +5052,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5062,22 +5086,22 @@
       <c r="E2" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>400</v>
+      <c r="F2" s="10" t="s">
+        <v>396</v>
       </c>
       <c r="G2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="H2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5086,24 +5110,24 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>402</v>
+        <v>178</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>398</v>
       </c>
       <c r="G3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="H3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5112,24 +5136,24 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="G4" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="H4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5138,24 +5162,24 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="G5" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="H5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5164,16 +5188,16 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G6" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="H6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -5196,24 +5220,24 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5230,39 +5254,39 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>455</v>
+      <c r="L1" s="12" t="s">
+        <v>451</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5271,25 +5295,25 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G2" t="s">
+        <v>450</v>
+      </c>
+      <c r="H2" t="s">
         <v>384</v>
       </c>
-      <c r="G2" t="s">
-        <v>454</v>
-      </c>
-      <c r="H2" t="s">
-        <v>388</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>409</v>
+      <c r="I2" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>405</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>10</v>
@@ -5298,12 +5322,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5315,22 +5339,22 @@
         <v>56</v>
       </c>
       <c r="F3" t="s">
+        <v>380</v>
+      </c>
+      <c r="G3" t="s">
+        <v>382</v>
+      </c>
+      <c r="H3" t="s">
         <v>384</v>
       </c>
-      <c r="G3" t="s">
-        <v>386</v>
-      </c>
-      <c r="H3" t="s">
-        <v>388</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>409</v>
+      <c r="I3" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>405</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>10</v>
@@ -5339,12 +5363,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5353,25 +5377,25 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F4" t="s">
+        <v>380</v>
+      </c>
+      <c r="G4" t="s">
+        <v>382</v>
+      </c>
+      <c r="H4" t="s">
         <v>384</v>
       </c>
-      <c r="G4" t="s">
-        <v>386</v>
-      </c>
-      <c r="H4" t="s">
-        <v>388</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>409</v>
+      <c r="I4" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>405</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -5380,12 +5404,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5394,25 +5418,25 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="F5" t="s">
+        <v>380</v>
+      </c>
+      <c r="G5" t="s">
+        <v>382</v>
+      </c>
+      <c r="H5" t="s">
         <v>384</v>
       </c>
-      <c r="G5" t="s">
-        <v>386</v>
-      </c>
-      <c r="H5" t="s">
-        <v>388</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>409</v>
+      <c r="I5" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>405</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>10</v>
@@ -5421,12 +5445,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B6" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5438,25 +5462,25 @@
         <v>59</v>
       </c>
       <c r="F6" t="s">
+        <v>380</v>
+      </c>
+      <c r="G6" t="s">
+        <v>382</v>
+      </c>
+      <c r="H6" t="s">
         <v>384</v>
       </c>
-      <c r="G6" t="s">
-        <v>386</v>
-      </c>
-      <c r="H6" t="s">
-        <v>388</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>409</v>
+      <c r="I6" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>405</v>
       </c>
       <c r="L6" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>10</v>
@@ -5487,16 +5511,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5504,21 +5528,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5527,15 +5551,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5544,15 +5568,15 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5561,15 +5585,15 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5578,15 +5602,15 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B6" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5595,7 +5619,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -5619,184 +5643,184 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="G1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="C1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>412</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="B2" t="s">
         <v>413</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="C2" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="13" t="s">
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
         <v>416</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>417</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>419</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>420</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>421</v>
       </c>
-      <c r="B3" t="s">
-        <v>417</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>423</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>424</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>425</v>
       </c>
-      <c r="B4" t="s">
-        <v>417</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>427</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
+        <v>423</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>428</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>413</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B5" t="s">
-        <v>417</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>431</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>424</v>
+      </c>
+      <c r="F6" t="s">
         <v>427</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>432</v>
-      </c>
-      <c r="B6" t="s">
-        <v>417</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>428</v>
-      </c>
-      <c r="F6" t="s">
-        <v>431</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Latest Code changes of Reports testcases
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46846041-F771-4525-8A00-DDD6A5F48126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8510A5B-8E64-410D-B0D4-D459C8134B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -445,9 +445,6 @@
     <t>Automation</t>
   </si>
   <si>
-    <t>Employee Details</t>
-  </si>
-  <si>
     <t>Travel and Expense Detailed Report</t>
   </si>
   <si>
@@ -1439,6 +1436,9 @@
   </si>
   <si>
     <t>Catalogues77</t>
+  </si>
+  <si>
+    <t>Personal</t>
   </si>
 </sst>
 </file>
@@ -1912,7 +1912,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>
@@ -1921,23 +1921,23 @@
         <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1945,82 +1945,82 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2028,82 +2028,82 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2111,82 +2111,82 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2194,85 +2194,85 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" t="s">
+        <v>322</v>
+      </c>
+      <c r="D25" t="s">
         <v>220</v>
-      </c>
-      <c r="C25" t="s">
-        <v>323</v>
-      </c>
-      <c r="D25" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2280,85 +2280,85 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C28" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C29" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" t="s">
+        <v>323</v>
+      </c>
+      <c r="D31" t="s">
         <v>227</v>
-      </c>
-      <c r="B31" t="s">
-        <v>175</v>
-      </c>
-      <c r="C31" t="s">
-        <v>324</v>
-      </c>
-      <c r="D31" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2366,79 +2366,79 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C33" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C34" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B37" t="s">
+        <v>238</v>
+      </c>
+      <c r="C37" t="s">
+        <v>324</v>
+      </c>
+      <c r="D37" t="s">
         <v>239</v>
-      </c>
-      <c r="C37" t="s">
-        <v>325</v>
-      </c>
-      <c r="D37" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2446,79 +2446,79 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C39" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D39" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C40" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C41" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D41" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B42" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C42" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D42" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B43" t="s">
+        <v>250</v>
+      </c>
+      <c r="C43" t="s">
+        <v>325</v>
+      </c>
+      <c r="D43" t="s">
         <v>251</v>
-      </c>
-      <c r="C43" t="s">
-        <v>326</v>
-      </c>
-      <c r="D43" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2526,72 +2526,72 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C45" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D45" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C46" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D46" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C47" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B49" t="s">
+        <v>261</v>
+      </c>
+      <c r="C49" t="s">
+        <v>331</v>
+      </c>
+      <c r="D49" t="s">
         <v>262</v>
-      </c>
-      <c r="C49" t="s">
-        <v>332</v>
-      </c>
-      <c r="D49" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,79 +2606,79 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B51" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C52" t="s">
         <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C53" t="s">
         <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B54" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B55" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2686,79 +2686,79 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B57" t="s">
         <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D57" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B58" t="s">
         <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D58" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B59" t="s">
         <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D59" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B60" t="s">
         <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D60" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B61" t="s">
         <v>38</v>
       </c>
       <c r="C61" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D61" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2766,79 +2766,79 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B63" t="s">
         <v>284</v>
       </c>
-      <c r="B63" t="s">
-        <v>285</v>
-      </c>
       <c r="C63" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D63" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C64" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D64" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C65" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C66" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D66" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B67" t="s">
+        <v>288</v>
+      </c>
+      <c r="C67" t="s">
+        <v>282</v>
+      </c>
+      <c r="D67" t="s">
         <v>289</v>
-      </c>
-      <c r="C67" t="s">
-        <v>283</v>
-      </c>
-      <c r="D67" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2846,79 +2846,79 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B69" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C69" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D69" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C70" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D70" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C71" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D71" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B72" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C72" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D72" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B73" t="s">
+        <v>298</v>
+      </c>
+      <c r="C73" t="s">
+        <v>300</v>
+      </c>
+      <c r="D73" t="s">
         <v>306</v>
-      </c>
-      <c r="B73" t="s">
-        <v>299</v>
-      </c>
-      <c r="C73" t="s">
-        <v>301</v>
-      </c>
-      <c r="D73" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -2926,72 +2926,72 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B75" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C75" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D75" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B76" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C76" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D76" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B77" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C77" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D77" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B78" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C78" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D78" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B79" t="s">
+        <v>317</v>
+      </c>
+      <c r="C79" t="s">
+        <v>372</v>
+      </c>
+      <c r="D79" t="s">
         <v>318</v>
-      </c>
-      <c r="C79" t="s">
-        <v>373</v>
-      </c>
-      <c r="D79" t="s">
-        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3080,7 +3080,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -3130,7 +3130,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -3372,7 +3372,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -3383,7 +3383,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -3397,7 +3397,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -3411,7 +3411,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -3425,7 +3425,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -3439,7 +3439,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -3499,45 +3499,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>433</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -3546,39 +3546,39 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -3587,39 +3587,39 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" t="s">
+        <v>368</v>
+      </c>
+      <c r="H3" t="s">
+        <v>369</v>
+      </c>
+      <c r="I3" t="s">
+        <v>370</v>
+      </c>
+      <c r="J3" t="s">
+        <v>371</v>
+      </c>
+      <c r="K3" t="s">
+        <v>365</v>
+      </c>
+      <c r="L3" t="s">
         <v>147</v>
       </c>
-      <c r="G3" t="s">
-        <v>369</v>
-      </c>
-      <c r="H3" t="s">
-        <v>370</v>
-      </c>
-      <c r="I3" t="s">
-        <v>371</v>
-      </c>
-      <c r="J3" t="s">
-        <v>372</v>
-      </c>
-      <c r="K3" t="s">
-        <v>366</v>
-      </c>
-      <c r="L3" t="s">
-        <v>148</v>
-      </c>
       <c r="M3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -3628,39 +3628,39 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>441</v>
+      </c>
+      <c r="F4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" t="s">
+        <v>437</v>
+      </c>
+      <c r="H4" t="s">
         <v>442</v>
       </c>
-      <c r="F4" t="s">
-        <v>168</v>
-      </c>
-      <c r="G4" t="s">
-        <v>438</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>433</v>
+      </c>
+      <c r="J4" t="s">
         <v>443</v>
       </c>
-      <c r="I4" t="s">
-        <v>434</v>
-      </c>
-      <c r="J4" t="s">
-        <v>444</v>
-      </c>
       <c r="K4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -3669,39 +3669,39 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -3710,31 +3710,31 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F6" t="s">
+        <v>446</v>
+      </c>
+      <c r="G6" t="s">
+        <v>370</v>
+      </c>
+      <c r="H6" t="s">
         <v>447</v>
       </c>
-      <c r="G6" t="s">
-        <v>371</v>
-      </c>
-      <c r="H6" t="s">
-        <v>448</v>
-      </c>
       <c r="I6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -3757,8 +3757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3791,36 +3791,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>33</v>
@@ -3829,34 +3829,34 @@
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>33</v>
@@ -3865,34 +3865,34 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -3901,34 +3901,34 @@
         <v>10</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G4" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="J4" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>33</v>
@@ -3937,34 +3937,34 @@
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G5" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="J5" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="K5" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>300</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>33</v>
@@ -3973,25 +3973,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G6" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="K6" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="L6" s="14"/>
     </row>
@@ -4038,48 +4038,48 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>393</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -4088,33 +4088,33 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>360</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" t="s">
         <v>361</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I2" t="s">
         <v>362</v>
       </c>
-      <c r="H2" t="s">
-        <v>362</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>363</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>364</v>
-      </c>
-      <c r="K2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -4123,33 +4123,33 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G3" t="s">
+        <v>361</v>
+      </c>
+      <c r="H3" t="s">
+        <v>361</v>
+      </c>
+      <c r="I3" t="s">
         <v>362</v>
       </c>
-      <c r="H3" t="s">
-        <v>362</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>363</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>364</v>
-      </c>
-      <c r="K3" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -4158,33 +4158,33 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F4" t="s">
         <v>367</v>
       </c>
-      <c r="F4" t="s">
-        <v>368</v>
-      </c>
       <c r="G4" t="s">
+        <v>361</v>
+      </c>
+      <c r="H4" t="s">
+        <v>361</v>
+      </c>
+      <c r="I4" t="s">
         <v>362</v>
       </c>
-      <c r="H4" t="s">
-        <v>362</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>363</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>364</v>
-      </c>
-      <c r="K4" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -4193,33 +4193,33 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>368</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>370</v>
-      </c>
       <c r="G5" t="s">
+        <v>361</v>
+      </c>
+      <c r="H5" t="s">
+        <v>361</v>
+      </c>
+      <c r="I5" t="s">
         <v>362</v>
       </c>
-      <c r="H5" t="s">
-        <v>362</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>363</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>364</v>
-      </c>
-      <c r="K5" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -4228,25 +4228,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>370</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>372</v>
-      </c>
       <c r="G6" t="s">
+        <v>361</v>
+      </c>
+      <c r="H6" t="s">
+        <v>361</v>
+      </c>
+      <c r="I6" t="s">
         <v>362</v>
       </c>
-      <c r="H6" t="s">
-        <v>362</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>363</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>364</v>
-      </c>
-      <c r="K6" t="s">
-        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -4303,7 +4303,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4317,7 +4317,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -4331,7 +4331,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -4345,7 +4345,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -4359,7 +4359,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4419,7 +4419,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -4428,10 +4428,10 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -4439,7 +4439,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4451,7 +4451,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4471,7 +4471,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4483,7 +4483,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -4503,7 +4503,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4515,7 +4515,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4535,7 +4535,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4547,7 +4547,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -4567,7 +4567,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4579,7 +4579,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4619,8 +4619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4629,7 +4629,7 @@
     <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
@@ -4666,7 +4666,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4678,13 +4678,13 @@
         <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G2" t="s">
         <v>134</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>466</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -4692,7 +4692,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4701,16 +4701,16 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F3" t="s">
         <v>133</v>
       </c>
       <c r="G3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4718,7 +4718,7 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4727,16 +4727,16 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F4" t="s">
         <v>133</v>
       </c>
       <c r="G4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" t="s">
         <v>140</v>
-      </c>
-      <c r="H4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4744,7 +4744,7 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4756,13 +4756,13 @@
         <v>132</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H5" t="s">
         <v>142</v>
-      </c>
-      <c r="H5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4770,7 +4770,7 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4779,16 +4779,16 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F6" t="s">
         <v>133</v>
       </c>
       <c r="G6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" t="s">
         <v>144</v>
-      </c>
-      <c r="H6" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4835,30 +4835,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4867,30 +4867,30 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G2" t="s">
         <v>134</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>340</v>
-      </c>
       <c r="J2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4899,30 +4899,30 @@
         <v>10</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G3" t="s">
         <v>134</v>
       </c>
       <c r="H3" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>343</v>
-      </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4931,30 +4931,30 @@
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G4" t="s">
         <v>134</v>
       </c>
       <c r="H4" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>346</v>
-      </c>
       <c r="J4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4963,30 +4963,30 @@
         <v>10</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
       </c>
       <c r="H5" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>349</v>
-      </c>
       <c r="J5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4995,22 +4995,22 @@
         <v>10</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G6" t="s">
         <v>134</v>
       </c>
       <c r="H6" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>352</v>
-      </c>
       <c r="J6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5052,30 +5052,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5087,10 +5087,10 @@
         <v>134</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="G2" t="s">
         <v>396</v>
-      </c>
-      <c r="G2" t="s">
-        <v>397</v>
       </c>
       <c r="H2" t="s">
         <v>107</v>
@@ -5098,10 +5098,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5110,24 +5110,24 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="G3" t="s">
+        <v>398</v>
+      </c>
+      <c r="H3" t="s">
         <v>178</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="G3" t="s">
-        <v>399</v>
-      </c>
-      <c r="H3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5136,13 +5136,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H4" t="s">
         <v>77</v>
@@ -5150,10 +5150,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5162,13 +5162,13 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H5" t="s">
         <v>107</v>
@@ -5176,10 +5176,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5188,16 +5188,16 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5254,39 +5254,39 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L1" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5295,25 +5295,25 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>404</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>405</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>10</v>
@@ -5324,10 +5324,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5339,22 +5339,22 @@
         <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I3" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>404</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>405</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>10</v>
@@ -5365,10 +5365,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5377,25 +5377,25 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I4" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>404</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>405</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -5406,10 +5406,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5418,25 +5418,25 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I5" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>404</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>405</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>10</v>
@@ -5447,10 +5447,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5462,25 +5462,25 @@
         <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I6" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>405</v>
-      </c>
       <c r="L6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>10</v>
@@ -5528,21 +5528,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5551,15 +5551,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5568,15 +5568,15 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5585,15 +5585,15 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5602,15 +5602,15 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5619,7 +5619,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -5657,22 +5657,22 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>407</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>408</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>409</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>410</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>42</v>
@@ -5681,30 +5681,30 @@
         <v>3</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" t="s">
         <v>412</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>414</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>415</v>
       </c>
-      <c r="F2" t="s">
-        <v>416</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>10</v>
@@ -5715,25 +5715,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B3" t="s">
+        <v>412</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B3" t="s">
-        <v>413</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>418</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>419</v>
       </c>
-      <c r="F3" t="s">
-        <v>420</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
@@ -5744,25 +5744,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B4" t="s">
-        <v>413</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>422</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>423</v>
       </c>
-      <c r="F4" t="s">
-        <v>424</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -5773,25 +5773,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B5" t="s">
+        <v>412</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B5" t="s">
-        <v>413</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>426</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>427</v>
-      </c>
       <c r="F5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>10</v>
@@ -5802,25 +5802,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>427</v>
+      </c>
+      <c r="B6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B6" t="s">
-        <v>413</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>429</v>
-      </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Latest validations are added by Asma
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16479\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8510A5B-8E64-410D-B0D4-D459C8134B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD12697B-E435-4DF8-9343-60213C3B1D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" tabRatio="877" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -1417,21 +1417,6 @@
     <t>Order number: 1550202</t>
   </si>
   <si>
-    <t>Charlie_QA1</t>
-  </si>
-  <si>
-    <t>Peter_QA1</t>
-  </si>
-  <si>
-    <t>Aaron_QA1</t>
-  </si>
-  <si>
-    <t>Daniel_QA1</t>
-  </si>
-  <si>
-    <t>Carla_QA1</t>
-  </si>
-  <si>
     <t>Employee Management</t>
   </si>
   <si>
@@ -1439,6 +1424,21 @@
   </si>
   <si>
     <t>Personal</t>
+  </si>
+  <si>
+    <t>Charlie_QA3</t>
+  </si>
+  <si>
+    <t>Peter_QA3</t>
+  </si>
+  <si>
+    <t>Aaron_QA3</t>
+  </si>
+  <si>
+    <t>Daniel_QA3</t>
+  </si>
+  <si>
+    <t>Carla_QA3</t>
   </si>
 </sst>
 </file>
@@ -1902,15 +1902,15 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1943,7 +1943,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>186</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>187</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>188</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>189</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>190</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -2026,7 +2026,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>193</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>194</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>195</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>196</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>197</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -2109,7 +2109,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>203</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>204</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>205</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>206</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>207</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2192,7 +2192,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
         <v>210</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
         <v>211</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
         <v>212</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="s">
         <v>213</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="s">
         <v>214</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2278,7 +2278,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
         <v>222</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
         <v>223</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
         <v>224</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="s">
         <v>225</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
         <v>226</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -2364,7 +2364,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
         <v>229</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="s">
         <v>230</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="s">
         <v>231</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="s">
         <v>232</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="s">
         <v>233</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -2444,7 +2444,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="s">
         <v>241</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
         <v>242</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3" t="s">
         <v>243</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3" t="s">
         <v>244</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="s">
         <v>245</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -2524,7 +2524,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
         <v>252</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="s">
         <v>253</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3" t="s">
         <v>254</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="s">
         <v>255</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3" t="s">
         <v>256</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2604,7 +2604,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3" t="s">
         <v>264</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3" t="s">
         <v>265</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3" t="s">
         <v>266</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3" t="s">
         <v>267</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3" t="s">
         <v>268</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -2684,7 +2684,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3" t="s">
         <v>276</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3" t="s">
         <v>277</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
         <v>278</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3" t="s">
         <v>279</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3" t="s">
         <v>280</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -2764,7 +2764,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3" t="s">
         <v>283</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3" t="s">
         <v>290</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3" t="s">
         <v>291</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3" t="s">
         <v>292</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
         <v>293</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -2844,7 +2844,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3" t="s">
         <v>301</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3" t="s">
         <v>302</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="3" t="s">
         <v>303</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="3" t="s">
         <v>304</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
         <v>305</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -2924,7 +2924,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3" t="s">
         <v>308</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3" t="s">
         <v>309</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3" t="s">
         <v>310</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="3" t="s">
         <v>311</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="3" t="s">
         <v>312</v>
       </c>
@@ -3008,27 +3008,27 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.89453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.89453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.3125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1015625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1015625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.3125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.1015625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1015625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>270</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>271</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>272</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>273</v>
       </c>
@@ -3356,15 +3356,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3474,24 +3474,24 @@
       <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1"/>
-    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.89453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.89453125" customWidth="1"/>
+    <col min="8" max="8" width="28.89453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1015625" customWidth="1"/>
+    <col min="10" max="10" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5234375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.89453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>284</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>285</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>286</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>287</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>288</v>
       </c>
@@ -3761,23 +3761,23 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.41796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.1015625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.89453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1015625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5234375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>294</v>
       </c>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>295</v>
       </c>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>296</v>
       </c>
@@ -3923,7 +3923,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>297</v>
       </c>
@@ -3959,7 +3959,7 @@
       </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>298</v>
       </c>
@@ -4021,22 +4021,22 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.89453125" customWidth="1"/>
+    <col min="5" max="5" width="15.89453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="59.68359375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1015625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.41796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>389</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>313</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>314</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>315</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>316</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>317</v>
       </c>
@@ -4276,15 +4276,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4384,25 +4384,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.89453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1015625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4466,7 +4466,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -4498,7 +4498,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4530,7 +4530,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -4562,7 +4562,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4619,23 +4619,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.89453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1015625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1015625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -4678,16 +4678,16 @@
         <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="G2" t="s">
         <v>134</v>
       </c>
       <c r="H2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -4707,13 +4707,13 @@
         <v>133</v>
       </c>
       <c r="G3" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="H3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -4812,16 +4812,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1015625" customWidth="1"/>
+    <col min="2" max="2" width="27.89453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>215</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>216</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>217</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>218</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>219</v>
       </c>
@@ -5033,18 +5033,18 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>173</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -5220,24 +5220,24 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.89453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.3125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1015625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.3125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1015625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.41796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.3125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>234</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>235</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>236</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>237</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>238</v>
       </c>
@@ -5511,16 +5511,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>247</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>248</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>249</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>250</v>
       </c>
@@ -5643,19 +5643,19 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1015625" customWidth="1"/>
+    <col min="7" max="7" width="25.5234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>405</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>411</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>416</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>420</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>424</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>427</v>
       </c>

</xml_diff>

<commit_message>
Latest changed done by Sathish
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16479\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD12697B-E435-4DF8-9343-60213C3B1D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE15271B-D04F-4B1E-9480-06DE293AC738}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" tabRatio="877" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="20925" windowHeight="12435" tabRatio="877" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="466">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -448,9 +448,6 @@
     <t>Travel and Expense Detailed Report</t>
   </si>
   <si>
-    <t>test one</t>
-  </si>
-  <si>
     <t>Travel Requests</t>
   </si>
   <si>
@@ -460,21 +457,9 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Claims</t>
-  </si>
-  <si>
-    <t>Selenium</t>
-  </si>
-  <si>
     <t>Estimated Expenses</t>
   </si>
   <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>Claimed Expenses</t>
-  </si>
-  <si>
     <t>Computing and Internet</t>
   </si>
   <si>
@@ -1439,6 +1424,18 @@
   </si>
   <si>
     <t>Carla_QA3</t>
+  </si>
+  <si>
+    <t>Automation77</t>
+  </si>
+  <si>
+    <t>Testing77</t>
+  </si>
+  <si>
+    <t>Selenium77</t>
+  </si>
+  <si>
+    <t>Java77</t>
   </si>
 </sst>
 </file>
@@ -1554,7 +1551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1581,6 +1578,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1902,17 +1900,17 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.1015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>
@@ -1921,680 +1919,680 @@
         <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D10" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D13" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E13" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D16" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D17" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D19" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" t="s">
         <v>210</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>317</v>
+      </c>
+      <c r="D21" t="s">
         <v>215</v>
       </c>
-      <c r="C21" t="s">
-        <v>322</v>
-      </c>
-      <c r="D21" t="s">
-        <v>220</v>
-      </c>
       <c r="E21" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" t="s">
         <v>211</v>
       </c>
-      <c r="B22" t="s">
-        <v>216</v>
-      </c>
       <c r="C22" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D22" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E22" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" t="s">
         <v>212</v>
       </c>
-      <c r="B23" t="s">
-        <v>217</v>
-      </c>
       <c r="C23" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D23" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B24" t="s">
         <v>213</v>
       </c>
-      <c r="B24" t="s">
-        <v>218</v>
-      </c>
       <c r="C24" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D24" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B25" t="s">
         <v>214</v>
       </c>
-      <c r="B25" t="s">
-        <v>219</v>
-      </c>
       <c r="C25" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" t="s">
+        <v>318</v>
+      </c>
+      <c r="D27" t="s">
         <v>222</v>
       </c>
-      <c r="B27" t="s">
-        <v>165</v>
-      </c>
-      <c r="C27" t="s">
-        <v>323</v>
-      </c>
-      <c r="D27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" t="s">
+        <v>318</v>
+      </c>
+      <c r="D28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B29" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" t="s">
+        <v>318</v>
+      </c>
+      <c r="D29" t="s">
+        <v>222</v>
+      </c>
+      <c r="E29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" t="s">
+        <v>318</v>
+      </c>
+      <c r="D30" t="s">
+        <v>222</v>
+      </c>
+      <c r="E30" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31" t="s">
         <v>169</v>
       </c>
-      <c r="C28" t="s">
-        <v>323</v>
-      </c>
-      <c r="D28" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C29" t="s">
-        <v>323</v>
-      </c>
-      <c r="D29" t="s">
-        <v>227</v>
-      </c>
-      <c r="E29" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B30" t="s">
-        <v>173</v>
-      </c>
-      <c r="C30" t="s">
-        <v>323</v>
-      </c>
-      <c r="D30" t="s">
-        <v>227</v>
-      </c>
-      <c r="E30" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B31" t="s">
-        <v>174</v>
-      </c>
       <c r="C31" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D31" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B33" t="s">
         <v>229</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>319</v>
+      </c>
+      <c r="D33" t="s">
         <v>234</v>
       </c>
-      <c r="C33" t="s">
-        <v>324</v>
-      </c>
-      <c r="D33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B34" t="s">
         <v>230</v>
       </c>
-      <c r="B34" t="s">
-        <v>235</v>
-      </c>
       <c r="C34" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B35" t="s">
         <v>231</v>
       </c>
-      <c r="B35" t="s">
-        <v>236</v>
-      </c>
       <c r="C35" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D35" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" t="s">
         <v>232</v>
       </c>
-      <c r="B36" t="s">
-        <v>237</v>
-      </c>
       <c r="C36" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D36" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B37" t="s">
         <v>233</v>
       </c>
-      <c r="B37" t="s">
-        <v>238</v>
-      </c>
       <c r="C37" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D37" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B39" t="s">
         <v>241</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>320</v>
+      </c>
+      <c r="D39" t="s">
         <v>246</v>
       </c>
-      <c r="C39" t="s">
-        <v>325</v>
-      </c>
-      <c r="D39" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B40" t="s">
         <v>242</v>
       </c>
-      <c r="B40" t="s">
-        <v>247</v>
-      </c>
       <c r="C40" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D40" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B41" t="s">
         <v>243</v>
       </c>
-      <c r="B41" t="s">
-        <v>248</v>
-      </c>
       <c r="C41" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D41" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B42" t="s">
         <v>244</v>
       </c>
-      <c r="B42" t="s">
-        <v>249</v>
-      </c>
       <c r="C42" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D42" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B43" t="s">
         <v>245</v>
       </c>
-      <c r="B43" t="s">
-        <v>250</v>
-      </c>
       <c r="C43" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D43" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B45" t="s">
         <v>252</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
+        <v>326</v>
+      </c>
+      <c r="D45" t="s">
         <v>257</v>
       </c>
-      <c r="C45" t="s">
-        <v>331</v>
-      </c>
-      <c r="D45" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B46" t="s">
         <v>253</v>
       </c>
-      <c r="B46" t="s">
-        <v>258</v>
-      </c>
       <c r="C46" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D46" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B47" t="s">
         <v>254</v>
       </c>
-      <c r="B47" t="s">
-        <v>259</v>
-      </c>
       <c r="C47" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D47" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B48" t="s">
         <v>255</v>
       </c>
-      <c r="B48" t="s">
-        <v>260</v>
-      </c>
       <c r="C48" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D48" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B49" t="s">
         <v>256</v>
       </c>
-      <c r="B49" t="s">
-        <v>261</v>
-      </c>
       <c r="C49" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D49" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2604,394 +2602,394 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B51" t="s">
         <v>264</v>
-      </c>
-      <c r="B51" t="s">
-        <v>269</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B52" t="s">
         <v>265</v>
-      </c>
-      <c r="B52" t="s">
-        <v>270</v>
       </c>
       <c r="C52" t="s">
         <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B53" t="s">
         <v>266</v>
-      </c>
-      <c r="B53" t="s">
-        <v>271</v>
       </c>
       <c r="C53" t="s">
         <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B54" t="s">
         <v>267</v>
-      </c>
-      <c r="B54" t="s">
-        <v>272</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B55" t="s">
         <v>268</v>
-      </c>
-      <c r="B55" t="s">
-        <v>273</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B57" t="s">
         <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D57" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B58" t="s">
         <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D58" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B59" t="s">
         <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D59" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B60" t="s">
         <v>37</v>
       </c>
       <c r="C60" t="s">
+        <v>270</v>
+      </c>
+      <c r="D60" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="D60" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="B61" t="s">
         <v>38</v>
       </c>
       <c r="C61" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D61" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B63" t="s">
+        <v>279</v>
+      </c>
+      <c r="C63" t="s">
+        <v>277</v>
+      </c>
+      <c r="D63" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B64" t="s">
+        <v>280</v>
+      </c>
+      <c r="C64" t="s">
+        <v>277</v>
+      </c>
+      <c r="D64" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B65" t="s">
+        <v>281</v>
+      </c>
+      <c r="C65" t="s">
+        <v>277</v>
+      </c>
+      <c r="D65" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B66" t="s">
+        <v>282</v>
+      </c>
+      <c r="C66" t="s">
+        <v>277</v>
+      </c>
+      <c r="D66" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B67" t="s">
         <v>283</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C67" t="s">
+        <v>277</v>
+      </c>
+      <c r="D67" t="s">
         <v>284</v>
       </c>
-      <c r="C63" t="s">
-        <v>282</v>
-      </c>
-      <c r="D63" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B64" t="s">
-        <v>285</v>
-      </c>
-      <c r="C64" t="s">
-        <v>282</v>
-      </c>
-      <c r="D64" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B65" t="s">
-        <v>286</v>
-      </c>
-      <c r="C65" t="s">
-        <v>282</v>
-      </c>
-      <c r="D65" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B66" t="s">
-        <v>287</v>
-      </c>
-      <c r="C66" t="s">
-        <v>282</v>
-      </c>
-      <c r="D66" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="B67" t="s">
-        <v>288</v>
-      </c>
-      <c r="C67" t="s">
-        <v>282</v>
-      </c>
-      <c r="D67" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B69" t="s">
+        <v>289</v>
+      </c>
+      <c r="C69" t="s">
+        <v>295</v>
+      </c>
+      <c r="D69" t="s">
         <v>301</v>
       </c>
-      <c r="B69" t="s">
-        <v>294</v>
-      </c>
-      <c r="C69" t="s">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B70" t="s">
+        <v>290</v>
+      </c>
+      <c r="C70" t="s">
+        <v>295</v>
+      </c>
+      <c r="D70" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B71" t="s">
+        <v>291</v>
+      </c>
+      <c r="C71" t="s">
+        <v>295</v>
+      </c>
+      <c r="D71" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B72" t="s">
+        <v>292</v>
+      </c>
+      <c r="C72" t="s">
+        <v>295</v>
+      </c>
+      <c r="D72" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D69" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
+        <v>293</v>
+      </c>
+      <c r="C73" t="s">
         <v>295</v>
       </c>
-      <c r="C70" t="s">
-        <v>300</v>
-      </c>
-      <c r="D70" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B71" t="s">
-        <v>296</v>
-      </c>
-      <c r="C71" t="s">
-        <v>300</v>
-      </c>
-      <c r="D71" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B72" t="s">
-        <v>297</v>
-      </c>
-      <c r="C72" t="s">
-        <v>300</v>
-      </c>
-      <c r="D72" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B73" t="s">
-        <v>298</v>
-      </c>
-      <c r="C73" t="s">
-        <v>300</v>
-      </c>
       <c r="D73" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B75" t="s">
         <v>308</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
+        <v>367</v>
+      </c>
+      <c r="D75" t="s">
         <v>313</v>
       </c>
-      <c r="C75" t="s">
-        <v>372</v>
-      </c>
-      <c r="D75" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B76" t="s">
         <v>309</v>
       </c>
-      <c r="B76" t="s">
-        <v>314</v>
-      </c>
       <c r="C76" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D76" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B77" t="s">
         <v>310</v>
       </c>
-      <c r="B77" t="s">
-        <v>315</v>
-      </c>
       <c r="C77" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D77" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B78" t="s">
         <v>311</v>
       </c>
-      <c r="B78" t="s">
-        <v>316</v>
-      </c>
       <c r="C78" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B79" t="s">
         <v>312</v>
       </c>
-      <c r="B79" t="s">
-        <v>317</v>
-      </c>
       <c r="C79" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D79" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3008,27 +3006,27 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.3125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1015625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1015625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.1015625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1015625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3078,9 +3076,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -3128,9 +3126,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -3178,9 +3176,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
@@ -3228,9 +3226,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -3278,9 +3276,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -3356,15 +3354,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3372,18 +3370,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -3392,12 +3390,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -3406,12 +3404,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -3420,12 +3418,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -3434,12 +3432,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -3474,24 +3472,24 @@
       <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.89453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.89453125" customWidth="1"/>
-    <col min="8" max="8" width="28.89453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.1015625" customWidth="1"/>
-    <col min="10" max="10" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5234375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.89453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.3125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3499,45 +3497,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>440</v>
-      </c>
       <c r="M1" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -3546,39 +3544,39 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G2" t="s">
+        <v>429</v>
+      </c>
+      <c r="H2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I2" t="s">
+        <v>432</v>
+      </c>
+      <c r="J2" t="s">
         <v>434</v>
       </c>
-      <c r="H2" t="s">
-        <v>157</v>
-      </c>
-      <c r="I2" t="s">
-        <v>437</v>
-      </c>
-      <c r="J2" t="s">
-        <v>439</v>
-      </c>
       <c r="K2" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="L2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="M2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -3587,39 +3585,39 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="F3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="H3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="I3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="J3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="K3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="L3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="M3" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -3628,39 +3626,39 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G4" t="s">
+        <v>432</v>
+      </c>
+      <c r="H4" t="s">
         <v>437</v>
       </c>
-      <c r="H4" t="s">
-        <v>442</v>
-      </c>
       <c r="I4" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="J4" t="s">
+        <v>438</v>
+      </c>
+      <c r="K4" t="s">
         <v>443</v>
       </c>
-      <c r="K4" t="s">
-        <v>448</v>
-      </c>
       <c r="L4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="M4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -3669,39 +3667,39 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G5" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="I5" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="J5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="L5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="M5" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -3710,31 +3708,31 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F6" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G6" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H6" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I6" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="J6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K6" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="L6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="M6" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -3761,23 +3759,23 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5234375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.89453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1015625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5234375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3791,36 +3789,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>299</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>33</v>
@@ -3829,34 +3827,34 @@
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>33</v>
@@ -3865,34 +3863,34 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="K3" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>162</v>
-      </c>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -3901,34 +3899,34 @@
         <v>10</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>33</v>
@@ -3937,34 +3935,34 @@
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>33</v>
@@ -3973,25 +3971,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F6" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L6" s="14"/>
     </row>
@@ -4021,65 +4019,65 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.89453125" customWidth="1"/>
-    <col min="5" max="5" width="15.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.68359375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1015625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B2" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -4088,33 +4086,33 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="J2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="K2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -4123,33 +4121,33 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="J3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="K3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -4158,33 +4156,33 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F4" t="s">
+        <v>362</v>
+      </c>
+      <c r="G4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H4" t="s">
+        <v>356</v>
+      </c>
+      <c r="I4" t="s">
+        <v>357</v>
+      </c>
+      <c r="J4" t="s">
+        <v>358</v>
+      </c>
+      <c r="K4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" t="s">
         <v>367</v>
-      </c>
-      <c r="G4" t="s">
-        <v>361</v>
-      </c>
-      <c r="H4" t="s">
-        <v>361</v>
-      </c>
-      <c r="I4" t="s">
-        <v>362</v>
-      </c>
-      <c r="J4" t="s">
-        <v>363</v>
-      </c>
-      <c r="K4" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>316</v>
-      </c>
-      <c r="B5" t="s">
-        <v>372</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -4193,33 +4191,33 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="G5" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H5" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I5" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="J5" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="K5" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B6" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -4228,25 +4226,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="G6" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H6" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I6" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="J6" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="K6" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -4276,15 +4274,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4298,12 +4296,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4312,12 +4310,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -4326,12 +4324,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -4340,12 +4338,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -4354,12 +4352,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4384,25 +4382,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.41796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4419,7 +4417,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -4428,18 +4426,18 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4451,7 +4449,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4466,12 +4464,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4483,7 +4481,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -4498,12 +4496,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4515,7 +4513,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4530,12 +4528,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4547,7 +4545,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -4562,12 +4560,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4579,7 +4577,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4619,186 +4617,186 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F2" t="s">
-        <v>459</v>
-      </c>
-      <c r="G2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="F2" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="G3" t="s">
-        <v>460</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="G3" s="14" t="s">
+        <v>455</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>321</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F4" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="G4" t="s">
-        <v>139</v>
-      </c>
-      <c r="H4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>321</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="G5" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="G5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>321</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G6" t="s">
-        <v>143</v>
-      </c>
-      <c r="H6" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{0FC73D77-BC6F-406C-93CE-143A84805A96}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{3FDDCF7C-7FD3-4E55-B21F-458640CB5CFD}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{C29F7A54-A4A2-4479-AED4-A50FF0AD0752}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{E68465D0-2582-42B1-91C9-8E1F81D98AE9}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{EDB4F9FC-5F65-4712-A234-7AFBBE81FA2D}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{165E166A-99CE-4ED9-B0B8-74EC9E8D61C4}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{E15F64F4-2545-4142-9338-629A10A0E6AF}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{801F95FD-483F-4DB1-8918-82C863B7F10C}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{21C73AC4-B425-46C7-832B-405B534CDE92}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{9D172760-9A04-4069-BFB0-9A7CD3BB6D1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4812,16 +4810,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1015625" customWidth="1"/>
-    <col min="2" max="2" width="27.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4835,30 +4833,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4867,30 +4865,30 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G2" t="s">
         <v>134</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="J2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4899,30 +4897,30 @@
         <v>10</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G3" t="s">
         <v>134</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="J3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4931,30 +4929,30 @@
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G4" t="s">
         <v>134</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="J4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4963,30 +4961,30 @@
         <v>10</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="J5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B6" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4995,22 +4993,22 @@
         <v>10</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="G6" t="s">
         <v>134</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="J6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -5033,18 +5031,18 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.89453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5052,30 +5050,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5087,21 +5085,21 @@
         <v>134</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="G2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5110,24 +5108,24 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="H3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5136,24 +5134,24 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G4" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5162,24 +5160,24 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="G5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="H5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5188,16 +5186,16 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G6" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -5220,24 +5218,24 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1015625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.3125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.1015625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1015625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.41796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.3125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5254,39 +5252,39 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>385</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5295,25 +5293,25 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F2" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G2" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="H2" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>10</v>
@@ -5322,12 +5320,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5339,22 +5337,22 @@
         <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>10</v>
@@ -5363,12 +5361,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5377,25 +5375,25 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F4" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G4" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H4" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -5404,12 +5402,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5418,25 +5416,25 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="F5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>10</v>
@@ -5445,12 +5443,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B6" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5462,25 +5460,25 @@
         <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G6" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="L6" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>10</v>
@@ -5511,16 +5509,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5528,21 +5526,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5551,15 +5549,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5568,15 +5566,15 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5585,15 +5583,15 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5602,15 +5600,15 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B6" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5619,7 +5617,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5643,36 +5641,36 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.1015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1015625" customWidth="1"/>
-    <col min="7" max="7" width="25.5234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>42</v>
@@ -5681,146 +5679,146 @@
         <v>3</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>409</v>
+      </c>
+      <c r="F2" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>411</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>413</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>414</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>415</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B3" t="s">
-        <v>412</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>417</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>418</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G4" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>419</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="B5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>421</v>
+      </c>
+      <c r="F5" t="s">
         <v>417</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="G5" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>422</v>
+      </c>
+      <c r="B6" t="s">
+        <v>407</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>418</v>
+      </c>
+      <c r="F6" t="s">
         <v>421</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>422</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G6" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>424</v>
-      </c>
-      <c r="B5" t="s">
-        <v>412</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>426</v>
-      </c>
-      <c r="F5" t="s">
-        <v>422</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>427</v>
-      </c>
-      <c r="B6" t="s">
-        <v>412</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>423</v>
-      </c>
-      <c r="F6" t="s">
-        <v>426</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>428</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Code Refactoring of HRM testcases is completed
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE15271B-D04F-4B1E-9480-06DE293AC738}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA89DB6A-EC47-4184-9E8A-DF9C55256E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="20925" windowHeight="12435" tabRatio="877" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="467">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1436,6 +1436,9 @@
   </si>
   <si>
     <t>Java77</t>
+  </si>
+  <si>
+    <t>CountryName</t>
   </si>
 </sst>
 </file>
@@ -1900,15 +1903,15 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>177</v>
       </c>
@@ -1931,7 +1934,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1941,7 +1944,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>181</v>
       </c>
@@ -1955,7 +1958,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>182</v>
       </c>
@@ -1969,7 +1972,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>183</v>
       </c>
@@ -1986,7 +1989,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>184</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>185</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -2024,7 +2027,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>188</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>189</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>190</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>191</v>
       </c>
@@ -2080,7 +2083,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>192</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -2107,7 +2110,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>198</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>199</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>200</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>201</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>202</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2190,7 +2193,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>205</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>206</v>
       </c>
@@ -2224,7 +2227,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>207</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>208</v>
       </c>
@@ -2252,7 +2255,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>209</v>
       </c>
@@ -2266,7 +2269,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2276,7 +2279,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>217</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>218</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>219</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>220</v>
       </c>
@@ -2338,7 +2341,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -2362,7 +2365,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>224</v>
       </c>
@@ -2376,7 +2379,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>225</v>
       </c>
@@ -2390,7 +2393,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>226</v>
       </c>
@@ -2404,7 +2407,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>227</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>228</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -2442,7 +2445,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>236</v>
       </c>
@@ -2456,7 +2459,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>237</v>
       </c>
@@ -2470,7 +2473,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>238</v>
       </c>
@@ -2484,7 +2487,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>239</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>240</v>
       </c>
@@ -2512,7 +2515,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -2522,7 +2525,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>247</v>
       </c>
@@ -2536,7 +2539,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>248</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>249</v>
       </c>
@@ -2564,7 +2567,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>250</v>
       </c>
@@ -2578,7 +2581,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>251</v>
       </c>
@@ -2592,7 +2595,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2602,7 +2605,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>259</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>260</v>
       </c>
@@ -2630,7 +2633,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>261</v>
       </c>
@@ -2644,7 +2647,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>262</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>263</v>
       </c>
@@ -2672,7 +2675,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -2682,7 +2685,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>271</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>272</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>273</v>
       </c>
@@ -2724,7 +2727,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>274</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>275</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -2762,7 +2765,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>278</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>285</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>286</v>
       </c>
@@ -2804,7 +2807,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>287</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>288</v>
       </c>
@@ -2832,7 +2835,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -2842,7 +2845,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>296</v>
       </c>
@@ -2856,7 +2859,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>297</v>
       </c>
@@ -2870,7 +2873,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>298</v>
       </c>
@@ -2884,7 +2887,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>299</v>
       </c>
@@ -2898,7 +2901,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>300</v>
       </c>
@@ -2912,7 +2915,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -2922,7 +2925,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>303</v>
       </c>
@@ -2936,7 +2939,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>304</v>
       </c>
@@ -2950,7 +2953,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>305</v>
       </c>
@@ -2964,7 +2967,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>306</v>
       </c>
@@ -2978,7 +2981,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>307</v>
       </c>
@@ -3006,27 +3009,27 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3076,7 +3079,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>264</v>
       </c>
@@ -3126,7 +3129,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>265</v>
       </c>
@@ -3176,7 +3179,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>266</v>
       </c>
@@ -3226,7 +3229,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -3276,7 +3279,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -3354,15 +3357,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3376,7 +3379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3390,7 +3393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3404,7 +3407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3418,7 +3421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3432,7 +3435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3472,24 +3475,24 @@
       <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3530,7 +3533,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -3571,7 +3574,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>280</v>
       </c>
@@ -3612,7 +3615,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>281</v>
       </c>
@@ -3653,7 +3656,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>282</v>
       </c>
@@ -3694,7 +3697,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>283</v>
       </c>
@@ -3759,23 +3762,23 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3813,7 +3816,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>289</v>
       </c>
@@ -3849,7 +3852,7 @@
       </c>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>290</v>
       </c>
@@ -3885,7 +3888,7 @@
       </c>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>291</v>
       </c>
@@ -3921,7 +3924,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>292</v>
       </c>
@@ -3957,7 +3960,7 @@
       </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>293</v>
       </c>
@@ -4019,22 +4022,22 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>384</v>
       </c>
@@ -4072,7 +4075,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>308</v>
       </c>
@@ -4107,7 +4110,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>309</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>310</v>
       </c>
@@ -4177,7 +4180,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>311</v>
       </c>
@@ -4212,7 +4215,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -4274,15 +4277,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4296,7 +4299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4310,7 +4313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4324,7 +4327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4338,7 +4341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4352,7 +4355,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4386,21 +4389,21 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4432,7 +4435,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4464,7 +4467,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4496,7 +4499,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -4528,7 +4531,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4560,7 +4563,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4617,23 +4620,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -4659,7 +4662,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>45</v>
       </c>
@@ -4711,7 +4714,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
@@ -4737,7 +4740,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
@@ -4763,7 +4766,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
@@ -4810,16 +4813,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4851,7 +4854,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -4883,7 +4886,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -4915,7 +4918,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -4947,7 +4950,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -4979,7 +4982,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -5031,18 +5034,18 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5068,7 +5071,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>160</v>
       </c>
@@ -5094,7 +5097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -5120,7 +5123,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -5146,7 +5149,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>168</v>
       </c>
@@ -5172,7 +5175,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>169</v>
       </c>
@@ -5218,24 +5221,24 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5279,7 +5282,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>229</v>
       </c>
@@ -5320,7 +5323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -5361,7 +5364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -5402,7 +5405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -5443,7 +5446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -5505,20 +5508,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5532,10 +5535,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -5552,7 +5555,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -5569,7 +5572,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -5586,7 +5589,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -5603,7 +5606,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>245</v>
       </c>
@@ -5641,19 +5644,19 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>400</v>
       </c>
@@ -5682,7 +5685,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>406</v>
       </c>
@@ -5711,7 +5714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>411</v>
       </c>
@@ -5740,7 +5743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>415</v>
       </c>
@@ -5769,7 +5772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>419</v>
       </c>
@@ -5798,7 +5801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>422</v>
       </c>

</xml_diff>

<commit_message>
Latest changed done by Sathish in TC03 & TC12
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA89DB6A-EC47-4184-9E8A-DF9C55256E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD243E9-F5B7-4894-9987-116C338BD46B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -1405,9 +1405,6 @@
     <t>Employee Management</t>
   </si>
   <si>
-    <t>Catalogues77</t>
-  </si>
-  <si>
     <t>Personal</t>
   </si>
   <si>
@@ -1426,19 +1423,22 @@
     <t>Carla_QA3</t>
   </si>
   <si>
-    <t>Automation77</t>
-  </si>
-  <si>
-    <t>Testing77</t>
-  </si>
-  <si>
-    <t>Selenium77</t>
-  </si>
-  <si>
-    <t>Java77</t>
-  </si>
-  <si>
     <t>CountryName</t>
+  </si>
+  <si>
+    <t>Automation44</t>
+  </si>
+  <si>
+    <t>Catalogue44</t>
+  </si>
+  <si>
+    <t>Testing44</t>
+  </si>
+  <si>
+    <t>Selenium44</t>
+  </si>
+  <si>
+    <t>Java44</t>
   </si>
 </sst>
 </file>
@@ -1903,15 +1903,15 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>177</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1944,7 +1944,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>181</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>182</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>183</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>184</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>185</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -2027,7 +2027,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>188</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>189</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>190</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>191</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>192</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -2110,7 +2110,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>198</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>199</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>200</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>201</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>202</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2193,7 +2193,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>205</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>206</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>207</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>208</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>209</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2279,7 +2279,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>217</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>218</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>219</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>220</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -2365,7 +2365,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>224</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>225</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>226</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>227</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>228</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -2445,7 +2445,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>236</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>237</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>238</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>239</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>240</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -2525,7 +2525,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>247</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>248</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>249</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>250</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>251</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2605,7 +2605,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>259</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>260</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>261</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>262</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>263</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -2685,7 +2685,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>271</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>272</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>273</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>274</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>275</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -2765,7 +2765,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>278</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>285</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>286</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>287</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>288</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -2845,7 +2845,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>296</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>297</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>298</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>299</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>300</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -2925,7 +2925,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>303</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>304</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>305</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>306</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>307</v>
       </c>
@@ -3009,27 +3009,27 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>264</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>265</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>266</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -3357,15 +3357,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3475,24 +3475,24 @@
       <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1"/>
-    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>280</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>281</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>282</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>283</v>
       </c>
@@ -3762,23 +3762,23 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>289</v>
       </c>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>290</v>
       </c>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>291</v>
       </c>
@@ -3924,7 +3924,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>292</v>
       </c>
@@ -3960,7 +3960,7 @@
       </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>293</v>
       </c>
@@ -4022,22 +4022,22 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>384</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>308</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>309</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>310</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>311</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -4277,15 +4277,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4389,21 +4389,21 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4467,7 +4467,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -4499,7 +4499,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4531,7 +4531,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -4563,7 +4563,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4620,23 +4620,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
@@ -4685,10 +4685,10 @@
         <v>462</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>45</v>
       </c>
@@ -4708,13 +4708,13 @@
         <v>133</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
@@ -4734,13 +4734,13 @@
         <v>133</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
@@ -4760,13 +4760,13 @@
         <v>133</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>133</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>136</v>
@@ -4813,16 +4813,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -5034,18 +5034,18 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>160</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>168</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>169</v>
       </c>
@@ -5221,24 +5221,24 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>229</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -5508,20 +5508,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5535,10 +5535,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>245</v>
       </c>
@@ -5644,19 +5644,19 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>400</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>406</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>411</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>415</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>419</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>422</v>
       </c>

</xml_diff>

<commit_message>
Latest changed done by Satish in TC03 & TC12
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD243E9-F5B7-4894-9987-116C338BD46B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B24F14-871C-490E-B934-B4152DB494CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1432,13 +1432,13 @@
     <t>Catalogue44</t>
   </si>
   <si>
-    <t>Testing44</t>
-  </si>
-  <si>
     <t>Selenium44</t>
   </si>
   <si>
     <t>Java44</t>
+  </si>
+  <si>
+    <t>Testing49</t>
   </si>
 </sst>
 </file>
@@ -4621,7 +4621,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4734,7 +4734,7 @@
         <v>133</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>139</v>
@@ -4760,7 +4760,7 @@
         <v>133</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>455</v>
@@ -4786,7 +4786,7 @@
         <v>133</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
OrangeHRM Report Analytics locator changes completed
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B24F14-871C-490E-B934-B4152DB494CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB1C142-412B-465C-837F-6CFFE0826151}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1426,19 +1426,19 @@
     <t>CountryName</t>
   </si>
   <si>
-    <t>Automation44</t>
-  </si>
-  <si>
-    <t>Catalogue44</t>
-  </si>
-  <si>
-    <t>Selenium44</t>
-  </si>
-  <si>
-    <t>Java44</t>
-  </si>
-  <si>
-    <t>Testing49</t>
+    <t>Testing491</t>
+  </si>
+  <si>
+    <t>Catalogue441</t>
+  </si>
+  <si>
+    <t>Automation441</t>
+  </si>
+  <si>
+    <t>Selenium441</t>
+  </si>
+  <si>
+    <t>Java441</t>
   </si>
 </sst>
 </file>
@@ -4621,7 +4621,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4682,7 +4682,7 @@
         <v>454</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>455</v>
@@ -4734,7 +4734,7 @@
         <v>133</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>139</v>
@@ -4760,7 +4760,7 @@
         <v>133</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>455</v>
@@ -4786,7 +4786,7 @@
         <v>133</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
Page locators added for Orange HRM Performance and Demo Webshop Total orders
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\IdeaProjects\AutomationCatalogue_TestingFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arunkumar/IdeaProjects/AutomationCatalogue_TestingFramework/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB1C142-412B-465C-837F-6CFFE0826151}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED4A93D-85DE-C341-876E-4F4DC37E510A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" tabRatio="877" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="473">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1156,9 +1156,6 @@
     <t>TC08_DemoWebshop_TotalOrders</t>
   </si>
   <si>
-    <t>Adella Lopez</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -1168,9 +1165,6 @@
     <t>Appraisal Cycle</t>
   </si>
   <si>
-    <t>End Year Review 2018- HR Executive</t>
-  </si>
-  <si>
     <t>Template</t>
   </si>
   <si>
@@ -1183,12 +1177,6 @@
     <t>To Date</t>
   </si>
   <si>
-    <t>Brody Alan</t>
-  </si>
-  <si>
-    <t>Aaliyah Haq</t>
-  </si>
-  <si>
     <t>Due Date</t>
   </si>
   <si>
@@ -1372,9 +1360,6 @@
     <t>Digital downloads</t>
   </si>
   <si>
-    <t>End Year Review 2018 - HQ-CA USA</t>
-  </si>
-  <si>
     <t>UserName_EmployeeName</t>
   </si>
   <si>
@@ -1439,15 +1424,55 @@
   </si>
   <si>
     <t>Java441</t>
+  </si>
+  <si>
+    <t>2023 - Annual Review for HR Department</t>
+  </si>
+  <si>
+    <t>2023 Annual Appraisal</t>
+  </si>
+  <si>
+    <t>Annual review for year 2023</t>
+  </si>
+  <si>
+    <t>Lisa Wagner</t>
+  </si>
+  <si>
+    <t>wagnerlisa</t>
+  </si>
+  <si>
+    <t>Tom Walker</t>
+  </si>
+  <si>
+    <t>walkertom</t>
+  </si>
+  <si>
+    <t>Shane Warn</t>
+  </si>
+  <si>
+    <t>Shane.Warn</t>
+  </si>
+  <si>
+    <t>Mazie Abraham</t>
+  </si>
+  <si>
+    <t>abrahammaize</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1552,17 +1577,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1571,17 +1596,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1903,15 +1930,15 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>177</v>
       </c>
@@ -1934,7 +1961,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1944,7 +1971,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>181</v>
       </c>
@@ -1958,7 +1985,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>182</v>
       </c>
@@ -1972,7 +1999,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>183</v>
       </c>
@@ -1989,7 +2016,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>184</v>
       </c>
@@ -2003,7 +2030,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>185</v>
       </c>
@@ -2017,7 +2044,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -2027,7 +2054,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>188</v>
       </c>
@@ -2041,7 +2068,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>189</v>
       </c>
@@ -2055,7 +2082,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>190</v>
       </c>
@@ -2069,7 +2096,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>191</v>
       </c>
@@ -2083,7 +2110,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>192</v>
       </c>
@@ -2100,7 +2127,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -2110,7 +2137,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>198</v>
       </c>
@@ -2124,7 +2151,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>199</v>
       </c>
@@ -2138,7 +2165,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>200</v>
       </c>
@@ -2155,7 +2182,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>201</v>
       </c>
@@ -2169,7 +2196,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>202</v>
       </c>
@@ -2183,7 +2210,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2193,7 +2220,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>205</v>
       </c>
@@ -2210,7 +2237,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>206</v>
       </c>
@@ -2227,7 +2254,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>207</v>
       </c>
@@ -2241,7 +2268,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>208</v>
       </c>
@@ -2255,7 +2282,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>209</v>
       </c>
@@ -2269,7 +2296,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2279,7 +2306,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>217</v>
       </c>
@@ -2293,7 +2320,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>218</v>
       </c>
@@ -2307,7 +2334,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>219</v>
       </c>
@@ -2324,7 +2351,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>220</v>
       </c>
@@ -2341,7 +2368,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -2355,7 +2382,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -2365,7 +2392,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>224</v>
       </c>
@@ -2379,7 +2406,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>225</v>
       </c>
@@ -2393,7 +2420,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>226</v>
       </c>
@@ -2407,7 +2434,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>227</v>
       </c>
@@ -2421,7 +2448,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>228</v>
       </c>
@@ -2435,7 +2462,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -2445,7 +2472,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>236</v>
       </c>
@@ -2459,7 +2486,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>237</v>
       </c>
@@ -2473,7 +2500,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>238</v>
       </c>
@@ -2487,7 +2514,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>239</v>
       </c>
@@ -2501,7 +2528,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>240</v>
       </c>
@@ -2515,7 +2542,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -2525,7 +2552,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>247</v>
       </c>
@@ -2539,7 +2566,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>248</v>
       </c>
@@ -2553,7 +2580,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>249</v>
       </c>
@@ -2567,7 +2594,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>250</v>
       </c>
@@ -2581,7 +2608,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>251</v>
       </c>
@@ -2595,7 +2622,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2605,7 +2632,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>259</v>
       </c>
@@ -2619,7 +2646,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>260</v>
       </c>
@@ -2633,7 +2660,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>261</v>
       </c>
@@ -2647,7 +2674,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>262</v>
       </c>
@@ -2661,7 +2688,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>263</v>
       </c>
@@ -2675,7 +2702,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -2685,7 +2712,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>271</v>
       </c>
@@ -2699,7 +2726,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>272</v>
       </c>
@@ -2713,7 +2740,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>273</v>
       </c>
@@ -2727,7 +2754,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>274</v>
       </c>
@@ -2741,7 +2768,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>275</v>
       </c>
@@ -2755,7 +2782,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -2765,7 +2792,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>278</v>
       </c>
@@ -2779,7 +2806,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>285</v>
       </c>
@@ -2793,7 +2820,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>286</v>
       </c>
@@ -2807,7 +2834,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>287</v>
       </c>
@@ -2821,7 +2848,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>288</v>
       </c>
@@ -2835,7 +2862,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -2845,7 +2872,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>296</v>
       </c>
@@ -2859,7 +2886,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>297</v>
       </c>
@@ -2873,7 +2900,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>298</v>
       </c>
@@ -2887,7 +2914,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>299</v>
       </c>
@@ -2901,7 +2928,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>300</v>
       </c>
@@ -2915,7 +2942,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -2925,7 +2952,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>303</v>
       </c>
@@ -2939,7 +2966,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>304</v>
       </c>
@@ -2953,7 +2980,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>305</v>
       </c>
@@ -2967,7 +2994,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>306</v>
       </c>
@@ -2981,7 +3008,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>307</v>
       </c>
@@ -2996,7 +3023,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3009,27 +3036,27 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3079,7 +3106,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>264</v>
       </c>
@@ -3129,7 +3156,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>265</v>
       </c>
@@ -3179,7 +3206,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>266</v>
       </c>
@@ -3229,7 +3256,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -3279,7 +3306,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -3330,7 +3357,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{0CFF6622-BAB0-4347-BF40-8454C1587B08}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{525EFD10-CCA5-4147-9725-D6BEDEE56E77}"/>
@@ -3357,15 +3384,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3379,7 +3406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3393,7 +3420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3407,7 +3434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3421,7 +3448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3435,7 +3462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3450,7 +3477,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
@@ -3475,24 +3502,24 @@
       <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3506,34 +3533,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>435</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -3553,28 +3580,28 @@
         <v>140</v>
       </c>
       <c r="G2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="H2" t="s">
         <v>152</v>
       </c>
       <c r="I2" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="J2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="L2" t="s">
         <v>165</v>
       </c>
       <c r="M2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>280</v>
       </c>
@@ -3588,7 +3615,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="F3" t="s">
         <v>141</v>
@@ -3612,10 +3639,10 @@
         <v>142</v>
       </c>
       <c r="M3" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>281</v>
       </c>
@@ -3629,34 +3656,34 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F4" t="s">
         <v>162</v>
       </c>
       <c r="G4" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H4" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="I4" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="K4" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="L4" t="s">
         <v>144</v>
       </c>
       <c r="M4" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>282</v>
       </c>
@@ -3679,7 +3706,7 @@
         <v>365</v>
       </c>
       <c r="H5" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="I5" t="s">
         <v>360</v>
@@ -3688,16 +3715,16 @@
         <v>145</v>
       </c>
       <c r="K5" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="L5" t="s">
         <v>152</v>
       </c>
       <c r="M5" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>283</v>
       </c>
@@ -3711,35 +3738,35 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F6" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G6" t="s">
         <v>365</v>
       </c>
       <c r="H6" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="I6" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="J6" t="s">
         <v>167</v>
       </c>
       <c r="K6" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="L6" t="s">
         <v>143</v>
       </c>
       <c r="M6" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
     <hyperlink ref="C3:C6" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
@@ -3762,23 +3789,23 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3792,10 +3819,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>146</v>
@@ -3816,7 +3843,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>289</v>
       </c>
@@ -3852,7 +3879,7 @@
       </c>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>290</v>
       </c>
@@ -3866,7 +3893,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="F3" t="s">
         <v>152</v>
@@ -3888,7 +3915,7 @@
       </c>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>291</v>
       </c>
@@ -3902,7 +3929,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>162</v>
@@ -3924,7 +3951,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>292</v>
       </c>
@@ -3960,7 +3987,7 @@
       </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>293</v>
       </c>
@@ -3974,10 +4001,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F6" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>153</v>
@@ -3997,7 +4024,7 @@
       <c r="L6" s="14"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{B284F8B5-B973-4DA0-AD0E-6728D7FF2354}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{BA950695-1ED2-4C3C-A09A-2262F4EB2FE2}"/>
@@ -4022,33 +4049,33 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>348</v>
@@ -4075,7 +4102,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>308</v>
       </c>
@@ -4110,7 +4137,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>309</v>
       </c>
@@ -4145,7 +4172,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>310</v>
       </c>
@@ -4180,7 +4207,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>311</v>
       </c>
@@ -4215,7 +4242,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -4251,7 +4278,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
@@ -4277,15 +4304,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4299,7 +4326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4313,7 +4340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4327,7 +4354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4341,7 +4368,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4355,7 +4382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4389,21 +4416,21 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4435,7 +4462,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4452,7 +4479,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4467,7 +4494,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4484,7 +4511,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -4499,7 +4526,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -4516,7 +4543,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4531,7 +4558,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4548,7 +4575,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -4563,7 +4590,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4580,7 +4607,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4596,7 +4623,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{9AD9969A-218A-4B7A-8213-84185638ECBE}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{C8A293E1-19AE-45A2-937B-B715A739FE8F}"/>
@@ -4620,23 +4647,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -4662,7 +4689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
@@ -4679,16 +4706,16 @@
         <v>132</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>45</v>
       </c>
@@ -4708,13 +4735,13 @@
         <v>133</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
@@ -4734,13 +4761,13 @@
         <v>133</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
@@ -4760,13 +4787,13 @@
         <v>133</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
@@ -4786,14 +4813,14 @@
         <v>133</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{165E166A-99CE-4ED9-B0B8-74EC9E8D61C4}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{E15F64F4-2545-4142-9338-629A10A0E6AF}"/>
@@ -4813,16 +4840,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4854,7 +4881,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -4886,7 +4913,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -4918,7 +4945,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -4950,7 +4977,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -4982,7 +5009,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -5034,18 +5061,18 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5065,13 +5092,13 @@
         <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>160</v>
       </c>
@@ -5088,16 +5115,16 @@
         <v>134</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="H2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -5114,16 +5141,16 @@
         <v>172</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="H3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -5140,16 +5167,16 @@
         <v>174</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G4" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="H4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>168</v>
       </c>
@@ -5166,16 +5193,16 @@
         <v>175</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G5" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="H5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>169</v>
       </c>
@@ -5192,10 +5219,10 @@
         <v>176</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="G6" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="H6" t="s">
         <v>173</v>
@@ -5217,28 +5244,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5255,34 +5282,34 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>383</v>
-      </c>
       <c r="L1" s="12" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>229</v>
       </c>
@@ -5295,26 +5322,29 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>372</v>
+      <c r="E2" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>374</v>
-      </c>
-      <c r="G2" t="s">
-        <v>444</v>
+        <v>373</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>462</v>
       </c>
       <c r="H2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>399</v>
+        <v>395</v>
+      </c>
+      <c r="L2" t="s">
+        <v>443</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>10</v>
@@ -5323,7 +5353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -5336,26 +5366,29 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>56</v>
+      <c r="E3" s="18" t="s">
+        <v>465</v>
       </c>
       <c r="F3" t="s">
-        <v>374</v>
-      </c>
-      <c r="G3" t="s">
+        <v>373</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>463</v>
+      </c>
+      <c r="H3" t="s">
         <v>376</v>
       </c>
-      <c r="H3" t="s">
-        <v>378</v>
-      </c>
       <c r="I3" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>399</v>
+        <v>395</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>466</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>10</v>
@@ -5364,7 +5397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -5377,26 +5410,29 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>381</v>
+      <c r="E4" s="18" t="s">
+        <v>467</v>
       </c>
       <c r="F4" t="s">
-        <v>374</v>
-      </c>
-      <c r="G4" t="s">
+        <v>373</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>464</v>
+      </c>
+      <c r="H4" t="s">
         <v>376</v>
       </c>
-      <c r="H4" t="s">
-        <v>378</v>
-      </c>
       <c r="I4" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>399</v>
+        <v>395</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>468</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -5405,7 +5441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -5418,26 +5454,29 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>382</v>
+      <c r="E5" s="18" t="s">
+        <v>469</v>
       </c>
       <c r="F5" t="s">
-        <v>374</v>
-      </c>
-      <c r="G5" t="s">
+        <v>373</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>463</v>
+      </c>
+      <c r="H5" t="s">
         <v>376</v>
       </c>
-      <c r="H5" t="s">
-        <v>378</v>
-      </c>
       <c r="I5" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>399</v>
+        <v>395</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>470</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>10</v>
@@ -5446,7 +5485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -5459,29 +5498,29 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
-        <v>59</v>
+      <c r="E6" s="18" t="s">
+        <v>471</v>
       </c>
       <c r="F6" t="s">
-        <v>374</v>
-      </c>
-      <c r="G6" t="s">
+        <v>373</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>464</v>
+      </c>
+      <c r="H6" t="s">
         <v>376</v>
       </c>
-      <c r="H6" t="s">
-        <v>378</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="L6" t="s">
-        <v>448</v>
+        <v>395</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>472</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>10</v>
@@ -5491,7 +5530,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{C39EAF5C-6B4F-497D-9205-270DC799982F}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{5742D762-70F8-4E32-935D-9EE50791260E}"/>
@@ -5512,16 +5551,16 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5535,10 +5574,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -5555,7 +5594,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -5572,7 +5611,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -5589,7 +5628,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -5606,7 +5645,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>245</v>
       </c>
@@ -5624,7 +5663,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
@@ -5644,36 +5683,36 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>42</v>
@@ -5682,146 +5721,146 @@
         <v>3</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
         <v>406</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>407</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>409</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>410</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>411</v>
       </c>
-      <c r="B3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>413</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>414</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>415</v>
       </c>
-      <c r="B4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" t="s">
+        <v>403</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>417</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
+        <v>413</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>418</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>403</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B5" t="s">
-        <v>407</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>421</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>414</v>
+      </c>
+      <c r="F6" t="s">
         <v>417</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>422</v>
-      </c>
-      <c r="B6" t="s">
-        <v>407</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>418</v>
-      </c>
-      <c r="F6" t="s">
-        <v>421</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>10</v>
@@ -5831,7 +5870,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{8505C122-2102-4146-B9D7-5E7E4E0527C2}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{F8A6FF10-0F6E-4529-B3EB-9DA5D19BBE35}"/>

</xml_diff>

<commit_message>
Implementation of POM methods is in progress
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arunkumar/IdeaProjects/AutomationCatalogue_TestingFramework/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED4A93D-85DE-C341-876E-4F4DC37E510A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1E9433-1320-4B5B-9FEE-9D2F60360B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" tabRatio="877" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="472">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1234,9 +1234,6 @@
     <t>Testcasename</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -1246,9 +1243,6 @@
     <t>Confirm password</t>
   </si>
   <si>
-    <t>TS08_01</t>
-  </si>
-  <si>
     <t>TS08_DemoWebshop_Registration</t>
   </si>
   <si>
@@ -1261,9 +1255,6 @@
     <t>ch</t>
   </si>
   <si>
-    <t>TS08_02</t>
-  </si>
-  <si>
     <t>anupreddy.desai@gmail.com</t>
   </si>
   <si>
@@ -1273,9 +1264,6 @@
     <t>reddy</t>
   </si>
   <si>
-    <t>TS08_03</t>
-  </si>
-  <si>
     <t>anupreddy2906@gmail.com</t>
   </si>
   <si>
@@ -1285,18 +1273,12 @@
     <t>Anup</t>
   </si>
   <si>
-    <t>TS08_04</t>
-  </si>
-  <si>
     <t>v.desai1295@gmail.com</t>
   </si>
   <si>
     <t>Venkata</t>
   </si>
   <si>
-    <t>TS08_05</t>
-  </si>
-  <si>
     <t>venkata.desai@gmail.com</t>
   </si>
   <si>
@@ -1457,6 +1439,21 @@
   </si>
   <si>
     <t>abrahammaize</t>
+  </si>
+  <si>
+    <t>TS08-01</t>
+  </si>
+  <si>
+    <t>TS08-02</t>
+  </si>
+  <si>
+    <t>TS08-03</t>
+  </si>
+  <si>
+    <t>TS08-04</t>
+  </si>
+  <si>
+    <t>TS08-05</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -1607,7 +1604,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1930,15 +1926,15 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>177</v>
       </c>
@@ -1961,7 +1957,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1971,7 +1967,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>181</v>
       </c>
@@ -1985,7 +1981,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>182</v>
       </c>
@@ -1999,7 +1995,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>183</v>
       </c>
@@ -2016,7 +2012,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>184</v>
       </c>
@@ -2030,7 +2026,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>185</v>
       </c>
@@ -2044,7 +2040,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -2054,7 +2050,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>188</v>
       </c>
@@ -2068,7 +2064,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>189</v>
       </c>
@@ -2082,7 +2078,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>190</v>
       </c>
@@ -2096,7 +2092,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>191</v>
       </c>
@@ -2110,7 +2106,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>192</v>
       </c>
@@ -2127,7 +2123,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -2137,7 +2133,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>198</v>
       </c>
@@ -2151,7 +2147,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>199</v>
       </c>
@@ -2165,7 +2161,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>200</v>
       </c>
@@ -2182,7 +2178,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>201</v>
       </c>
@@ -2196,7 +2192,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>202</v>
       </c>
@@ -2210,7 +2206,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2220,7 +2216,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>205</v>
       </c>
@@ -2237,7 +2233,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>206</v>
       </c>
@@ -2254,7 +2250,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>207</v>
       </c>
@@ -2268,7 +2264,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>208</v>
       </c>
@@ -2282,7 +2278,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>209</v>
       </c>
@@ -2296,7 +2292,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2306,7 +2302,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>217</v>
       </c>
@@ -2320,7 +2316,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>218</v>
       </c>
@@ -2334,7 +2330,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>219</v>
       </c>
@@ -2351,7 +2347,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>220</v>
       </c>
@@ -2368,7 +2364,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -2382,7 +2378,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -2392,7 +2388,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>224</v>
       </c>
@@ -2406,7 +2402,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>225</v>
       </c>
@@ -2420,7 +2416,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>226</v>
       </c>
@@ -2434,7 +2430,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>227</v>
       </c>
@@ -2448,7 +2444,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>228</v>
       </c>
@@ -2462,7 +2458,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -2472,7 +2468,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>236</v>
       </c>
@@ -2486,7 +2482,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>237</v>
       </c>
@@ -2500,7 +2496,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>238</v>
       </c>
@@ -2514,7 +2510,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>239</v>
       </c>
@@ -2528,7 +2524,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>240</v>
       </c>
@@ -2542,7 +2538,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -2552,7 +2548,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>247</v>
       </c>
@@ -2566,7 +2562,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>248</v>
       </c>
@@ -2580,7 +2576,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>249</v>
       </c>
@@ -2594,7 +2590,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>250</v>
       </c>
@@ -2608,7 +2604,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>251</v>
       </c>
@@ -2622,7 +2618,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2632,7 +2628,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>259</v>
       </c>
@@ -2646,7 +2642,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>260</v>
       </c>
@@ -2660,7 +2656,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>261</v>
       </c>
@@ -2674,7 +2670,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>262</v>
       </c>
@@ -2688,7 +2684,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>263</v>
       </c>
@@ -2702,7 +2698,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -2712,7 +2708,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>271</v>
       </c>
@@ -2726,7 +2722,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>272</v>
       </c>
@@ -2740,7 +2736,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>273</v>
       </c>
@@ -2754,7 +2750,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>274</v>
       </c>
@@ -2768,7 +2764,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>275</v>
       </c>
@@ -2782,7 +2778,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -2792,7 +2788,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>278</v>
       </c>
@@ -2806,7 +2802,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>285</v>
       </c>
@@ -2820,7 +2816,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>286</v>
       </c>
@@ -2834,7 +2830,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>287</v>
       </c>
@@ -2848,7 +2844,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>288</v>
       </c>
@@ -2862,7 +2858,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -2872,7 +2868,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>296</v>
       </c>
@@ -2886,7 +2882,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>297</v>
       </c>
@@ -2900,7 +2896,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>298</v>
       </c>
@@ -2914,7 +2910,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>299</v>
       </c>
@@ -2928,7 +2924,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>300</v>
       </c>
@@ -2942,7 +2938,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -2952,7 +2948,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>303</v>
       </c>
@@ -2966,7 +2962,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>304</v>
       </c>
@@ -2980,7 +2976,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>305</v>
       </c>
@@ -2994,7 +2990,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>306</v>
       </c>
@@ -3008,7 +3004,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>307</v>
       </c>
@@ -3036,27 +3032,27 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3106,7 +3102,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>264</v>
       </c>
@@ -3156,7 +3152,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>265</v>
       </c>
@@ -3206,7 +3202,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>266</v>
       </c>
@@ -3256,7 +3252,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -3306,7 +3302,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -3384,15 +3380,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3406,7 +3402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3420,7 +3416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3434,7 +3430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3448,7 +3444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3462,7 +3458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3502,24 +3498,24 @@
       <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3533,34 +3529,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>426</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>427</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -3580,28 +3576,28 @@
         <v>140</v>
       </c>
       <c r="G2" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="H2" t="s">
         <v>152</v>
       </c>
       <c r="I2" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="J2" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="K2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="L2" t="s">
         <v>165</v>
       </c>
       <c r="M2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>280</v>
       </c>
@@ -3615,7 +3611,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="F3" t="s">
         <v>141</v>
@@ -3639,10 +3635,10 @@
         <v>142</v>
       </c>
       <c r="M3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>281</v>
       </c>
@@ -3656,34 +3652,34 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="F4" t="s">
         <v>162</v>
       </c>
       <c r="G4" t="s">
+        <v>422</v>
+      </c>
+      <c r="H4" t="s">
+        <v>427</v>
+      </c>
+      <c r="I4" t="s">
+        <v>418</v>
+      </c>
+      <c r="J4" t="s">
         <v>428</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>433</v>
-      </c>
-      <c r="I4" t="s">
-        <v>424</v>
-      </c>
-      <c r="J4" t="s">
-        <v>434</v>
-      </c>
-      <c r="K4" t="s">
-        <v>439</v>
       </c>
       <c r="L4" t="s">
         <v>144</v>
       </c>
       <c r="M4" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>282</v>
       </c>
@@ -3706,7 +3702,7 @@
         <v>365</v>
       </c>
       <c r="H5" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="I5" t="s">
         <v>360</v>
@@ -3715,16 +3711,16 @@
         <v>145</v>
       </c>
       <c r="K5" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="L5" t="s">
         <v>152</v>
       </c>
       <c r="M5" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>283</v>
       </c>
@@ -3738,31 +3734,31 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="F6" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="G6" t="s">
         <v>365</v>
       </c>
       <c r="H6" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="I6" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="J6" t="s">
         <v>167</v>
       </c>
       <c r="K6" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="L6" t="s">
         <v>143</v>
       </c>
       <c r="M6" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -3789,23 +3785,23 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3819,10 +3815,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>146</v>
@@ -3843,7 +3839,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>289</v>
       </c>
@@ -3879,7 +3875,7 @@
       </c>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>290</v>
       </c>
@@ -3893,7 +3889,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="F3" t="s">
         <v>152</v>
@@ -3915,7 +3911,7 @@
       </c>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>291</v>
       </c>
@@ -3929,7 +3925,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>162</v>
@@ -3951,7 +3947,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>292</v>
       </c>
@@ -3987,7 +3983,7 @@
       </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>293</v>
       </c>
@@ -4001,10 +3997,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="F6" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>153</v>
@@ -4049,22 +4045,22 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>380</v>
       </c>
@@ -4102,7 +4098,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>308</v>
       </c>
@@ -4137,7 +4133,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>309</v>
       </c>
@@ -4172,7 +4168,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>310</v>
       </c>
@@ -4207,7 +4203,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>311</v>
       </c>
@@ -4242,7 +4238,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -4304,15 +4300,15 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4326,7 +4322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4340,7 +4336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4354,7 +4350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4368,7 +4364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4382,7 +4378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4416,21 +4412,21 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4462,7 +4458,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4479,7 +4475,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4494,7 +4490,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4511,7 +4507,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -4526,7 +4522,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -4543,7 +4539,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4558,7 +4554,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4575,7 +4571,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -4590,7 +4586,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4607,7 +4603,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4651,19 +4647,19 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -4689,7 +4685,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
@@ -4706,16 +4702,16 @@
         <v>132</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>45</v>
       </c>
@@ -4735,13 +4731,13 @@
         <v>133</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
@@ -4761,13 +4757,13 @@
         <v>133</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
@@ -4787,13 +4783,13 @@
         <v>133</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
@@ -4813,7 +4809,7 @@
         <v>133</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>136</v>
@@ -4840,16 +4836,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4881,7 +4877,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -4913,7 +4909,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -4945,7 +4941,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -4977,7 +4973,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -5009,7 +5005,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -5061,18 +5057,18 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5098,7 +5094,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>160</v>
       </c>
@@ -5124,7 +5120,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -5150,7 +5146,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -5176,7 +5172,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>168</v>
       </c>
@@ -5202,7 +5198,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>169</v>
       </c>
@@ -5244,28 +5240,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5300,16 +5296,16 @@
         <v>379</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>229</v>
       </c>
@@ -5322,14 +5318,14 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>59</v>
       </c>
       <c r="F2" t="s">
         <v>373</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>462</v>
+      <c r="G2" t="s">
+        <v>456</v>
       </c>
       <c r="H2" t="s">
         <v>376</v>
@@ -5344,7 +5340,7 @@
         <v>395</v>
       </c>
       <c r="L2" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>10</v>
@@ -5353,7 +5349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -5366,14 +5362,14 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>465</v>
+      <c r="E3" s="17" t="s">
+        <v>459</v>
       </c>
       <c r="F3" t="s">
         <v>373</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>463</v>
+      <c r="G3" t="s">
+        <v>457</v>
       </c>
       <c r="H3" t="s">
         <v>376</v>
@@ -5387,8 +5383,8 @@
       <c r="K3" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="L3" s="18" t="s">
-        <v>466</v>
+      <c r="L3" s="17" t="s">
+        <v>460</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>10</v>
@@ -5397,7 +5393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -5410,14 +5406,14 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>467</v>
+      <c r="E4" s="17" t="s">
+        <v>461</v>
       </c>
       <c r="F4" t="s">
         <v>373</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>464</v>
+      <c r="G4" t="s">
+        <v>458</v>
       </c>
       <c r="H4" t="s">
         <v>376</v>
@@ -5431,8 +5427,8 @@
       <c r="K4" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>468</v>
+      <c r="L4" s="17" t="s">
+        <v>462</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -5441,7 +5437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -5454,14 +5450,14 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>469</v>
+      <c r="E5" s="17" t="s">
+        <v>463</v>
       </c>
       <c r="F5" t="s">
         <v>373</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>463</v>
+      <c r="G5" t="s">
+        <v>457</v>
       </c>
       <c r="H5" t="s">
         <v>376</v>
@@ -5475,8 +5471,8 @@
       <c r="K5" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="L5" s="18" t="s">
-        <v>470</v>
+      <c r="L5" s="17" t="s">
+        <v>464</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>10</v>
@@ -5485,7 +5481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -5498,14 +5494,14 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>471</v>
+      <c r="E6" s="17" t="s">
+        <v>465</v>
       </c>
       <c r="F6" t="s">
         <v>373</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>464</v>
+      <c r="G6" t="s">
+        <v>458</v>
       </c>
       <c r="H6" t="s">
         <v>376</v>
@@ -5519,8 +5515,8 @@
       <c r="K6" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="L6" s="18" t="s">
-        <v>472</v>
+      <c r="L6" s="17" t="s">
+        <v>466</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>10</v>
@@ -5551,16 +5547,16 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5574,10 +5570,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -5594,7 +5590,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -5611,7 +5607,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -5628,7 +5624,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -5645,7 +5641,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>245</v>
       </c>
@@ -5677,25 +5673,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>396</v>
       </c>
@@ -5706,197 +5700,151 @@
         <v>398</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="F2" t="s">
-        <v>406</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>407</v>
-      </c>
-      <c r="B3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" t="s">
+        <v>409</v>
+      </c>
+      <c r="D4" t="s">
+        <v>410</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>470</v>
+      </c>
+      <c r="B5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D5" t="s">
         <v>409</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E5" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>471</v>
+      </c>
+      <c r="B6" t="s">
+        <v>401</v>
+      </c>
+      <c r="C6" t="s">
         <v>410</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>411</v>
-      </c>
-      <c r="B4" t="s">
-        <v>403</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D6" t="s">
         <v>412</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E6" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="F4" t="s">
-        <v>414</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B5" t="s">
-        <v>403</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>417</v>
-      </c>
-      <c r="F5" t="s">
-        <v>413</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>418</v>
-      </c>
-      <c r="B6" t="s">
-        <v>403</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>414</v>
-      </c>
-      <c r="F6" t="s">
-        <v>417</v>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{8505C122-2102-4146-B9D7-5E7E4E0527C2}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{F8A6FF10-0F6E-4529-B3EB-9DA5D19BBE35}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{D688E348-9F41-4365-8635-E3E497D8044D}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{A6E973EA-A807-4CDA-9F4D-CA5679A28AE2}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{773D28DD-AEFD-4B00-A8CC-371A958C9482}"/>
-    <hyperlink ref="D2" r:id="rId6" xr:uid="{913C1F99-88B3-40E2-88A9-0E73642C298A}"/>
-    <hyperlink ref="D3" r:id="rId7" xr:uid="{85555F14-1A00-489D-839F-4962623D89F4}"/>
-    <hyperlink ref="D4" r:id="rId8" xr:uid="{EC2AE3C3-D60E-40A7-9EA9-C860104A0FFC}"/>
-    <hyperlink ref="D5" r:id="rId9" xr:uid="{BA0F4533-F1FE-48E4-979E-0E8B44A92DA2}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{6D3FCDCB-044E-49E6-87F5-319651F27EE0}"/>
-    <hyperlink ref="G2" r:id="rId11" xr:uid="{2A0F8DDB-929D-4DB5-B961-AB1107EF2462}"/>
-    <hyperlink ref="G3" r:id="rId12" xr:uid="{AB13969F-4570-4481-A4F9-799148F68C6F}"/>
-    <hyperlink ref="G4" r:id="rId13" xr:uid="{045939CD-A3D8-433B-AE4A-17DE3C120125}"/>
-    <hyperlink ref="G5" r:id="rId14" xr:uid="{9EC052A2-EE02-49EA-B598-D49BB2777863}"/>
-    <hyperlink ref="G6" r:id="rId15" xr:uid="{3882F933-D459-432F-82B8-857CA1B4CBCA}"/>
-    <hyperlink ref="H2" r:id="rId16" xr:uid="{A02253FE-E3B4-415C-A6D2-E7E4896454DF}"/>
-    <hyperlink ref="H3" r:id="rId17" xr:uid="{499E51C2-76E4-4589-9D09-2EFA90EAC863}"/>
-    <hyperlink ref="H4" r:id="rId18" xr:uid="{9014AEF5-BFDD-4BCA-866A-BF730D30FA20}"/>
-    <hyperlink ref="H5" r:id="rId19" xr:uid="{FFC4B713-AD34-45A1-9833-7C5705B6263D}"/>
-    <hyperlink ref="H6" r:id="rId20" xr:uid="{030AE3A3-14E1-486F-BD5E-106C4A85DE27}"/>
-    <hyperlink ref="I2" r:id="rId21" xr:uid="{18F148A7-E58C-42B5-9FF9-E47C5E943794}"/>
-    <hyperlink ref="I3" r:id="rId22" xr:uid="{7C2E4059-26E3-4700-AEF4-6CC447E57C3C}"/>
-    <hyperlink ref="I4" r:id="rId23" xr:uid="{591360A2-F11D-4865-9ABC-BD80B8FFA414}"/>
-    <hyperlink ref="I5" r:id="rId24" xr:uid="{57834260-FD0C-4DC5-BBAE-34A140B13157}"/>
-    <hyperlink ref="I6" r:id="rId25" xr:uid="{31445ED0-F4B7-454D-92D0-F5E877CB8B1D}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{2A0F8DDB-929D-4DB5-B961-AB1107EF2462}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{AB13969F-4570-4481-A4F9-799148F68C6F}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{045939CD-A3D8-433B-AE4A-17DE3C120125}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{9EC052A2-EE02-49EA-B598-D49BB2777863}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{3882F933-D459-432F-82B8-857CA1B4CBCA}"/>
+    <hyperlink ref="F2" r:id="rId6" xr:uid="{A02253FE-E3B4-415C-A6D2-E7E4896454DF}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{499E51C2-76E4-4589-9D09-2EFA90EAC863}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{9014AEF5-BFDD-4BCA-866A-BF730D30FA20}"/>
+    <hyperlink ref="F5" r:id="rId9" xr:uid="{FFC4B713-AD34-45A1-9833-7C5705B6263D}"/>
+    <hyperlink ref="F6" r:id="rId10" xr:uid="{030AE3A3-14E1-486F-BD5E-106C4A85DE27}"/>
+    <hyperlink ref="G2" r:id="rId11" xr:uid="{18F148A7-E58C-42B5-9FF9-E47C5E943794}"/>
+    <hyperlink ref="G3" r:id="rId12" xr:uid="{7C2E4059-26E3-4700-AEF4-6CC447E57C3C}"/>
+    <hyperlink ref="G4" r:id="rId13" xr:uid="{591360A2-F11D-4865-9ABC-BD80B8FFA414}"/>
+    <hyperlink ref="G5" r:id="rId14" xr:uid="{57834260-FD0C-4DC5-BBAE-34A140B13157}"/>
+    <hyperlink ref="G6" r:id="rId15" xr:uid="{31445ED0-F4B7-454D-92D0-F5E877CB8B1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Completed Code changes of POM of all testcases
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -8,25 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1E9433-1320-4B5B-9FEE-9D2F60360B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E597B175-82BB-4CB9-B74B-20C5A882B76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
     <sheet name="HRM_Login" sheetId="2" r:id="rId2"/>
     <sheet name="HRM_AddUser" sheetId="3" r:id="rId3"/>
     <sheet name="HRM_Reports" sheetId="4" r:id="rId4"/>
-    <sheet name="HRM_Attendance" sheetId="5" r:id="rId5"/>
-    <sheet name="HRM_Leave" sheetId="6" r:id="rId6"/>
-    <sheet name="HRM_Performance" sheetId="7" r:id="rId7"/>
-    <sheet name="HRM_Nationality" sheetId="8" r:id="rId8"/>
-    <sheet name="Demo_Registration" sheetId="9" r:id="rId9"/>
-    <sheet name="Demo_CreateAddress" sheetId="10" r:id="rId10"/>
-    <sheet name="Demo_TotalOrders" sheetId="12" r:id="rId11"/>
-    <sheet name="Demo_MultipleProducts" sheetId="11" r:id="rId12"/>
-    <sheet name="Demo_ApplyDiscount" sheetId="13" r:id="rId13"/>
-    <sheet name="Demo_PlaceOrder" sheetId="14" r:id="rId14"/>
+    <sheet name="HRM_Leave" sheetId="6" r:id="rId5"/>
+    <sheet name="HRM_Performance" sheetId="7" r:id="rId6"/>
+    <sheet name="HRM_Nationality" sheetId="8" r:id="rId7"/>
+    <sheet name="Demo_Registration" sheetId="9" r:id="rId8"/>
+    <sheet name="Demo_CreateAddress" sheetId="10" r:id="rId9"/>
+    <sheet name="Demo_TotalOrders" sheetId="12" r:id="rId10"/>
+    <sheet name="Demo_MultipleProducts" sheetId="11" r:id="rId11"/>
+    <sheet name="Demo_ApplyDiscount" sheetId="13" r:id="rId12"/>
+    <sheet name="Demo_PlaceOrder" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="438">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -454,9 +453,6 @@
     <t>Travel and Expense Summary Report</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Estimated Expenses</t>
   </si>
   <si>
@@ -523,9 +519,6 @@
     <t>TC05-01</t>
   </si>
   <si>
-    <t>Demo_MultipleProducts</t>
-  </si>
-  <si>
     <t>14.1-inch Laptop</t>
   </si>
   <si>
@@ -631,9 +624,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Orange HRM Reports</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -652,9 +642,6 @@
     <t>Reports and Analytics TestData in OrangeHRM Application</t>
   </si>
   <si>
-    <t>Orange HRM Attendance</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -685,9 +672,6 @@
     <t>TC04-05</t>
   </si>
   <si>
-    <t>Validating the PunchIn and Puchout of Employee</t>
-  </si>
-  <si>
     <t>Orange HRM Leave</t>
   </si>
   <si>
@@ -922,9 +906,6 @@
     <t>TC12-05</t>
   </si>
   <si>
-    <t>DemoWebshop ApplyDiscount</t>
-  </si>
-  <si>
     <t>Demo Webshop Apply Discount</t>
   </si>
   <si>
@@ -949,36 +930,6 @@
     <t>Demo Webshop Place Order</t>
   </si>
   <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>TC13-01</t>
-  </si>
-  <si>
-    <t>TC13-02</t>
-  </si>
-  <si>
-    <t>TC13-03</t>
-  </si>
-  <si>
-    <t>TC13-04</t>
-  </si>
-  <si>
-    <t>TC13-05</t>
-  </si>
-  <si>
     <t>Placing an Order using In-Store Pickup in Demo Webshop</t>
   </si>
   <si>
@@ -991,18 +942,6 @@
     <t>TC03_OrangeHRM_Reports_Analytics</t>
   </si>
   <si>
-    <t>TC04_OrangeHRM_Attendance</t>
-  </si>
-  <si>
-    <t>TC05_OrangeHRM_Leave</t>
-  </si>
-  <si>
-    <t>TC06_OrangeHRM_Performance</t>
-  </si>
-  <si>
-    <t>TC07_OrangeHRM_Nationality</t>
-  </si>
-  <si>
     <t>IndiaA</t>
   </si>
   <si>
@@ -1018,72 +957,6 @@
     <t>BazilE</t>
   </si>
   <si>
-    <t>TC08_DemoWebshop_Registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Out Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Out Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Out Note</t>
-  </si>
-  <si>
-    <t>1/6/2020</t>
-  </si>
-  <si>
-    <t>10:30</t>
-  </si>
-  <si>
-    <t>5:30</t>
-  </si>
-  <si>
-    <t>1/6/2021</t>
-  </si>
-  <si>
-    <t>10:31</t>
-  </si>
-  <si>
-    <t>5:31</t>
-  </si>
-  <si>
-    <t>1/6/2022</t>
-  </si>
-  <si>
-    <t>10:32</t>
-  </si>
-  <si>
-    <t>5:32</t>
-  </si>
-  <si>
-    <t>1/6/2023</t>
-  </si>
-  <si>
-    <t>10:33</t>
-  </si>
-  <si>
-    <t>5:33</t>
-  </si>
-  <si>
-    <t>1/6/2024</t>
-  </si>
-  <si>
-    <t>10:34</t>
-  </si>
-  <si>
-    <t>5:34</t>
-  </si>
-  <si>
     <t>Categories</t>
   </si>
   <si>
@@ -1141,9 +1014,6 @@
     <t>$5 Virtual Gift Card</t>
   </si>
   <si>
-    <t>TC13_DemoWebshop_PlaceOrder</t>
-  </si>
-  <si>
     <t>CreateUserName</t>
   </si>
   <si>
@@ -1153,9 +1023,6 @@
     <t>NewUser Confirm Password</t>
   </si>
   <si>
-    <t>TC08_DemoWebshop_TotalOrders</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -1243,9 +1110,6 @@
     <t>Confirm password</t>
   </si>
   <si>
-    <t>TS08_DemoWebshop_Registration</t>
-  </si>
-  <si>
     <t>aarosagarch@gamil.com</t>
   </si>
   <si>
@@ -1441,19 +1305,52 @@
     <t>abrahammaize</t>
   </si>
   <si>
-    <t>TS08-01</t>
-  </si>
-  <si>
-    <t>TS08-02</t>
-  </si>
-  <si>
-    <t>TS08-03</t>
-  </si>
-  <si>
-    <t>TS08-04</t>
-  </si>
-  <si>
-    <t>TS08-05</t>
+    <t>Orange HRM Reports And Analytics</t>
+  </si>
+  <si>
+    <t>TC04_OrangeHRM_Leave</t>
+  </si>
+  <si>
+    <t>TC05_OrangeHRM_Performance</t>
+  </si>
+  <si>
+    <t>TC06_OrangeHRM_Nationality</t>
+  </si>
+  <si>
+    <t>TC07_DemoWebshop_Registration</t>
+  </si>
+  <si>
+    <t>TC08_DemoWebShop_CreateAddress</t>
+  </si>
+  <si>
+    <t>TC09_DemoWebShop_TotalOrders</t>
+  </si>
+  <si>
+    <t>TC10_DemoWebShop_MultipleOrders</t>
+  </si>
+  <si>
+    <t>TC11_DemoWebShop_ApplyDiscount</t>
+  </si>
+  <si>
+    <t>TC12_DemoWebShop_PlaceOrder</t>
+  </si>
+  <si>
+    <t>TS07-01</t>
+  </si>
+  <si>
+    <t>TS07-02</t>
+  </si>
+  <si>
+    <t>TS07-03</t>
+  </si>
+  <si>
+    <t>TS07-04</t>
+  </si>
+  <si>
+    <t>TS07-05</t>
+  </si>
+  <si>
+    <t>TS07_DemoWebshop_Registration</t>
   </si>
 </sst>
 </file>
@@ -1576,7 +1473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -1605,6 +1502,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1920,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1936,7 +1836,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>
@@ -1945,23 +1845,23 @@
         <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1969,82 +1869,82 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2052,82 +1952,82 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="D13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>197</v>
+        <v>422</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2135,82 +2035,82 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="D15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="D16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="D17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="D18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2218,85 +2118,85 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C21" t="s">
-        <v>317</v>
+        <v>423</v>
       </c>
       <c r="D21" t="s">
-        <v>215</v>
-      </c>
-      <c r="E21" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
-        <v>317</v>
+        <v>423</v>
       </c>
       <c r="D22" t="s">
-        <v>215</v>
-      </c>
-      <c r="E22" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C23" t="s">
-        <v>317</v>
+        <v>423</v>
       </c>
       <c r="D23" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="E23" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C24" t="s">
-        <v>317</v>
+        <v>423</v>
       </c>
       <c r="D24" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="E24" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C25" t="s">
-        <v>317</v>
+        <v>423</v>
       </c>
       <c r="D25" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2304,85 +2204,79 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
-        <v>318</v>
+        <v>424</v>
       </c>
       <c r="D27" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C28" t="s">
-        <v>318</v>
+        <v>424</v>
       </c>
       <c r="D28" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C29" t="s">
-        <v>318</v>
+        <v>424</v>
       </c>
       <c r="D29" t="s">
-        <v>222</v>
-      </c>
-      <c r="E29" t="s">
-        <v>196</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
-        <v>318</v>
+        <v>424</v>
       </c>
       <c r="D30" t="s">
-        <v>222</v>
-      </c>
-      <c r="E30" t="s">
-        <v>196</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
-        <v>318</v>
+        <v>424</v>
       </c>
       <c r="D31" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2390,79 +2284,79 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B33" t="s">
         <v>224</v>
       </c>
-      <c r="B33" t="s">
-        <v>229</v>
-      </c>
       <c r="C33" t="s">
-        <v>319</v>
+        <v>425</v>
       </c>
       <c r="D33" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B34" t="s">
         <v>225</v>
       </c>
-      <c r="B34" t="s">
-        <v>230</v>
-      </c>
       <c r="C34" t="s">
-        <v>319</v>
+        <v>425</v>
       </c>
       <c r="D34" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B35" t="s">
         <v>226</v>
       </c>
-      <c r="B35" t="s">
-        <v>231</v>
-      </c>
       <c r="C35" t="s">
-        <v>319</v>
+        <v>425</v>
       </c>
       <c r="D35" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" t="s">
         <v>227</v>
       </c>
-      <c r="B36" t="s">
-        <v>232</v>
-      </c>
       <c r="C36" t="s">
-        <v>319</v>
+        <v>425</v>
       </c>
       <c r="D36" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B37" t="s">
         <v>228</v>
       </c>
-      <c r="B37" t="s">
-        <v>233</v>
-      </c>
       <c r="C37" t="s">
-        <v>319</v>
+        <v>425</v>
       </c>
       <c r="D37" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2470,79 +2364,79 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B39" t="s">
         <v>236</v>
       </c>
-      <c r="B39" t="s">
-        <v>241</v>
-      </c>
       <c r="C39" t="s">
-        <v>320</v>
+        <v>426</v>
       </c>
       <c r="D39" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" t="s">
         <v>237</v>
       </c>
-      <c r="B40" t="s">
-        <v>242</v>
-      </c>
       <c r="C40" t="s">
-        <v>320</v>
+        <v>426</v>
       </c>
       <c r="D40" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B41" t="s">
         <v>238</v>
       </c>
-      <c r="B41" t="s">
-        <v>243</v>
-      </c>
       <c r="C41" t="s">
-        <v>320</v>
+        <v>426</v>
       </c>
       <c r="D41" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" t="s">
         <v>239</v>
       </c>
-      <c r="B42" t="s">
-        <v>244</v>
-      </c>
       <c r="C42" t="s">
-        <v>320</v>
+        <v>426</v>
       </c>
       <c r="D42" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B43" t="s">
         <v>240</v>
       </c>
-      <c r="B43" t="s">
-        <v>245</v>
-      </c>
       <c r="C43" t="s">
-        <v>320</v>
+        <v>426</v>
       </c>
       <c r="D43" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>258</v>
+        <v>39</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2550,79 +2444,79 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" t="s">
         <v>247</v>
       </c>
-      <c r="B45" t="s">
-        <v>252</v>
-      </c>
       <c r="C45" t="s">
-        <v>326</v>
+        <v>427</v>
       </c>
       <c r="D45" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" t="s">
         <v>248</v>
       </c>
-      <c r="B46" t="s">
-        <v>253</v>
-      </c>
       <c r="C46" t="s">
-        <v>326</v>
+        <v>427</v>
       </c>
       <c r="D46" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B47" t="s">
         <v>249</v>
       </c>
-      <c r="B47" t="s">
-        <v>254</v>
-      </c>
       <c r="C47" t="s">
-        <v>326</v>
+        <v>427</v>
       </c>
       <c r="D47" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B48" t="s">
         <v>250</v>
       </c>
-      <c r="B48" t="s">
-        <v>255</v>
-      </c>
       <c r="C48" t="s">
-        <v>326</v>
+        <v>427</v>
       </c>
       <c r="D48" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B49" t="s">
         <v>251</v>
       </c>
-      <c r="B49" t="s">
-        <v>256</v>
-      </c>
       <c r="C49" t="s">
-        <v>326</v>
+        <v>427</v>
       </c>
       <c r="D49" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>39</v>
+        <v>265</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2630,79 +2524,79 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B51" t="s">
         <v>259</v>
       </c>
-      <c r="B51" t="s">
-        <v>264</v>
-      </c>
       <c r="C51" t="s">
-        <v>39</v>
+        <v>428</v>
       </c>
       <c r="D51" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B52" t="s">
         <v>260</v>
       </c>
-      <c r="B52" t="s">
-        <v>265</v>
-      </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>428</v>
       </c>
       <c r="D52" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B53" t="s">
         <v>261</v>
       </c>
-      <c r="B53" t="s">
-        <v>266</v>
-      </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>428</v>
       </c>
       <c r="D53" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B54" t="s">
         <v>262</v>
       </c>
-      <c r="B54" t="s">
-        <v>267</v>
-      </c>
       <c r="C54" t="s">
-        <v>39</v>
+        <v>428</v>
       </c>
       <c r="D54" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B55" t="s">
         <v>263</v>
       </c>
-      <c r="B55" t="s">
-        <v>268</v>
-      </c>
       <c r="C55" t="s">
-        <v>39</v>
+        <v>428</v>
       </c>
       <c r="D55" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2710,79 +2604,79 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B57" t="s">
         <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>270</v>
+        <v>429</v>
       </c>
       <c r="D57" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B58" t="s">
         <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>270</v>
+        <v>429</v>
       </c>
       <c r="D58" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B59" t="s">
         <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>270</v>
+        <v>429</v>
       </c>
       <c r="D59" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B60" t="s">
         <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>270</v>
+        <v>429</v>
       </c>
       <c r="D60" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B61" t="s">
         <v>38</v>
       </c>
       <c r="C61" t="s">
-        <v>270</v>
+        <v>429</v>
       </c>
       <c r="D61" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2790,79 +2684,79 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B63" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C63" t="s">
-        <v>277</v>
+        <v>430</v>
       </c>
       <c r="D63" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B64" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C64" t="s">
-        <v>277</v>
+        <v>430</v>
       </c>
       <c r="D64" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B65" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C65" t="s">
-        <v>277</v>
+        <v>430</v>
       </c>
       <c r="D65" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B66" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C66" t="s">
-        <v>277</v>
+        <v>430</v>
       </c>
       <c r="D66" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B67" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C67" t="s">
-        <v>277</v>
+        <v>430</v>
       </c>
       <c r="D67" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2870,152 +2764,72 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B69" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C69" t="s">
-        <v>295</v>
+        <v>431</v>
       </c>
       <c r="D69" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B70" t="s">
+        <v>285</v>
+      </c>
+      <c r="C70" t="s">
+        <v>431</v>
+      </c>
+      <c r="D70" t="s">
         <v>297</v>
-      </c>
-      <c r="B70" t="s">
-        <v>290</v>
-      </c>
-      <c r="C70" t="s">
-        <v>295</v>
-      </c>
-      <c r="D70" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B71" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C71" t="s">
-        <v>295</v>
+        <v>431</v>
       </c>
       <c r="D71" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B72" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C72" t="s">
-        <v>295</v>
+        <v>431</v>
       </c>
       <c r="D72" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B73" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C73" t="s">
-        <v>295</v>
+        <v>431</v>
       </c>
       <c r="D73" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B75" t="s">
-        <v>308</v>
-      </c>
-      <c r="C75" t="s">
-        <v>367</v>
-      </c>
-      <c r="D75" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B76" t="s">
-        <v>309</v>
-      </c>
-      <c r="C76" t="s">
-        <v>367</v>
-      </c>
-      <c r="D76" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B77" t="s">
-        <v>310</v>
-      </c>
-      <c r="C77" t="s">
-        <v>367</v>
-      </c>
-      <c r="D77" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="B78" t="s">
-        <v>311</v>
-      </c>
-      <c r="C78" t="s">
-        <v>367</v>
-      </c>
-      <c r="D78" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B79" t="s">
-        <v>312</v>
-      </c>
-      <c r="C79" t="s">
-        <v>367</v>
-      </c>
-      <c r="D79" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -3025,354 +2839,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:P6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M2" t="s">
-        <v>81</v>
-      </c>
-      <c r="N2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>265</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" t="s">
-        <v>88</v>
-      </c>
-      <c r="K3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M3" t="s">
-        <v>91</v>
-      </c>
-      <c r="N3" t="s">
-        <v>92</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" t="s">
-        <v>98</v>
-      </c>
-      <c r="K4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L4" t="s">
-        <v>100</v>
-      </c>
-      <c r="M4" t="s">
-        <v>101</v>
-      </c>
-      <c r="N4" t="s">
-        <v>102</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>267</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" t="s">
-        <v>108</v>
-      </c>
-      <c r="L5" t="s">
-        <v>109</v>
-      </c>
-      <c r="M5" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>268</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" t="s">
-        <v>115</v>
-      </c>
-      <c r="J6" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L6" t="s">
-        <v>117</v>
-      </c>
-      <c r="M6" t="s">
-        <v>125</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{0CFF6622-BAB0-4347-BF40-8454C1587B08}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{525EFD10-CCA5-4147-9725-D6BEDEE56E77}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{95AB71B3-4F4B-4D6A-B569-80362339980B}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{ED03B573-C665-46CB-B7C4-927872D8665B}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{C6C3BEA3-AFDF-4421-B679-B47318860373}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{42AC4B95-883A-4B03-8546-2347A0DEC06E}"/>
-    <hyperlink ref="C3:C6" r:id="rId7" display="aarosagarch@gmail.com" xr:uid="{55484541-91C2-427A-AAD4-4C4E61824716}"/>
-    <hyperlink ref="G2" r:id="rId8" xr:uid="{AA2F8371-C8C6-4427-AFBA-C78BEE2FB2F0}"/>
-    <hyperlink ref="G3" r:id="rId9" xr:uid="{E9A37910-8F5B-4DDE-8C09-6425CB5A7F2C}"/>
-    <hyperlink ref="G4" r:id="rId10" xr:uid="{C8AF07B7-5BEE-4826-BEB2-83257AF3C032}"/>
-    <hyperlink ref="G5" r:id="rId11" xr:uid="{4C0578FF-503E-4494-BA41-62B8D45BE900}"/>
-    <hyperlink ref="G6" r:id="rId12" xr:uid="{1ED313F1-8BB0-40AA-9458-C814A11521E4}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -3396,7 +2862,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -3404,10 +2870,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>428</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -3418,10 +2884,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>260</v>
       </c>
       <c r="B3" t="s">
-        <v>371</v>
+        <v>428</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -3432,10 +2898,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
-        <v>371</v>
+        <v>428</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -3446,10 +2912,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>262</v>
       </c>
       <c r="B5" t="s">
-        <v>371</v>
+        <v>428</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -3460,10 +2926,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>263</v>
       </c>
       <c r="B6" t="s">
-        <v>371</v>
+        <v>428</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -3490,18 +2956,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
@@ -3523,45 +2989,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>414</v>
+        <v>369</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>420</v>
+        <v>375</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>415</v>
+        <v>370</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>421</v>
+        <v>376</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>416</v>
+        <v>371</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>423</v>
+        <v>378</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>417</v>
+        <v>372</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>425</v>
+        <v>380</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>429</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -3570,39 +3036,39 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G2" t="s">
-        <v>419</v>
+        <v>374</v>
       </c>
       <c r="H2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I2" t="s">
-        <v>422</v>
+        <v>377</v>
       </c>
       <c r="J2" t="s">
-        <v>424</v>
+        <v>379</v>
       </c>
       <c r="K2" t="s">
-        <v>418</v>
+        <v>373</v>
       </c>
       <c r="L2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M2" t="s">
-        <v>438</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>429</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -3611,39 +3077,39 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>433</v>
+        <v>388</v>
       </c>
       <c r="F3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" t="s">
+        <v>321</v>
+      </c>
+      <c r="H3" t="s">
+        <v>322</v>
+      </c>
+      <c r="I3" t="s">
+        <v>323</v>
+      </c>
+      <c r="J3" t="s">
+        <v>324</v>
+      </c>
+      <c r="K3" t="s">
+        <v>318</v>
+      </c>
+      <c r="L3" t="s">
         <v>141</v>
       </c>
-      <c r="G3" t="s">
-        <v>363</v>
-      </c>
-      <c r="H3" t="s">
-        <v>364</v>
-      </c>
-      <c r="I3" t="s">
-        <v>365</v>
-      </c>
-      <c r="J3" t="s">
-        <v>366</v>
-      </c>
-      <c r="K3" t="s">
-        <v>360</v>
-      </c>
-      <c r="L3" t="s">
-        <v>142</v>
-      </c>
       <c r="M3" t="s">
-        <v>439</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>429</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -3652,39 +3118,39 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>426</v>
+        <v>381</v>
       </c>
       <c r="F4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G4" t="s">
-        <v>422</v>
+        <v>377</v>
       </c>
       <c r="H4" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="I4" t="s">
-        <v>418</v>
+        <v>373</v>
       </c>
       <c r="J4" t="s">
-        <v>428</v>
+        <v>383</v>
       </c>
       <c r="K4" t="s">
-        <v>433</v>
+        <v>388</v>
       </c>
       <c r="L4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M4" t="s">
-        <v>440</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>429</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -3693,39 +3159,39 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
       <c r="F5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G5" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
       <c r="H5" t="s">
-        <v>429</v>
+        <v>384</v>
       </c>
       <c r="I5" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="J5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K5" t="s">
-        <v>419</v>
+        <v>374</v>
       </c>
       <c r="L5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M5" t="s">
-        <v>441</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>283</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>429</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -3734,31 +3200,31 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>418</v>
+        <v>373</v>
       </c>
       <c r="F6" t="s">
-        <v>431</v>
+        <v>386</v>
       </c>
       <c r="G6" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
       <c r="H6" t="s">
-        <v>432</v>
+        <v>387</v>
       </c>
       <c r="I6" t="s">
-        <v>430</v>
+        <v>385</v>
       </c>
       <c r="J6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K6" t="s">
-        <v>418</v>
+        <v>373</v>
       </c>
       <c r="L6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M6" t="s">
-        <v>442</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -3777,18 +3243,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
@@ -3815,36 +3281,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>414</v>
+        <v>369</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>420</v>
+        <v>375</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>151</v>
-      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>289</v>
+      <c r="A2" s="18" t="s">
+        <v>274</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>294</v>
+        <v>430</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>33</v>
@@ -3853,34 +3319,34 @@
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G2" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="K2" s="15" t="s">
-        <v>157</v>
-      </c>
       <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>290</v>
+      <c r="A3" s="18" t="s">
+        <v>275</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>294</v>
+        <v>430</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>33</v>
@@ -3889,34 +3355,34 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>419</v>
+        <v>374</v>
       </c>
       <c r="F3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>157</v>
-      </c>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>291</v>
+      <c r="A4" s="18" t="s">
+        <v>276</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>294</v>
+        <v>430</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -3925,34 +3391,34 @@
         <v>10</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>426</v>
+        <v>381</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G4" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="J4" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>157</v>
-      </c>
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>292</v>
+      <c r="A5" s="18" t="s">
+        <v>277</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>294</v>
+        <v>430</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>33</v>
@@ -3961,34 +3427,34 @@
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G5" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="J5" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="K5" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="K5" s="15" t="s">
-        <v>157</v>
-      </c>
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>293</v>
+      <c r="A6" s="18" t="s">
+        <v>278</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>294</v>
+        <v>430</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>33</v>
@@ -3997,25 +3463,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>422</v>
+        <v>377</v>
       </c>
       <c r="F6" t="s">
-        <v>424</v>
+        <v>379</v>
       </c>
       <c r="G6" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="K6" s="15" t="s">
         <v>156</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>157</v>
       </c>
       <c r="L6" s="14"/>
     </row>
@@ -4037,17 +3503,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
@@ -4062,48 +3528,48 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>380</v>
+        <v>336</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>381</v>
+        <v>337</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>382</v>
+        <v>338</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>383</v>
+        <v>339</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>351</v>
+        <v>309</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>352</v>
+        <v>310</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>353</v>
+        <v>311</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>354</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
+        <v>431</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -4112,33 +3578,33 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>355</v>
+        <v>313</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G2" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="H2" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="I2" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="J2" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="K2" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="B3" t="s">
-        <v>367</v>
+        <v>431</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -4147,33 +3613,33 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G3" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="H3" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="I3" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="J3" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="K3" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>367</v>
+        <v>431</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -4182,33 +3648,33 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>361</v>
+        <v>319</v>
       </c>
       <c r="F4" t="s">
-        <v>362</v>
+        <v>320</v>
       </c>
       <c r="G4" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="H4" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="I4" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="J4" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="K4" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="B5" t="s">
-        <v>367</v>
+        <v>431</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -4217,33 +3683,33 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="G5" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="H5" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="I5" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="J5" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="K5" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="B6" t="s">
-        <v>367</v>
+        <v>431</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -4252,25 +3718,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>366</v>
+        <v>324</v>
       </c>
       <c r="G6" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="H6" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="I6" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="J6" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="K6" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4327,7 +3793,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4341,7 +3807,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -4355,7 +3821,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -4369,7 +3835,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -4383,7 +3849,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4443,7 +3909,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>368</v>
+        <v>325</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -4452,10 +3918,10 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -4463,7 +3929,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4475,7 +3941,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>445</v>
+        <v>400</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4495,7 +3961,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -4507,7 +3973,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>446</v>
+        <v>401</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -4527,7 +3993,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4539,7 +4005,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>447</v>
+        <v>402</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4559,7 +4025,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4571,7 +4037,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>448</v>
+        <v>403</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -4591,7 +4057,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -4603,7 +4069,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>449</v>
+        <v>404</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4690,7 +4156,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>9</v>
@@ -4702,13 +4168,13 @@
         <v>132</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>443</v>
+        <v>398</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>453</v>
+        <v>408</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>444</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -4716,7 +4182,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>9</v>
@@ -4731,7 +4197,7 @@
         <v>133</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>452</v>
+        <v>407</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>136</v>
@@ -4742,7 +4208,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>9</v>
@@ -4757,10 +4223,10 @@
         <v>133</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>451</v>
+        <v>406</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4768,7 +4234,7 @@
         <v>47</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>9</v>
@@ -4783,10 +4249,10 @@
         <v>133</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>454</v>
+        <v>409</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>444</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4794,7 +4260,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>9</v>
@@ -4809,7 +4275,7 @@
         <v>133</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>455</v>
+        <v>410</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>136</v>
@@ -4829,232 +4295,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="J2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="G3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="J3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>212</v>
-      </c>
-      <c r="B4" t="s">
-        <v>317</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="G4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="J4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="G5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="J5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>214</v>
-      </c>
-      <c r="B6" t="s">
-        <v>317</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="G6" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>345</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="J6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5076,30 +4321,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>384</v>
+        <v>340</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>385</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>423</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5111,10 +4356,10 @@
         <v>134</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>386</v>
+        <v>342</v>
       </c>
       <c r="G2" t="s">
-        <v>387</v>
+        <v>343</v>
       </c>
       <c r="H2" t="s">
         <v>107</v>
@@ -5122,10 +4367,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
-        <v>318</v>
+        <v>423</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5134,24 +4379,24 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>388</v>
+        <v>344</v>
       </c>
       <c r="G3" t="s">
-        <v>389</v>
+        <v>345</v>
       </c>
       <c r="H3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>318</v>
+        <v>423</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5160,13 +4405,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>390</v>
+        <v>346</v>
       </c>
       <c r="G4" t="s">
-        <v>387</v>
+        <v>343</v>
       </c>
       <c r="H4" t="s">
         <v>77</v>
@@ -5174,10 +4419,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>318</v>
+        <v>423</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5186,13 +4431,13 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>391</v>
+        <v>347</v>
       </c>
       <c r="G5" t="s">
-        <v>389</v>
+        <v>345</v>
       </c>
       <c r="H5" t="s">
         <v>107</v>
@@ -5200,10 +4445,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s">
-        <v>318</v>
+        <v>423</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5212,19 +4457,20 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>392</v>
+        <v>348</v>
       </c>
       <c r="G6" t="s">
-        <v>387</v>
+        <v>343</v>
       </c>
       <c r="H6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
     <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
@@ -5236,12 +4482,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5278,39 +4524,39 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>372</v>
+        <v>328</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>374</v>
+        <v>330</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>375</v>
+        <v>331</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>377</v>
+        <v>333</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>378</v>
+        <v>334</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>379</v>
+        <v>335</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>434</v>
+        <v>389</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>435</v>
+        <v>390</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>436</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>424</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5322,25 +4568,25 @@
         <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>373</v>
+        <v>329</v>
       </c>
       <c r="G2" t="s">
-        <v>456</v>
+        <v>411</v>
       </c>
       <c r="H2" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>393</v>
+        <v>349</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>395</v>
+        <v>351</v>
       </c>
       <c r="L2" t="s">
-        <v>437</v>
+        <v>392</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>10</v>
@@ -5351,10 +4597,10 @@
     </row>
     <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>319</v>
+        <v>424</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5363,28 +4609,28 @@
         <v>10</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>459</v>
+        <v>414</v>
       </c>
       <c r="F3" t="s">
-        <v>373</v>
+        <v>329</v>
       </c>
       <c r="G3" t="s">
-        <v>457</v>
+        <v>412</v>
       </c>
       <c r="H3" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>393</v>
+        <v>349</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>395</v>
+        <v>351</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>460</v>
+        <v>415</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>10</v>
@@ -5395,10 +4641,10 @@
     </row>
     <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>424</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5407,28 +4653,28 @@
         <v>10</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>461</v>
+        <v>416</v>
       </c>
       <c r="F4" t="s">
-        <v>373</v>
+        <v>329</v>
       </c>
       <c r="G4" t="s">
-        <v>458</v>
+        <v>413</v>
       </c>
       <c r="H4" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>393</v>
+        <v>349</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>395</v>
+        <v>351</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>462</v>
+        <v>417</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -5439,10 +4685,10 @@
     </row>
     <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>319</v>
+        <v>424</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5451,28 +4697,28 @@
         <v>10</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>463</v>
+        <v>418</v>
       </c>
       <c r="F5" t="s">
-        <v>373</v>
+        <v>329</v>
       </c>
       <c r="G5" t="s">
-        <v>457</v>
+        <v>412</v>
       </c>
       <c r="H5" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>393</v>
+        <v>349</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>395</v>
+        <v>351</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>464</v>
+        <v>419</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>10</v>
@@ -5483,10 +4729,10 @@
     </row>
     <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
+        <v>424</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5495,28 +4741,28 @@
         <v>10</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>465</v>
+        <v>420</v>
       </c>
       <c r="F6" t="s">
-        <v>373</v>
+        <v>329</v>
       </c>
       <c r="G6" t="s">
-        <v>458</v>
+        <v>413</v>
       </c>
       <c r="H6" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>393</v>
+        <v>349</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>395</v>
+        <v>351</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>466</v>
+        <v>421</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>10</v>
@@ -5539,12 +4785,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5564,21 +4810,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>450</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>425</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -5587,15 +4833,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>425</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5604,15 +4850,15 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>425</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -5621,15 +4867,15 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="B5" t="s">
-        <v>320</v>
+        <v>425</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -5638,15 +4884,15 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s">
-        <v>320</v>
+        <v>425</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5655,7 +4901,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -5671,12 +4917,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5691,16 +4937,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>396</v>
+        <v>352</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>397</v>
+        <v>353</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>398</v>
+        <v>354</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>399</v>
+        <v>355</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>42</v>
@@ -5709,24 +4955,24 @@
         <v>3</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>400</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>467</v>
+        <v>432</v>
       </c>
       <c r="B2" t="s">
-        <v>401</v>
+        <v>437</v>
       </c>
       <c r="C2" t="s">
-        <v>403</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
-        <v>404</v>
+        <v>359</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>402</v>
+        <v>357</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -5737,19 +4983,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>468</v>
+        <v>433</v>
       </c>
       <c r="B3" t="s">
-        <v>401</v>
+        <v>437</v>
       </c>
       <c r="C3" t="s">
-        <v>406</v>
+        <v>361</v>
       </c>
       <c r="D3" t="s">
-        <v>407</v>
+        <v>362</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>405</v>
+        <v>360</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
@@ -5760,19 +5006,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>469</v>
+        <v>434</v>
       </c>
       <c r="B4" t="s">
-        <v>401</v>
+        <v>437</v>
       </c>
       <c r="C4" t="s">
-        <v>409</v>
+        <v>364</v>
       </c>
       <c r="D4" t="s">
-        <v>410</v>
+        <v>365</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>408</v>
+        <v>363</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
@@ -5783,19 +5029,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>470</v>
+        <v>435</v>
       </c>
       <c r="B5" t="s">
-        <v>401</v>
+        <v>437</v>
       </c>
       <c r="C5" t="s">
-        <v>412</v>
+        <v>367</v>
       </c>
       <c r="D5" t="s">
-        <v>409</v>
+        <v>364</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>411</v>
+        <v>366</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
@@ -5806,19 +5052,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>471</v>
+        <v>436</v>
       </c>
       <c r="B6" t="s">
-        <v>401</v>
+        <v>437</v>
       </c>
       <c r="C6" t="s">
-        <v>410</v>
+        <v>365</v>
       </c>
       <c r="D6" t="s">
-        <v>412</v>
+        <v>367</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>413</v>
+        <v>368</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
@@ -5849,4 +5095,352 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:P6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>427</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" t="s">
+        <v>427</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L6" t="s">
+        <v>117</v>
+      </c>
+      <c r="M6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0CFF6622-BAB0-4347-BF40-8454C1587B08}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{525EFD10-CCA5-4147-9725-D6BEDEE56E77}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{95AB71B3-4F4B-4D6A-B569-80362339980B}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{ED03B573-C665-46CB-B7C4-927872D8665B}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{C6C3BEA3-AFDF-4421-B679-B47318860373}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{42AC4B95-883A-4B03-8546-2347A0DEC06E}"/>
+    <hyperlink ref="C3:C6" r:id="rId7" display="aarosagarch@gmail.com" xr:uid="{55484541-91C2-427A-AAD4-4C4E61824716}"/>
+    <hyperlink ref="G2" r:id="rId8" xr:uid="{AA2F8371-C8C6-4427-AFBA-C78BEE2FB2F0}"/>
+    <hyperlink ref="G3" r:id="rId9" xr:uid="{E9A37910-8F5B-4DDE-8C09-6425CB5A7F2C}"/>
+    <hyperlink ref="G4" r:id="rId10" xr:uid="{C8AF07B7-5BEE-4826-BEB2-83257AF3C032}"/>
+    <hyperlink ref="G5" r:id="rId11" xr:uid="{4C0578FF-503E-4494-BA41-62B8D45BE900}"/>
+    <hyperlink ref="G6" r:id="rId12" xr:uid="{1ED313F1-8BB0-40AA-9458-C814A11521E4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Random Utils class is introduced
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E597B175-82BB-4CB9-B74B-20C5A882B76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7690E9C0-CCB4-4268-857D-77FC373FF015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="459">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1335,28 +1335,92 @@
     <t>TC12_DemoWebShop_PlaceOrder</t>
   </si>
   <si>
-    <t>TS07-01</t>
-  </si>
-  <si>
-    <t>TS07-02</t>
-  </si>
-  <si>
-    <t>TS07-03</t>
-  </si>
-  <si>
-    <t>TS07-04</t>
-  </si>
-  <si>
-    <t>TS07-05</t>
-  </si>
-  <si>
     <t>TS07_DemoWebshop_Registration</t>
+  </si>
+  <si>
+    <t>Gayle</t>
+  </si>
+  <si>
+    <t>Kunze</t>
+  </si>
+  <si>
+    <t>WzDGTaLO@test.org</t>
+  </si>
+  <si>
+    <t>Connie</t>
+  </si>
+  <si>
+    <t>Wunsch</t>
+  </si>
+  <si>
+    <t>XFjxWRRy@test.org</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>Braun</t>
+  </si>
+  <si>
+    <t>LNkOLwUC@test.org</t>
+  </si>
+  <si>
+    <t>Treutel-Huel</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Port Frank</t>
+  </si>
+  <si>
+    <t>3462</t>
+  </si>
+  <si>
+    <t>8828 Loma Shore</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>651-861-5504</t>
+  </si>
+  <si>
+    <t>Catherina</t>
+  </si>
+  <si>
+    <t>Brekke</t>
+  </si>
+  <si>
+    <t>UISSUDyU@test.org</t>
+  </si>
+  <si>
+    <t>Leuschke, Rosenbaum and Schimmel</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Armstrongfort</t>
+  </si>
+  <si>
+    <t>739</t>
+  </si>
+  <si>
+    <t>9981 Rheba Shores</t>
+  </si>
+  <si>
+    <t>YT</t>
+  </si>
+  <si>
+    <t>(219) 255-6859</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1828,10 +1892,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="63.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1871,13 +1935,13 @@
       <c r="A3" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>184</v>
       </c>
     </row>
@@ -1885,13 +1949,13 @@
       <c r="A4" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>184</v>
       </c>
     </row>
@@ -1899,16 +1963,16 @@
       <c r="A5" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>194</v>
       </c>
     </row>
@@ -1916,13 +1980,13 @@
       <c r="A6" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>184</v>
       </c>
     </row>
@@ -1930,13 +1994,13 @@
       <c r="A7" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>184</v>
       </c>
     </row>
@@ -1954,13 +2018,13 @@
       <c r="A9" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>191</v>
       </c>
     </row>
@@ -1968,13 +2032,13 @@
       <c r="A10" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>191</v>
       </c>
     </row>
@@ -1982,13 +2046,13 @@
       <c r="A11" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>191</v>
       </c>
     </row>
@@ -1996,13 +2060,13 @@
       <c r="A12" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>191</v>
       </c>
     </row>
@@ -2010,16 +2074,16 @@
       <c r="A13" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>194</v>
       </c>
     </row>
@@ -2037,13 +2101,13 @@
       <c r="A15" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>200</v>
       </c>
     </row>
@@ -2051,13 +2115,13 @@
       <c r="A16" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>200</v>
       </c>
     </row>
@@ -2065,16 +2129,16 @@
       <c r="A17" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>194</v>
       </c>
     </row>
@@ -2082,13 +2146,13 @@
       <c r="A18" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>200</v>
       </c>
     </row>
@@ -2096,13 +2160,13 @@
       <c r="A19" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>200</v>
       </c>
     </row>
@@ -2120,13 +2184,13 @@
       <c r="A21" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>217</v>
       </c>
     </row>
@@ -2134,13 +2198,13 @@
       <c r="A22" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>217</v>
       </c>
     </row>
@@ -2148,16 +2212,16 @@
       <c r="A23" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>194</v>
       </c>
     </row>
@@ -2165,16 +2229,16 @@
       <c r="A24" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>209</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" t="s" s="0">
         <v>194</v>
       </c>
     </row>
@@ -2182,13 +2246,13 @@
       <c r="A25" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>210</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>217</v>
       </c>
     </row>
@@ -2206,13 +2270,13 @@
       <c r="A27" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2220,13 +2284,13 @@
       <c r="A28" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>162</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2234,13 +2298,13 @@
       <c r="A29" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2248,13 +2312,13 @@
       <c r="A30" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>166</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2262,13 +2326,13 @@
       <c r="A31" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" t="s" s="0">
         <v>229</v>
       </c>
     </row>
@@ -2286,13 +2350,13 @@
       <c r="A33" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" t="s" s="0">
         <v>241</v>
       </c>
     </row>
@@ -2300,13 +2364,13 @@
       <c r="A34" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="s" s="0">
         <v>241</v>
       </c>
     </row>
@@ -2314,13 +2378,13 @@
       <c r="A35" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" t="s" s="0">
         <v>241</v>
       </c>
     </row>
@@ -2328,13 +2392,13 @@
       <c r="A36" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" t="s" s="0">
         <v>241</v>
       </c>
     </row>
@@ -2342,13 +2406,13 @@
       <c r="A37" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>228</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" t="s" s="0">
         <v>241</v>
       </c>
     </row>
@@ -2366,13 +2430,13 @@
       <c r="A39" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>236</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" t="s" s="0">
         <v>426</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" t="s" s="0">
         <v>252</v>
       </c>
     </row>
@@ -2380,13 +2444,13 @@
       <c r="A40" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>237</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="0">
         <v>426</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" t="s" s="0">
         <v>252</v>
       </c>
     </row>
@@ -2394,13 +2458,13 @@
       <c r="A41" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="s" s="0">
         <v>238</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" t="s" s="0">
         <v>426</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" t="s" s="0">
         <v>252</v>
       </c>
     </row>
@@ -2408,13 +2472,13 @@
       <c r="A42" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" t="s" s="0">
         <v>426</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>252</v>
       </c>
     </row>
@@ -2422,13 +2486,13 @@
       <c r="A43" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" t="s" s="0">
         <v>240</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="0">
         <v>426</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" t="s" s="0">
         <v>252</v>
       </c>
     </row>
@@ -2446,13 +2510,13 @@
       <c r="A45" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" t="s" s="0">
         <v>247</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" t="s" s="0">
         <v>264</v>
       </c>
     </row>
@@ -2460,13 +2524,13 @@
       <c r="A46" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" t="s" s="0">
         <v>248</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" t="s" s="0">
         <v>264</v>
       </c>
     </row>
@@ -2474,13 +2538,13 @@
       <c r="A47" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" t="s" s="0">
         <v>249</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" t="s" s="0">
         <v>264</v>
       </c>
     </row>
@@ -2488,13 +2552,13 @@
       <c r="A48" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" t="s" s="0">
         <v>264</v>
       </c>
     </row>
@@ -2502,13 +2566,13 @@
       <c r="A49" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" t="s" s="0">
         <v>251</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" t="s" s="0">
         <v>264</v>
       </c>
     </row>
@@ -2526,13 +2590,13 @@
       <c r="A51" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" t="s" s="0">
         <v>428</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" t="s" s="0">
         <v>271</v>
       </c>
     </row>
@@ -2540,13 +2604,13 @@
       <c r="A52" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" t="s" s="0">
         <v>260</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" t="s" s="0">
         <v>428</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" t="s" s="0">
         <v>271</v>
       </c>
     </row>
@@ -2554,13 +2618,13 @@
       <c r="A53" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" t="s" s="0">
         <v>261</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" t="s" s="0">
         <v>428</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" t="s" s="0">
         <v>271</v>
       </c>
     </row>
@@ -2568,13 +2632,13 @@
       <c r="A54" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" t="s" s="0">
         <v>262</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" t="s" s="0">
         <v>428</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>271</v>
       </c>
     </row>
@@ -2582,13 +2646,13 @@
       <c r="A55" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" t="s" s="0">
         <v>263</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" t="s" s="0">
         <v>428</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" t="s" s="0">
         <v>271</v>
       </c>
     </row>
@@ -2606,13 +2670,13 @@
       <c r="A57" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" t="s" s="0">
         <v>279</v>
       </c>
     </row>
@@ -2620,13 +2684,13 @@
       <c r="A58" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>279</v>
       </c>
     </row>
@@ -2634,13 +2698,13 @@
       <c r="A59" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" t="s" s="0">
         <v>279</v>
       </c>
     </row>
@@ -2648,13 +2712,13 @@
       <c r="A60" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" t="s" s="0">
         <v>279</v>
       </c>
     </row>
@@ -2662,13 +2726,13 @@
       <c r="A61" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" t="s" s="0">
         <v>279</v>
       </c>
     </row>
@@ -2686,13 +2750,13 @@
       <c r="A63" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" t="s" s="0">
         <v>430</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" t="s" s="0">
         <v>295</v>
       </c>
     </row>
@@ -2700,13 +2764,13 @@
       <c r="A64" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" t="s" s="0">
         <v>430</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" t="s" s="0">
         <v>295</v>
       </c>
     </row>
@@ -2714,13 +2778,13 @@
       <c r="A65" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" t="s" s="0">
         <v>276</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" t="s" s="0">
         <v>430</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" t="s" s="0">
         <v>295</v>
       </c>
     </row>
@@ -2728,13 +2792,13 @@
       <c r="A66" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" t="s" s="0">
         <v>277</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" t="s" s="0">
         <v>430</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" t="s" s="0">
         <v>295</v>
       </c>
     </row>
@@ -2742,13 +2806,13 @@
       <c r="A67" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" t="s" s="0">
         <v>278</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" t="s" s="0">
         <v>430</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" t="s" s="0">
         <v>295</v>
       </c>
     </row>
@@ -2766,13 +2830,13 @@
       <c r="A69" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" t="s" s="0">
         <v>284</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" t="s" s="0">
         <v>431</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" t="s" s="0">
         <v>297</v>
       </c>
     </row>
@@ -2780,13 +2844,13 @@
       <c r="A70" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" t="s" s="0">
         <v>285</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" t="s" s="0">
         <v>431</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" t="s" s="0">
         <v>297</v>
       </c>
     </row>
@@ -2794,13 +2858,13 @@
       <c r="A71" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" t="s" s="0">
         <v>286</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" t="s" s="0">
         <v>431</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" t="s" s="0">
         <v>297</v>
       </c>
     </row>
@@ -2808,13 +2872,13 @@
       <c r="A72" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" t="s" s="0">
         <v>287</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" t="s" s="0">
         <v>431</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" t="s" s="0">
         <v>297</v>
       </c>
     </row>
@@ -2822,13 +2886,13 @@
       <c r="A73" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" t="s" s="0">
         <v>288</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" t="s" s="0">
         <v>431</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" t="s" s="0">
         <v>297</v>
       </c>
     </row>
@@ -2848,10 +2912,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -2869,10 +2933,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>428</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2883,10 +2947,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>260</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>428</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2897,10 +2961,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>261</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>428</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2911,10 +2975,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>262</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>428</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2925,10 +2989,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>263</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>428</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2966,19 +3030,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="8" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.77734375"/>
+    <col min="7" max="7" customWidth="true" width="21.77734375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="28.77734375"/>
+    <col min="9" max="9" customWidth="true" width="24.109375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.44140625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="28.77734375"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="21.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -3023,207 +3087,207 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>318</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>374</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>377</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>379</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>373</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>163</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>388</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>321</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>322</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>323</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>324</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>318</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>381</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>377</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>382</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>373</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>383</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>388</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>321</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>161</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>323</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>384</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>318</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>374</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>373</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>386</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>323</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>387</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>385</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>373</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>397</v>
       </c>
     </row>
@@ -3253,18 +3317,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.44140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="59.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.44140625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.77734375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.109375"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.44140625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -3354,10 +3418,10 @@
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>374</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>151</v>
       </c>
       <c r="G3" s="14" t="s">
@@ -3462,10 +3526,10 @@
       <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>377</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>379</v>
       </c>
       <c r="G6" s="14" t="s">
@@ -3507,23 +3571,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.6640625"/>
+    <col min="4" max="4" customWidth="true" width="13.77734375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="59.6640625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.109375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.44140625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.0"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -3565,10 +3629,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>284</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>431</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -3577,33 +3641,33 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>313</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>316</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>285</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>431</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3612,33 +3676,33 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>318</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>316</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>286</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>431</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -3647,33 +3711,33 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>319</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>320</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>316</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>287</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>431</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -3682,33 +3746,33 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>321</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>316</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>288</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>431</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -3717,25 +3781,25 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>323</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>316</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>317</v>
       </c>
     </row>
@@ -3768,10 +3832,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -3789,13 +3853,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3803,13 +3867,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3817,13 +3881,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -3831,13 +3895,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3845,13 +3909,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -3880,16 +3944,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.44140625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="25.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -3925,28 +3989,28 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>400</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -3957,28 +4021,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>401</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>32</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -3989,28 +4053,28 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>402</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>57</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -4021,60 +4085,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>403</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>404</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>63</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -4115,14 +4179,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -4304,13 +4368,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.6640625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.77734375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -4340,132 +4404,132 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>134</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>343</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>170</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>345</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>172</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>343</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>209</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>173</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>345</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>210</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>174</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>343</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>171</v>
       </c>
     </row>
@@ -4492,19 +4556,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.44140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="32.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="26.109375"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" width="14.33203125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.109375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.44140625"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.33203125"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4552,13 +4616,13 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4567,13 +4631,13 @@
       <c r="E2" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>411</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>332</v>
       </c>
       <c r="I2" s="9" t="s">
@@ -4585,7 +4649,7 @@
       <c r="K2" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>392</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -4596,13 +4660,13 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>162</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4611,13 +4675,13 @@
       <c r="E3" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>412</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>332</v>
       </c>
       <c r="I3" s="9" t="s">
@@ -4640,13 +4704,13 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -4655,13 +4719,13 @@
       <c r="E4" s="17" t="s">
         <v>416</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>413</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>332</v>
       </c>
       <c r="I4" s="9" t="s">
@@ -4684,13 +4748,13 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>166</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -4699,13 +4763,13 @@
       <c r="E5" s="17" t="s">
         <v>418</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>412</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>332</v>
       </c>
       <c r="I5" s="9" t="s">
@@ -4728,13 +4792,13 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -4743,13 +4807,13 @@
       <c r="E6" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>413</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>332</v>
       </c>
       <c r="I6" s="9" t="s">
@@ -4795,11 +4859,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -4820,87 +4884,87 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>228</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>305</v>
       </c>
     </row>
@@ -4921,18 +4985,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.109375"/>
+    <col min="4" max="4" customWidth="true" width="9.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.44140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -4959,20 +5023,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>432</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s" s="0">
+        <v>436</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>437</v>
       </c>
-      <c r="C2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D2" t="s">
-        <v>359</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>357</v>
+        <v>438</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -4982,16 +5046,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>433</v>
-      </c>
-      <c r="B3" t="s">
-        <v>437</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" t="s" s="0">
+        <v>237</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>432</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>361</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>362</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -5005,16 +5069,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>434</v>
-      </c>
-      <c r="B4" t="s">
-        <v>437</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="A4" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>432</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>364</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>365</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -5028,16 +5092,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>435</v>
-      </c>
-      <c r="B5" t="s">
-        <v>437</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" t="s" s="0">
+        <v>239</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>432</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>367</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>364</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -5051,16 +5115,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>436</v>
-      </c>
-      <c r="B6" t="s">
-        <v>437</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="A6" t="s" s="0">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>432</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>365</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>367</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -5107,22 +5171,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.88671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.44140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.109375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.44140625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.109375"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.33203125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="40.109375"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="17.109375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.44140625"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.77734375"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -5176,10 +5240,10 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>247</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>427</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5188,48 +5252,48 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>74</v>
+      <c r="E2" t="s" s="0">
+        <v>449</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>450</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" t="s">
+        <v>451</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>452</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>453</v>
+      </c>
+      <c r="J2" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="K2" t="s">
-        <v>79</v>
+      <c r="K2" t="s" s="0">
+        <v>454</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M2" t="s">
-        <v>81</v>
-      </c>
-      <c r="N2" t="s">
-        <v>82</v>
+        <v>455</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>456</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>457</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>118</v>
+        <v>458</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>248</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>427</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5238,34 +5302,34 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>84</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>92</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -5276,10 +5340,10 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>249</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>427</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5288,34 +5352,34 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>94</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>102</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -5326,10 +5390,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>427</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5338,31 +5402,31 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>104</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>110</v>
       </c>
       <c r="N5" s="3" t="s">
@@ -5376,10 +5440,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>251</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>427</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5388,31 +5452,31 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>112</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>125</v>
       </c>
       <c r="N6" s="3" t="s">

</xml_diff>

<commit_message>
Execution of DemoWebShop testcases inprogress
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="477">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1414,6 +1414,60 @@
   </si>
   <si>
     <t>(219) 255-6859</t>
+  </si>
+  <si>
+    <t>Allan</t>
+  </si>
+  <si>
+    <t>Luettgen</t>
+  </si>
+  <si>
+    <t>QhdEmipn@test.org</t>
+  </si>
+  <si>
+    <t>Nickole</t>
+  </si>
+  <si>
+    <t>Schultz</t>
+  </si>
+  <si>
+    <t>fvrfvahy@test.org</t>
+  </si>
+  <si>
+    <t>Schneider Group</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>New Marcustown</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>621 Haag Green</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>910-797-3373</t>
+  </si>
+  <si>
+    <t>Order number: 1576750</t>
+  </si>
+  <si>
+    <t>Order number: 1576753</t>
+  </si>
+  <si>
+    <t>Order number: 1576757</t>
+  </si>
+  <si>
+    <t>Order number: 1576766</t>
+  </si>
+  <si>
+    <t>Order number: 1576770</t>
   </si>
 </sst>
 </file>
@@ -3124,7 +3178,7 @@
         <v>163</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>393</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -3165,7 +3219,7 @@
         <v>141</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>394</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -3206,7 +3260,7 @@
         <v>143</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>395</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -3247,7 +3301,7 @@
         <v>151</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>396</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -3288,7 +3342,7 @@
         <v>142</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>397</v>
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -5030,13 +5084,13 @@
         <v>432</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>437</v>
+        <v>460</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>438</v>
+        <v>461</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -5253,37 +5307,37 @@
         <v>10</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>450</v>
+        <v>463</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="J2" t="s" s="0">
         <v>78</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>454</v>
+        <v>467</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>455</v>
+        <v>468</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>456</v>
+        <v>469</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>457</v>
+        <v>470</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>458</v>
+        <v>471</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
TestNG Annotations and TestNG XML introduction
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\AutomationCatalogue_TestingFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7690E9C0-CCB4-4268-857D-77FC373FF015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F778DEE9-164F-47CE-B852-FAA33A6BA06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="435">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -258,36 +258,12 @@
     <t>Fax number</t>
   </si>
   <si>
-    <t>Charlie</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>charlie@gmail.com</t>
-  </si>
-  <si>
-    <t>Gap</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
     <t>Alberta</t>
   </si>
   <si>
-    <t>Calgary</t>
-  </si>
-  <si>
-    <t>43rd Avenue Road</t>
-  </si>
-  <si>
-    <t>Northwest</t>
-  </si>
-  <si>
-    <t>L6H0N4</t>
-  </si>
-  <si>
     <t>Peter</t>
   </si>
   <si>
@@ -393,9 +369,6 @@
     <t>C-21_C ,Petronas towerConcourse Expansion</t>
   </si>
   <si>
-    <t>4168794033</t>
-  </si>
-  <si>
     <t>9875533262</t>
   </si>
   <si>
@@ -1110,15 +1083,6 @@
     <t>Confirm password</t>
   </si>
   <si>
-    <t>aarosagarch@gamil.com</t>
-  </si>
-  <si>
-    <t>sagar</t>
-  </si>
-  <si>
-    <t>ch</t>
-  </si>
-  <si>
     <t>anupreddy.desai@gmail.com</t>
   </si>
   <si>
@@ -1218,21 +1182,6 @@
     <t>daniel.upton</t>
   </si>
   <si>
-    <t>Order number: 1550156</t>
-  </si>
-  <si>
-    <t>Order number: 1550173</t>
-  </si>
-  <si>
-    <t>Order number: 1550182</t>
-  </si>
-  <si>
-    <t>Order number: 1550185</t>
-  </si>
-  <si>
-    <t>Order number: 1550202</t>
-  </si>
-  <si>
     <t>Employee Management</t>
   </si>
   <si>
@@ -1338,84 +1287,6 @@
     <t>TS07_DemoWebshop_Registration</t>
   </si>
   <si>
-    <t>Gayle</t>
-  </si>
-  <si>
-    <t>Kunze</t>
-  </si>
-  <si>
-    <t>WzDGTaLO@test.org</t>
-  </si>
-  <si>
-    <t>Connie</t>
-  </si>
-  <si>
-    <t>Wunsch</t>
-  </si>
-  <si>
-    <t>XFjxWRRy@test.org</t>
-  </si>
-  <si>
-    <t>Parker</t>
-  </si>
-  <si>
-    <t>Braun</t>
-  </si>
-  <si>
-    <t>LNkOLwUC@test.org</t>
-  </si>
-  <si>
-    <t>Treutel-Huel</t>
-  </si>
-  <si>
-    <t>Djibouti</t>
-  </si>
-  <si>
-    <t>Port Frank</t>
-  </si>
-  <si>
-    <t>3462</t>
-  </si>
-  <si>
-    <t>8828 Loma Shore</t>
-  </si>
-  <si>
-    <t>SG</t>
-  </si>
-  <si>
-    <t>651-861-5504</t>
-  </si>
-  <si>
-    <t>Catherina</t>
-  </si>
-  <si>
-    <t>Brekke</t>
-  </si>
-  <si>
-    <t>UISSUDyU@test.org</t>
-  </si>
-  <si>
-    <t>Leuschke, Rosenbaum and Schimmel</t>
-  </si>
-  <si>
-    <t>Cameroon</t>
-  </si>
-  <si>
-    <t>Armstrongfort</t>
-  </si>
-  <si>
-    <t>739</t>
-  </si>
-  <si>
-    <t>9981 Rheba Shores</t>
-  </si>
-  <si>
-    <t>YT</t>
-  </si>
-  <si>
-    <t>(219) 255-6859</t>
-  </si>
-  <si>
     <t>Allan</t>
   </si>
   <si>
@@ -1468,6 +1339,9 @@
   </si>
   <si>
     <t>Order number: 1576770</t>
+  </si>
+  <si>
+    <t>Chris</t>
   </si>
 </sst>
 </file>
@@ -1954,7 +1828,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>
@@ -1963,23 +1837,23 @@
         <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1987,82 +1861,82 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>7</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2070,82 +1944,82 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>22</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>23</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B11" t="s" s="0">
         <v>24</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>25</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s" s="0">
         <v>26</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2153,82 +2027,82 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s" s="0">
         <v>44</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B16" t="s" s="0">
         <v>45</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B17" t="s" s="0">
         <v>46</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>47</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B19" t="s" s="0">
         <v>48</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2236,85 +2110,85 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B23" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>406</v>
+      </c>
+      <c r="D23" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="C23" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="D23" t="s" s="0">
-        <v>217</v>
-      </c>
       <c r="E23" t="s" s="0">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2322,79 +2196,79 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2402,79 +2276,79 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2482,72 +2356,72 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="D39" t="s" s="0">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="D40" t="s" s="0">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2562,79 +2436,79 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2642,79 +2516,79 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B54" t="s" s="0">
+        <v>253</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>411</v>
+      </c>
+      <c r="D54" t="s" s="0">
         <v>262</v>
-      </c>
-      <c r="C54" t="s" s="0">
-        <v>428</v>
-      </c>
-      <c r="D54" t="s" s="0">
-        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2722,79 +2596,79 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B57" t="s" s="0">
         <v>34</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B58" t="s" s="0">
         <v>35</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B59" t="s" s="0">
         <v>36</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B60" t="s" s="0">
         <v>37</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B61" t="s" s="0">
         <v>38</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2802,79 +2676,79 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2882,72 +2756,72 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="D69" t="s" s="0">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="D70" t="s" s="0">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="D71" t="s" s="0">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B73" t="s" s="0">
+        <v>279</v>
+      </c>
+      <c r="C73" t="s" s="0">
+        <v>414</v>
+      </c>
+      <c r="D73" t="s" s="0">
         <v>288</v>
-      </c>
-      <c r="C73" t="s" s="0">
-        <v>431</v>
-      </c>
-      <c r="D73" t="s" s="0">
-        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2980,7 +2854,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -2988,10 +2862,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -3002,10 +2876,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -3016,10 +2890,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -3030,10 +2904,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -3044,10 +2918,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -3107,37 +2981,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -3145,7 +3019,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>33</v>
@@ -3154,31 +3028,31 @@
         <v>10</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>472</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -3186,7 +3060,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>33</v>
@@ -3195,31 +3069,31 @@
         <v>10</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>473</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -3227,7 +3101,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>33</v>
@@ -3236,31 +3110,31 @@
         <v>10</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>474</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -3268,7 +3142,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>33</v>
@@ -3277,31 +3151,31 @@
         <v>10</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>475</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -3309,7 +3183,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>33</v>
@@ -3318,31 +3192,31 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="0">
+        <v>361</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>374</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>314</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="I6" t="s" s="0">
         <v>373</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>386</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>323</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>387</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>385</v>
-      </c>
       <c r="J6" t="s" s="0">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>476</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -3399,36 +3273,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>33</v>
@@ -3437,34 +3311,34 @@
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>33</v>
@@ -3473,34 +3347,34 @@
         <v>10</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -3509,34 +3383,34 @@
         <v>10</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>33</v>
@@ -3545,34 +3419,34 @@
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>33</v>
@@ -3581,25 +3455,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L6" s="14"/>
     </row>
@@ -3646,48 +3520,48 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -3696,33 +3570,33 @@
         <v>10</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -3731,33 +3605,33 @@
         <v>10</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -3766,33 +3640,33 @@
         <v>10</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -3801,33 +3675,33 @@
         <v>10</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -3836,25 +3710,25 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3911,7 +3785,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>9</v>
@@ -3925,7 +3799,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>11</v>
@@ -3939,7 +3813,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>13</v>
@@ -3953,7 +3827,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>15</v>
@@ -3967,7 +3841,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>17</v>
@@ -3992,8 +3866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4027,7 +3901,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -4036,10 +3910,10 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -4047,7 +3921,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>9</v>
@@ -4059,7 +3933,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>400</v>
+        <v>434</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>29</v>
@@ -4079,7 +3953,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>9</v>
@@ -4091,7 +3965,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>30</v>
@@ -4111,7 +3985,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>9</v>
@@ -4123,7 +3997,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>29</v>
@@ -4143,7 +4017,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>9</v>
@@ -4155,7 +4029,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>30</v>
@@ -4175,7 +4049,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>9</v>
@@ -4187,7 +4061,7 @@
         <v>62</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>29</v>
@@ -4257,7 +4131,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>49</v>
@@ -4274,7 +4148,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>9</v>
@@ -4283,16 +4157,16 @@
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -4300,7 +4174,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>9</v>
@@ -4309,16 +4183,16 @@
         <v>10</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4326,7 +4200,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>9</v>
@@ -4335,16 +4209,16 @@
         <v>10</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4352,7 +4226,7 @@
         <v>47</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>9</v>
@@ -4361,16 +4235,16 @@
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4378,7 +4252,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>9</v>
@@ -4387,16 +4261,16 @@
         <v>10</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4439,30 +4313,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>9</v>
@@ -4471,24 +4345,24 @@
         <v>10</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>9</v>
@@ -4497,24 +4371,24 @@
         <v>10</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>9</v>
@@ -4523,24 +4397,24 @@
         <v>10</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>9</v>
@@ -4549,24 +4423,24 @@
         <v>10</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>9</v>
@@ -4575,16 +4449,16 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4642,39 +4516,39 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>9</v>
@@ -4686,25 +4560,25 @@
         <v>59</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>10</v>
@@ -4715,10 +4589,10 @@
     </row>
     <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>9</v>
@@ -4727,28 +4601,28 @@
         <v>10</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>10</v>
@@ -4759,10 +4633,10 @@
     </row>
     <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>9</v>
@@ -4771,28 +4645,28 @@
         <v>10</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>413</v>
+        <v>396</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -4803,10 +4677,10 @@
     </row>
     <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>9</v>
@@ -4815,28 +4689,28 @@
         <v>10</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>10</v>
@@ -4847,10 +4721,10 @@
     </row>
     <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>9</v>
@@ -4859,28 +4733,28 @@
         <v>10</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>413</v>
+        <v>396</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>10</v>
@@ -4928,21 +4802,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>9</v>
@@ -4951,15 +4825,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>9</v>
@@ -4968,15 +4842,15 @@
         <v>10</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>9</v>
@@ -4985,15 +4859,15 @@
         <v>10</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>9</v>
@@ -5002,15 +4876,15 @@
         <v>10</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>9</v>
@@ -5019,7 +4893,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -5039,7 +4913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -5055,16 +4929,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>42</v>
@@ -5073,24 +4947,24 @@
         <v>3</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>459</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>460</v>
+        <v>417</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>461</v>
+        <v>418</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -5101,19 +4975,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
@@ -5124,19 +4998,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
@@ -5147,19 +5021,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
@@ -5170,19 +5044,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
@@ -5295,10 +5169,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -5307,48 +5181,48 @@
         <v>10</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>462</v>
+        <v>419</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>463</v>
+        <v>420</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>464</v>
+        <v>421</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>465</v>
+        <v>422</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>466</v>
+        <v>423</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>467</v>
+        <v>424</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>468</v>
+        <v>425</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>469</v>
+        <v>426</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>470</v>
+        <v>427</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>471</v>
+        <v>428</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
@@ -5357,48 +5231,48 @@
         <v>10</v>
       </c>
       <c r="E3" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="M3" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="N3" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>87</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="L3" t="s" s="0">
-        <v>90</v>
-      </c>
-      <c r="M3" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="N3" t="s" s="0">
-        <v>92</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -5407,48 +5281,48 @@
         <v>10</v>
       </c>
       <c r="E4" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="M4" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="N4" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>96</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>98</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="L4" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="M4" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="N4" t="s" s="0">
-        <v>102</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -5457,48 +5331,48 @@
         <v>10</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -5507,40 +5381,40 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H6" t="s" s="0">
-        <v>114</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>115</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>98</v>
-      </c>
-      <c r="K6" t="s" s="0">
-        <v>116</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>117</v>
-      </c>
-      <c r="M6" t="s" s="0">
-        <v>125</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="P6" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TestNG Annotations implemented in Framework
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="436">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1342,6 +1342,9 @@
   </si>
   <si>
     <t>Chris</t>
+  </si>
+  <si>
+    <t>Shanon</t>
   </si>
 </sst>
 </file>
@@ -3933,7 +3936,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>29</v>

</xml_diff>

<commit_message>
TestNG Annotations BeforeSuite and xml implemented
</commit_message>
<xml_diff>
--- a/TestData/Automation_TestData.xlsx
+++ b/TestData/Automation_TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="437">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1345,6 +1345,9 @@
   </si>
   <si>
     <t>Shanon</t>
+  </si>
+  <si>
+    <t>Elbert</t>
   </si>
 </sst>
 </file>
@@ -3936,7 +3939,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>29</v>

</xml_diff>